<commit_message>
Update measures of Tuong
</commit_message>
<xml_diff>
--- a/Project Plan/Mesurement.xlsx
+++ b/Project Plan/Mesurement.xlsx
@@ -14,12 +14,12 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$199</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="47">
   <si>
     <t>No.</t>
   </si>
@@ -121,13 +121,52 @@
   </si>
   <si>
     <t>Finished date</t>
+  </si>
+  <si>
+    <t>Research about the MVVM pattern, WCF</t>
+  </si>
+  <si>
+    <t>Tuong Nguyen</t>
+  </si>
+  <si>
+    <t>Research about the ACDM</t>
+  </si>
+  <si>
+    <t>Document Snarios for "Đào tạo"</t>
+  </si>
+  <si>
+    <t>Low</t>
+  </si>
+  <si>
+    <t>Concept Operation</t>
+  </si>
+  <si>
+    <t>Prepare for Architecture Driver</t>
+  </si>
+  <si>
+    <t>Update Architecture Driver</t>
+  </si>
+  <si>
+    <t>Design Database</t>
+  </si>
+  <si>
+    <t>Write Architecture Design</t>
+  </si>
+  <si>
+    <t>Program "Nghề nghiệp" Interface</t>
+  </si>
+  <si>
+    <t>Review Architecture driver</t>
+  </si>
+  <si>
+    <t>Design System Context</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -161,6 +200,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
@@ -225,7 +271,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -234,15 +280,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -587,8 +634,8 @@
   <dimension ref="A1:I205"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <pane ySplit="2" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,17 +652,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
     </row>
     <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -650,7 +697,7 @@
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -662,13 +709,13 @@
       <c r="E3" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="7">
         <v>40734</v>
       </c>
       <c r="G3" s="3">
         <v>8</v>
       </c>
-      <c r="H3" s="7">
+      <c r="H3" s="6">
         <v>2</v>
       </c>
       <c r="I3" s="2">
@@ -679,7 +726,7 @@
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="4" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -691,11 +738,11 @@
       <c r="E4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="7"/>
       <c r="G4" s="3">
         <v>3</v>
       </c>
-      <c r="H4" s="7">
+      <c r="H4" s="6">
         <v>2.5</v>
       </c>
       <c r="I4" s="2">
@@ -706,7 +753,7 @@
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="2" t="s">
@@ -718,11 +765,11 @@
       <c r="E5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="7"/>
       <c r="G5" s="3">
         <v>3</v>
       </c>
-      <c r="H5" s="7">
+      <c r="H5" s="6">
         <v>1.5</v>
       </c>
       <c r="I5" s="2">
@@ -733,7 +780,7 @@
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="2" t="s">
@@ -745,11 +792,11 @@
       <c r="E6" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="7"/>
       <c r="G6" s="3">
         <v>16</v>
       </c>
-      <c r="H6" s="7">
+      <c r="H6" s="6">
         <v>24</v>
       </c>
       <c r="I6" s="2">
@@ -760,7 +807,7 @@
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="2" t="s">
@@ -772,11 +819,11 @@
       <c r="E7" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="8"/>
+      <c r="F7" s="7"/>
       <c r="G7" s="3">
         <v>3</v>
       </c>
-      <c r="H7" s="7">
+      <c r="H7" s="6">
         <v>4.5</v>
       </c>
       <c r="I7" s="2">
@@ -787,7 +834,7 @@
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="2" t="s">
@@ -799,11 +846,11 @@
       <c r="E8" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="8"/>
+      <c r="F8" s="7"/>
       <c r="G8" s="3">
         <v>70</v>
       </c>
-      <c r="H8" s="7">
+      <c r="H8" s="6">
         <v>45.5</v>
       </c>
       <c r="I8" s="2">
@@ -814,7 +861,7 @@
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -826,11 +873,11 @@
       <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="8"/>
+      <c r="F9" s="7"/>
       <c r="G9" s="3">
         <v>6</v>
       </c>
-      <c r="H9" s="7">
+      <c r="H9" s="6">
         <v>2</v>
       </c>
       <c r="I9" s="2">
@@ -841,7 +888,7 @@
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="2" t="s">
@@ -853,11 +900,11 @@
       <c r="E10" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="8"/>
+      <c r="F10" s="7"/>
       <c r="G10" s="3">
         <v>15</v>
       </c>
-      <c r="H10" s="7">
+      <c r="H10" s="6">
         <v>6.5</v>
       </c>
       <c r="I10" s="2">
@@ -868,7 +915,7 @@
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -880,11 +927,11 @@
       <c r="E11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="8"/>
+      <c r="F11" s="7"/>
       <c r="G11" s="3">
         <v>20</v>
       </c>
-      <c r="H11" s="7">
+      <c r="H11" s="6">
         <v>14</v>
       </c>
       <c r="I11" s="2">
@@ -895,7 +942,7 @@
       <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="2" t="s">
@@ -907,11 +954,11 @@
       <c r="E12" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="7"/>
       <c r="G12" s="3">
         <v>5</v>
       </c>
-      <c r="H12" s="7">
+      <c r="H12" s="6">
         <v>3</v>
       </c>
       <c r="I12" s="2">
@@ -922,7 +969,7 @@
       <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="2" t="s">
@@ -934,11 +981,11 @@
       <c r="E13" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="8"/>
+      <c r="F13" s="7"/>
       <c r="G13" s="3">
         <v>35</v>
       </c>
-      <c r="H13" s="7">
+      <c r="H13" s="6">
         <v>8</v>
       </c>
       <c r="I13" s="2">
@@ -949,7 +996,7 @@
       <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="B14" s="5" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -961,11 +1008,11 @@
       <c r="E14" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="8"/>
+      <c r="F14" s="7"/>
       <c r="G14" s="3">
         <v>35</v>
       </c>
-      <c r="H14" s="7">
+      <c r="H14" s="6">
         <v>11</v>
       </c>
       <c r="I14" s="2">
@@ -976,7 +1023,7 @@
       <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="4" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="2" t="s">
@@ -988,11 +1035,11 @@
       <c r="E15" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="8"/>
+      <c r="F15" s="7"/>
       <c r="G15" s="3">
         <v>35</v>
       </c>
-      <c r="H15" s="7">
+      <c r="H15" s="6">
         <v>1.5</v>
       </c>
       <c r="I15" s="2">
@@ -1003,7 +1050,7 @@
       <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -1015,11 +1062,11 @@
       <c r="E16" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="8"/>
+      <c r="F16" s="7"/>
       <c r="G16" s="3">
         <v>6</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="6">
         <v>6.5</v>
       </c>
       <c r="I16" s="2">
@@ -1030,7 +1077,7 @@
       <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="4" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -1042,11 +1089,11 @@
       <c r="E17" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="8"/>
+      <c r="F17" s="7"/>
       <c r="G17" s="3">
         <v>42</v>
       </c>
-      <c r="H17" s="7">
+      <c r="H17" s="6">
         <v>5</v>
       </c>
       <c r="I17" s="2">
@@ -1055,572 +1102,730 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
-        <v>26</v>
-      </c>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="2"/>
-      <c r="H18" s="2"/>
-      <c r="I18" s="2"/>
+        <v>16</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F18" s="7"/>
+      <c r="G18" s="3">
+        <v>5</v>
+      </c>
+      <c r="H18" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="I18" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
+        <v>17</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="2"/>
-      <c r="H19" s="2"/>
-      <c r="I19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="7"/>
+      <c r="G19" s="3">
+        <v>8</v>
+      </c>
+      <c r="H19" s="3">
+        <v>6.5</v>
+      </c>
+      <c r="I19" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="8"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2"/>
-      <c r="I20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="7"/>
+      <c r="G20" s="3">
+        <v>1</v>
+      </c>
+      <c r="H20" s="3">
+        <v>2</v>
+      </c>
+      <c r="I20" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
-        <v>29</v>
-      </c>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="2"/>
-      <c r="H21" s="2"/>
-      <c r="I21" s="2"/>
+        <v>19</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F21" s="7"/>
+      <c r="G21" s="3">
+        <v>7</v>
+      </c>
+      <c r="H21" s="3">
+        <v>5</v>
+      </c>
+      <c r="I21" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
-        <v>30</v>
-      </c>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="2"/>
-      <c r="H22" s="2"/>
-      <c r="I22" s="2"/>
+        <v>20</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F22" s="7">
+        <v>40613</v>
+      </c>
+      <c r="G22" s="3">
+        <v>2</v>
+      </c>
+      <c r="H22" s="3">
+        <v>3</v>
+      </c>
+      <c r="I22" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
-        <v>31</v>
-      </c>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="2"/>
-      <c r="H23" s="2"/>
-      <c r="I23" s="2"/>
+        <v>21</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" s="7"/>
+      <c r="G23" s="3">
+        <v>4</v>
+      </c>
+      <c r="H23" s="3">
+        <v>5</v>
+      </c>
+      <c r="I23" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
-        <v>32</v>
-      </c>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="2"/>
-      <c r="H24" s="2"/>
-      <c r="I24" s="2"/>
+        <v>22</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F24" s="7"/>
+      <c r="G24" s="3">
+        <v>6</v>
+      </c>
+      <c r="H24" s="3">
+        <v>3</v>
+      </c>
+      <c r="I24" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
-        <v>33</v>
-      </c>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="2"/>
-      <c r="H25" s="2"/>
-      <c r="I25" s="2"/>
+        <v>23</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F25" s="7"/>
+      <c r="G25" s="3">
+        <v>6</v>
+      </c>
+      <c r="H25" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="I25" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3">
-        <v>34</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2"/>
-      <c r="I26" s="2"/>
+        <v>24</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F26" s="7">
+        <v>40798</v>
+      </c>
+      <c r="G26" s="3">
+        <v>2</v>
+      </c>
+      <c r="H26" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="I26" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
+        <v>25</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
+      <c r="F27" s="7"/>
+      <c r="G27" s="3">
+        <v>5</v>
+      </c>
+      <c r="H27" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="I27" s="2">
+        <v>50</v>
+      </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
-        <v>36</v>
-      </c>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
-      <c r="I28" s="2"/>
+        <v>26</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="F28" s="7"/>
+      <c r="G28" s="3">
+        <v>4</v>
+      </c>
+      <c r="H28" s="3">
+        <v>2</v>
+      </c>
+      <c r="I28" s="2">
+        <v>100</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
-        <v>37</v>
+        <v>27</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="8"/>
+      <c r="F29" s="7"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="8"/>
+      <c r="F30" s="7"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
-      <c r="F31" s="8"/>
+      <c r="F31" s="7"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
-      <c r="F32" s="8"/>
+      <c r="F32" s="7"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="8"/>
+      <c r="F33" s="7"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2"/>
       <c r="I33" s="2"/>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
-        <v>42</v>
+        <v>32</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="8"/>
+      <c r="F34" s="7"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="8"/>
+      <c r="F35" s="7"/>
       <c r="G35" s="2"/>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3">
-        <v>44</v>
+        <v>34</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="8"/>
+      <c r="F36" s="7"/>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="8"/>
+      <c r="F37" s="7"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
-      <c r="F38" s="8"/>
+      <c r="F38" s="7"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
       <c r="E39" s="2"/>
-      <c r="F39" s="8"/>
+      <c r="F39" s="7"/>
       <c r="G39" s="2"/>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2"/>
-      <c r="F40" s="8"/>
+      <c r="F40" s="7"/>
       <c r="G40" s="2"/>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
       <c r="D41" s="2"/>
       <c r="E41" s="2"/>
-      <c r="F41" s="8"/>
+      <c r="F41" s="7"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
       <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
-      <c r="F42" s="8"/>
+      <c r="F42" s="7"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
       <c r="D43" s="2"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="8"/>
+      <c r="F43" s="7"/>
       <c r="G43" s="2"/>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
       <c r="D44" s="2"/>
       <c r="E44" s="2"/>
-      <c r="F44" s="8"/>
+      <c r="F44" s="7"/>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
       <c r="D45" s="2"/>
       <c r="E45" s="2"/>
-      <c r="F45" s="8"/>
+      <c r="F45" s="7"/>
       <c r="G45" s="2"/>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
       <c r="D46" s="2"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="8"/>
+      <c r="F46" s="7"/>
       <c r="G46" s="2"/>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
       <c r="E47" s="2"/>
-      <c r="F47" s="8"/>
+      <c r="F47" s="7"/>
       <c r="G47" s="2"/>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
       <c r="E48" s="2"/>
-      <c r="F48" s="8"/>
+      <c r="F48" s="7"/>
       <c r="G48" s="2"/>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
       <c r="E49" s="2"/>
-      <c r="F49" s="8"/>
+      <c r="F49" s="7"/>
       <c r="G49" s="2"/>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
-      <c r="F50" s="8"/>
+      <c r="F50" s="7"/>
       <c r="G50" s="2"/>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
       <c r="E51" s="2"/>
-      <c r="F51" s="8"/>
+      <c r="F51" s="7"/>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
       <c r="I51" s="2"/>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
       <c r="D52" s="2"/>
       <c r="E52" s="2"/>
-      <c r="F52" s="8"/>
+      <c r="F52" s="7"/>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
       <c r="I52" s="2"/>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
       <c r="E53" s="2"/>
-      <c r="F53" s="8"/>
+      <c r="F53" s="7"/>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
       <c r="I53" s="2"/>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
       <c r="E54" s="2"/>
-      <c r="F54" s="8"/>
+      <c r="F54" s="7"/>
       <c r="G54" s="2"/>
       <c r="H54" s="2"/>
       <c r="I54" s="2"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
       <c r="E55" s="2"/>
-      <c r="F55" s="8"/>
+      <c r="F55" s="7"/>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2"/>
-      <c r="F56" s="8"/>
+      <c r="F56" s="7"/>
       <c r="G56" s="2"/>
       <c r="H56" s="2"/>
       <c r="I56" s="2"/>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
-        <v>65</v>
+        <v>55</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
       <c r="E57" s="2"/>
-      <c r="F57" s="8"/>
+      <c r="F57" s="7"/>
       <c r="G57" s="2"/>
       <c r="H57" s="2"/>
       <c r="I57" s="2"/>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
       <c r="E58" s="2"/>
-      <c r="F58" s="8"/>
+      <c r="F58" s="7"/>
       <c r="G58" s="2"/>
       <c r="H58" s="2"/>
       <c r="I58" s="2"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
       <c r="E59" s="2"/>
-      <c r="F59" s="8"/>
+      <c r="F59" s="7"/>
       <c r="G59" s="2"/>
       <c r="H59" s="2"/>
       <c r="I59" s="2"/>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
       <c r="E60" s="2"/>
-      <c r="F60" s="8"/>
+      <c r="F60" s="7"/>
       <c r="G60" s="2"/>
       <c r="H60" s="2"/>
       <c r="I60" s="2"/>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
       <c r="E61" s="2"/>
-      <c r="F61" s="8"/>
+      <c r="F61" s="7"/>
       <c r="G61" s="2"/>
       <c r="H61" s="2"/>
       <c r="I61" s="2"/>
@@ -1633,7 +1838,7 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
       <c r="E62" s="2"/>
-      <c r="F62" s="8"/>
+      <c r="F62" s="7"/>
       <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
@@ -1646,7 +1851,7 @@
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
       <c r="E63" s="2"/>
-      <c r="F63" s="8"/>
+      <c r="F63" s="7"/>
       <c r="G63" s="2"/>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
@@ -1659,7 +1864,7 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
       <c r="E64" s="2"/>
-      <c r="F64" s="8"/>
+      <c r="F64" s="7"/>
       <c r="G64" s="2"/>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
@@ -1672,7 +1877,7 @@
       <c r="C65" s="2"/>
       <c r="D65" s="2"/>
       <c r="E65" s="2"/>
-      <c r="F65" s="8"/>
+      <c r="F65" s="7"/>
       <c r="G65" s="2"/>
       <c r="H65" s="2"/>
       <c r="I65" s="2"/>
@@ -1685,7 +1890,7 @@
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
       <c r="E66" s="2"/>
-      <c r="F66" s="8"/>
+      <c r="F66" s="7"/>
       <c r="G66" s="2"/>
       <c r="H66" s="2"/>
       <c r="I66" s="2"/>
@@ -1698,7 +1903,7 @@
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
       <c r="E67" s="2"/>
-      <c r="F67" s="8"/>
+      <c r="F67" s="7"/>
       <c r="G67" s="2"/>
       <c r="H67" s="2"/>
       <c r="I67" s="2"/>
@@ -1711,7 +1916,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
       <c r="E68" s="2"/>
-      <c r="F68" s="8"/>
+      <c r="F68" s="7"/>
       <c r="G68" s="2"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
@@ -1724,7 +1929,7 @@
       <c r="C69" s="2"/>
       <c r="D69" s="2"/>
       <c r="E69" s="2"/>
-      <c r="F69" s="8"/>
+      <c r="F69" s="7"/>
       <c r="G69" s="2"/>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
@@ -1737,7 +1942,7 @@
       <c r="C70" s="2"/>
       <c r="D70" s="2"/>
       <c r="E70" s="2"/>
-      <c r="F70" s="8"/>
+      <c r="F70" s="7"/>
       <c r="G70" s="2"/>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -1750,7 +1955,7 @@
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
       <c r="E71" s="2"/>
-      <c r="F71" s="8"/>
+      <c r="F71" s="7"/>
       <c r="G71" s="2"/>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
@@ -1763,7 +1968,7 @@
       <c r="C72" s="2"/>
       <c r="D72" s="2"/>
       <c r="E72" s="2"/>
-      <c r="F72" s="8"/>
+      <c r="F72" s="7"/>
       <c r="G72" s="2"/>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
@@ -1776,7 +1981,7 @@
       <c r="C73" s="2"/>
       <c r="D73" s="2"/>
       <c r="E73" s="2"/>
-      <c r="F73" s="8"/>
+      <c r="F73" s="7"/>
       <c r="G73" s="2"/>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
@@ -1789,7 +1994,7 @@
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
       <c r="E74" s="2"/>
-      <c r="F74" s="8"/>
+      <c r="F74" s="7"/>
       <c r="G74" s="2"/>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
@@ -1802,7 +2007,7 @@
       <c r="C75" s="2"/>
       <c r="D75" s="2"/>
       <c r="E75" s="2"/>
-      <c r="F75" s="8"/>
+      <c r="F75" s="7"/>
       <c r="G75" s="2"/>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
@@ -1815,7 +2020,7 @@
       <c r="C76" s="2"/>
       <c r="D76" s="2"/>
       <c r="E76" s="2"/>
-      <c r="F76" s="8"/>
+      <c r="F76" s="7"/>
       <c r="G76" s="2"/>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -1828,7 +2033,7 @@
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
       <c r="E77" s="2"/>
-      <c r="F77" s="8"/>
+      <c r="F77" s="7"/>
       <c r="G77" s="2"/>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -1841,7 +2046,7 @@
       <c r="C78" s="2"/>
       <c r="D78" s="2"/>
       <c r="E78" s="2"/>
-      <c r="F78" s="8"/>
+      <c r="F78" s="7"/>
       <c r="G78" s="2"/>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -1854,7 +2059,7 @@
       <c r="C79" s="2"/>
       <c r="D79" s="2"/>
       <c r="E79" s="2"/>
-      <c r="F79" s="8"/>
+      <c r="F79" s="7"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
@@ -1867,7 +2072,7 @@
       <c r="C80" s="2"/>
       <c r="D80" s="2"/>
       <c r="E80" s="2"/>
-      <c r="F80" s="8"/>
+      <c r="F80" s="7"/>
       <c r="G80" s="2"/>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
@@ -1880,7 +2085,7 @@
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
       <c r="E81" s="2"/>
-      <c r="F81" s="8"/>
+      <c r="F81" s="7"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
@@ -1893,7 +2098,7 @@
       <c r="C82" s="2"/>
       <c r="D82" s="2"/>
       <c r="E82" s="2"/>
-      <c r="F82" s="8"/>
+      <c r="F82" s="7"/>
       <c r="G82" s="2"/>
       <c r="H82" s="2"/>
       <c r="I82" s="2"/>
@@ -1906,7 +2111,7 @@
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
       <c r="E83" s="2"/>
-      <c r="F83" s="8"/>
+      <c r="F83" s="7"/>
       <c r="G83" s="2"/>
       <c r="H83" s="2"/>
       <c r="I83" s="2"/>
@@ -1919,7 +2124,7 @@
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
       <c r="E84" s="2"/>
-      <c r="F84" s="8"/>
+      <c r="F84" s="7"/>
       <c r="G84" s="2"/>
       <c r="H84" s="2"/>
       <c r="I84" s="2"/>
@@ -1932,7 +2137,7 @@
       <c r="C85" s="2"/>
       <c r="D85" s="2"/>
       <c r="E85" s="2"/>
-      <c r="F85" s="8"/>
+      <c r="F85" s="7"/>
       <c r="G85" s="2"/>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -1945,7 +2150,7 @@
       <c r="C86" s="2"/>
       <c r="D86" s="2"/>
       <c r="E86" s="2"/>
-      <c r="F86" s="8"/>
+      <c r="F86" s="7"/>
       <c r="G86" s="2"/>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
@@ -1958,7 +2163,7 @@
       <c r="C87" s="2"/>
       <c r="D87" s="2"/>
       <c r="E87" s="2"/>
-      <c r="F87" s="8"/>
+      <c r="F87" s="7"/>
       <c r="G87" s="2"/>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -1971,7 +2176,7 @@
       <c r="C88" s="2"/>
       <c r="D88" s="2"/>
       <c r="E88" s="2"/>
-      <c r="F88" s="8"/>
+      <c r="F88" s="7"/>
       <c r="G88" s="2"/>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -1984,7 +2189,7 @@
       <c r="C89" s="2"/>
       <c r="D89" s="2"/>
       <c r="E89" s="2"/>
-      <c r="F89" s="8"/>
+      <c r="F89" s="7"/>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
@@ -1997,7 +2202,7 @@
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
       <c r="E90" s="2"/>
-      <c r="F90" s="8"/>
+      <c r="F90" s="7"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
       <c r="I90" s="2"/>
@@ -2010,7 +2215,7 @@
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
       <c r="E91" s="2"/>
-      <c r="F91" s="8"/>
+      <c r="F91" s="7"/>
       <c r="G91" s="2"/>
       <c r="H91" s="2"/>
       <c r="I91" s="2"/>
@@ -2023,7 +2228,7 @@
       <c r="C92" s="2"/>
       <c r="D92" s="2"/>
       <c r="E92" s="2"/>
-      <c r="F92" s="8"/>
+      <c r="F92" s="7"/>
       <c r="G92" s="2"/>
       <c r="H92" s="2"/>
       <c r="I92" s="2"/>
@@ -2036,7 +2241,7 @@
       <c r="C93" s="2"/>
       <c r="D93" s="2"/>
       <c r="E93" s="2"/>
-      <c r="F93" s="8"/>
+      <c r="F93" s="7"/>
       <c r="G93" s="2"/>
       <c r="H93" s="2"/>
       <c r="I93" s="2"/>
@@ -2049,7 +2254,7 @@
       <c r="C94" s="2"/>
       <c r="D94" s="2"/>
       <c r="E94" s="2"/>
-      <c r="F94" s="8"/>
+      <c r="F94" s="7"/>
       <c r="G94" s="2"/>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
@@ -2062,7 +2267,7 @@
       <c r="C95" s="2"/>
       <c r="D95" s="2"/>
       <c r="E95" s="2"/>
-      <c r="F95" s="8"/>
+      <c r="F95" s="7"/>
       <c r="G95" s="2"/>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
@@ -2075,7 +2280,7 @@
       <c r="C96" s="2"/>
       <c r="D96" s="2"/>
       <c r="E96" s="2"/>
-      <c r="F96" s="8"/>
+      <c r="F96" s="7"/>
       <c r="G96" s="2"/>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
@@ -2088,7 +2293,7 @@
       <c r="C97" s="2"/>
       <c r="D97" s="2"/>
       <c r="E97" s="2"/>
-      <c r="F97" s="8"/>
+      <c r="F97" s="7"/>
       <c r="G97" s="2"/>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
@@ -2101,7 +2306,7 @@
       <c r="C98" s="2"/>
       <c r="D98" s="2"/>
       <c r="E98" s="2"/>
-      <c r="F98" s="8"/>
+      <c r="F98" s="7"/>
       <c r="G98" s="2"/>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
@@ -2114,7 +2319,7 @@
       <c r="C99" s="2"/>
       <c r="D99" s="2"/>
       <c r="E99" s="2"/>
-      <c r="F99" s="8"/>
+      <c r="F99" s="7"/>
       <c r="G99" s="2"/>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
@@ -2127,7 +2332,7 @@
       <c r="C100" s="2"/>
       <c r="D100" s="2"/>
       <c r="E100" s="2"/>
-      <c r="F100" s="8"/>
+      <c r="F100" s="7"/>
       <c r="G100" s="2"/>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
@@ -2140,7 +2345,7 @@
       <c r="C101" s="2"/>
       <c r="D101" s="2"/>
       <c r="E101" s="2"/>
-      <c r="F101" s="8"/>
+      <c r="F101" s="7"/>
       <c r="G101" s="2"/>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
@@ -2153,7 +2358,7 @@
       <c r="C102" s="2"/>
       <c r="D102" s="2"/>
       <c r="E102" s="2"/>
-      <c r="F102" s="8"/>
+      <c r="F102" s="7"/>
       <c r="G102" s="2"/>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
@@ -2166,7 +2371,7 @@
       <c r="C103" s="2"/>
       <c r="D103" s="2"/>
       <c r="E103" s="2"/>
-      <c r="F103" s="8"/>
+      <c r="F103" s="7"/>
       <c r="G103" s="2"/>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
@@ -2179,7 +2384,7 @@
       <c r="C104" s="2"/>
       <c r="D104" s="2"/>
       <c r="E104" s="2"/>
-      <c r="F104" s="8"/>
+      <c r="F104" s="7"/>
       <c r="G104" s="2"/>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
@@ -2192,7 +2397,7 @@
       <c r="C105" s="2"/>
       <c r="D105" s="2"/>
       <c r="E105" s="2"/>
-      <c r="F105" s="8"/>
+      <c r="F105" s="7"/>
       <c r="G105" s="2"/>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
@@ -2205,7 +2410,7 @@
       <c r="C106" s="2"/>
       <c r="D106" s="2"/>
       <c r="E106" s="2"/>
-      <c r="F106" s="8"/>
+      <c r="F106" s="7"/>
       <c r="G106" s="2"/>
       <c r="H106" s="2"/>
       <c r="I106" s="2"/>
@@ -2218,7 +2423,7 @@
       <c r="C107" s="2"/>
       <c r="D107" s="2"/>
       <c r="E107" s="2"/>
-      <c r="F107" s="8"/>
+      <c r="F107" s="7"/>
       <c r="G107" s="2"/>
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
@@ -2231,7 +2436,7 @@
       <c r="C108" s="2"/>
       <c r="D108" s="2"/>
       <c r="E108" s="2"/>
-      <c r="F108" s="8"/>
+      <c r="F108" s="7"/>
       <c r="G108" s="2"/>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
@@ -2244,7 +2449,7 @@
       <c r="C109" s="2"/>
       <c r="D109" s="2"/>
       <c r="E109" s="2"/>
-      <c r="F109" s="8"/>
+      <c r="F109" s="7"/>
       <c r="G109" s="2"/>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
@@ -2257,7 +2462,7 @@
       <c r="C110" s="2"/>
       <c r="D110" s="2"/>
       <c r="E110" s="2"/>
-      <c r="F110" s="8"/>
+      <c r="F110" s="7"/>
       <c r="G110" s="2"/>
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
@@ -2270,7 +2475,7 @@
       <c r="C111" s="2"/>
       <c r="D111" s="2"/>
       <c r="E111" s="2"/>
-      <c r="F111" s="8"/>
+      <c r="F111" s="7"/>
       <c r="G111" s="2"/>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
@@ -2283,7 +2488,7 @@
       <c r="C112" s="2"/>
       <c r="D112" s="2"/>
       <c r="E112" s="2"/>
-      <c r="F112" s="8"/>
+      <c r="F112" s="7"/>
       <c r="G112" s="2"/>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
@@ -2296,7 +2501,7 @@
       <c r="C113" s="2"/>
       <c r="D113" s="2"/>
       <c r="E113" s="2"/>
-      <c r="F113" s="8"/>
+      <c r="F113" s="7"/>
       <c r="G113" s="2"/>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
@@ -2309,7 +2514,7 @@
       <c r="C114" s="2"/>
       <c r="D114" s="2"/>
       <c r="E114" s="2"/>
-      <c r="F114" s="8"/>
+      <c r="F114" s="7"/>
       <c r="G114" s="2"/>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
@@ -2322,7 +2527,7 @@
       <c r="C115" s="2"/>
       <c r="D115" s="2"/>
       <c r="E115" s="2"/>
-      <c r="F115" s="8"/>
+      <c r="F115" s="7"/>
       <c r="G115" s="2"/>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
@@ -2335,7 +2540,7 @@
       <c r="C116" s="2"/>
       <c r="D116" s="2"/>
       <c r="E116" s="2"/>
-      <c r="F116" s="8"/>
+      <c r="F116" s="7"/>
       <c r="G116" s="2"/>
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
@@ -2348,7 +2553,7 @@
       <c r="C117" s="2"/>
       <c r="D117" s="2"/>
       <c r="E117" s="2"/>
-      <c r="F117" s="8"/>
+      <c r="F117" s="7"/>
       <c r="G117" s="2"/>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
@@ -2361,7 +2566,7 @@
       <c r="C118" s="2"/>
       <c r="D118" s="2"/>
       <c r="E118" s="2"/>
-      <c r="F118" s="8"/>
+      <c r="F118" s="7"/>
       <c r="G118" s="2"/>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
@@ -2374,7 +2579,7 @@
       <c r="C119" s="2"/>
       <c r="D119" s="2"/>
       <c r="E119" s="2"/>
-      <c r="F119" s="8"/>
+      <c r="F119" s="7"/>
       <c r="G119" s="2"/>
       <c r="H119" s="2"/>
       <c r="I119" s="2"/>
@@ -2387,7 +2592,7 @@
       <c r="C120" s="2"/>
       <c r="D120" s="2"/>
       <c r="E120" s="2"/>
-      <c r="F120" s="8"/>
+      <c r="F120" s="7"/>
       <c r="G120" s="2"/>
       <c r="H120" s="2"/>
       <c r="I120" s="2"/>
@@ -2400,7 +2605,7 @@
       <c r="C121" s="2"/>
       <c r="D121" s="2"/>
       <c r="E121" s="2"/>
-      <c r="F121" s="8"/>
+      <c r="F121" s="7"/>
       <c r="G121" s="2"/>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
@@ -2413,7 +2618,7 @@
       <c r="C122" s="2"/>
       <c r="D122" s="2"/>
       <c r="E122" s="2"/>
-      <c r="F122" s="8"/>
+      <c r="F122" s="7"/>
       <c r="G122" s="2"/>
       <c r="H122" s="2"/>
       <c r="I122" s="2"/>
@@ -2426,7 +2631,7 @@
       <c r="C123" s="2"/>
       <c r="D123" s="2"/>
       <c r="E123" s="2"/>
-      <c r="F123" s="8"/>
+      <c r="F123" s="7"/>
       <c r="G123" s="2"/>
       <c r="H123" s="2"/>
       <c r="I123" s="2"/>
@@ -2439,7 +2644,7 @@
       <c r="C124" s="2"/>
       <c r="D124" s="2"/>
       <c r="E124" s="2"/>
-      <c r="F124" s="8"/>
+      <c r="F124" s="7"/>
       <c r="G124" s="2"/>
       <c r="H124" s="2"/>
       <c r="I124" s="2"/>
@@ -2452,7 +2657,7 @@
       <c r="C125" s="2"/>
       <c r="D125" s="2"/>
       <c r="E125" s="2"/>
-      <c r="F125" s="8"/>
+      <c r="F125" s="7"/>
       <c r="G125" s="2"/>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
@@ -2465,7 +2670,7 @@
       <c r="C126" s="2"/>
       <c r="D126" s="2"/>
       <c r="E126" s="2"/>
-      <c r="F126" s="8"/>
+      <c r="F126" s="7"/>
       <c r="G126" s="2"/>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
@@ -2478,7 +2683,7 @@
       <c r="C127" s="2"/>
       <c r="D127" s="2"/>
       <c r="E127" s="2"/>
-      <c r="F127" s="8"/>
+      <c r="F127" s="7"/>
       <c r="G127" s="2"/>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
@@ -2491,7 +2696,7 @@
       <c r="C128" s="2"/>
       <c r="D128" s="2"/>
       <c r="E128" s="2"/>
-      <c r="F128" s="8"/>
+      <c r="F128" s="7"/>
       <c r="G128" s="2"/>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
@@ -2504,7 +2709,7 @@
       <c r="C129" s="2"/>
       <c r="D129" s="2"/>
       <c r="E129" s="2"/>
-      <c r="F129" s="8"/>
+      <c r="F129" s="7"/>
       <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
@@ -2517,7 +2722,7 @@
       <c r="C130" s="2"/>
       <c r="D130" s="2"/>
       <c r="E130" s="2"/>
-      <c r="F130" s="8"/>
+      <c r="F130" s="7"/>
       <c r="G130" s="2"/>
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
@@ -2530,7 +2735,7 @@
       <c r="C131" s="2"/>
       <c r="D131" s="2"/>
       <c r="E131" s="2"/>
-      <c r="F131" s="8"/>
+      <c r="F131" s="7"/>
       <c r="G131" s="2"/>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
@@ -2543,7 +2748,7 @@
       <c r="C132" s="2"/>
       <c r="D132" s="2"/>
       <c r="E132" s="2"/>
-      <c r="F132" s="8"/>
+      <c r="F132" s="7"/>
       <c r="G132" s="2"/>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
@@ -2556,7 +2761,7 @@
       <c r="C133" s="2"/>
       <c r="D133" s="2"/>
       <c r="E133" s="2"/>
-      <c r="F133" s="8"/>
+      <c r="F133" s="7"/>
       <c r="G133" s="2"/>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
@@ -2569,7 +2774,7 @@
       <c r="C134" s="2"/>
       <c r="D134" s="2"/>
       <c r="E134" s="2"/>
-      <c r="F134" s="8"/>
+      <c r="F134" s="7"/>
       <c r="G134" s="2"/>
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
@@ -2582,7 +2787,7 @@
       <c r="C135" s="2"/>
       <c r="D135" s="2"/>
       <c r="E135" s="2"/>
-      <c r="F135" s="8"/>
+      <c r="F135" s="7"/>
       <c r="G135" s="2"/>
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
@@ -2595,7 +2800,7 @@
       <c r="C136" s="2"/>
       <c r="D136" s="2"/>
       <c r="E136" s="2"/>
-      <c r="F136" s="8"/>
+      <c r="F136" s="7"/>
       <c r="G136" s="2"/>
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
@@ -2608,7 +2813,7 @@
       <c r="C137" s="2"/>
       <c r="D137" s="2"/>
       <c r="E137" s="2"/>
-      <c r="F137" s="8"/>
+      <c r="F137" s="7"/>
       <c r="G137" s="2"/>
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
@@ -2621,7 +2826,7 @@
       <c r="C138" s="2"/>
       <c r="D138" s="2"/>
       <c r="E138" s="2"/>
-      <c r="F138" s="8"/>
+      <c r="F138" s="7"/>
       <c r="G138" s="2"/>
       <c r="H138" s="2"/>
       <c r="I138" s="2"/>
@@ -2634,7 +2839,7 @@
       <c r="C139" s="2"/>
       <c r="D139" s="2"/>
       <c r="E139" s="2"/>
-      <c r="F139" s="8"/>
+      <c r="F139" s="7"/>
       <c r="G139" s="2"/>
       <c r="H139" s="2"/>
       <c r="I139" s="2"/>
@@ -2647,7 +2852,7 @@
       <c r="C140" s="2"/>
       <c r="D140" s="2"/>
       <c r="E140" s="2"/>
-      <c r="F140" s="8"/>
+      <c r="F140" s="7"/>
       <c r="G140" s="2"/>
       <c r="H140" s="2"/>
       <c r="I140" s="2"/>
@@ -2660,7 +2865,7 @@
       <c r="C141" s="2"/>
       <c r="D141" s="2"/>
       <c r="E141" s="2"/>
-      <c r="F141" s="8"/>
+      <c r="F141" s="7"/>
       <c r="G141" s="2"/>
       <c r="H141" s="2"/>
       <c r="I141" s="2"/>
@@ -2673,7 +2878,7 @@
       <c r="C142" s="2"/>
       <c r="D142" s="2"/>
       <c r="E142" s="2"/>
-      <c r="F142" s="8"/>
+      <c r="F142" s="7"/>
       <c r="G142" s="2"/>
       <c r="H142" s="2"/>
       <c r="I142" s="2"/>
@@ -2686,7 +2891,7 @@
       <c r="C143" s="2"/>
       <c r="D143" s="2"/>
       <c r="E143" s="2"/>
-      <c r="F143" s="8"/>
+      <c r="F143" s="7"/>
       <c r="G143" s="2"/>
       <c r="H143" s="2"/>
       <c r="I143" s="2"/>
@@ -2699,7 +2904,7 @@
       <c r="C144" s="2"/>
       <c r="D144" s="2"/>
       <c r="E144" s="2"/>
-      <c r="F144" s="8"/>
+      <c r="F144" s="7"/>
       <c r="G144" s="2"/>
       <c r="H144" s="2"/>
       <c r="I144" s="2"/>
@@ -2712,7 +2917,7 @@
       <c r="C145" s="2"/>
       <c r="D145" s="2"/>
       <c r="E145" s="2"/>
-      <c r="F145" s="8"/>
+      <c r="F145" s="7"/>
       <c r="G145" s="2"/>
       <c r="H145" s="2"/>
       <c r="I145" s="2"/>
@@ -2725,7 +2930,7 @@
       <c r="C146" s="2"/>
       <c r="D146" s="2"/>
       <c r="E146" s="2"/>
-      <c r="F146" s="8"/>
+      <c r="F146" s="7"/>
       <c r="G146" s="2"/>
       <c r="H146" s="2"/>
       <c r="I146" s="2"/>
@@ -2738,7 +2943,7 @@
       <c r="C147" s="2"/>
       <c r="D147" s="2"/>
       <c r="E147" s="2"/>
-      <c r="F147" s="8"/>
+      <c r="F147" s="7"/>
       <c r="G147" s="2"/>
       <c r="H147" s="2"/>
       <c r="I147" s="2"/>
@@ -2751,7 +2956,7 @@
       <c r="C148" s="2"/>
       <c r="D148" s="2"/>
       <c r="E148" s="2"/>
-      <c r="F148" s="8"/>
+      <c r="F148" s="7"/>
       <c r="G148" s="2"/>
       <c r="H148" s="2"/>
       <c r="I148" s="2"/>
@@ -2764,7 +2969,7 @@
       <c r="C149" s="2"/>
       <c r="D149" s="2"/>
       <c r="E149" s="2"/>
-      <c r="F149" s="8"/>
+      <c r="F149" s="7"/>
       <c r="G149" s="2"/>
       <c r="H149" s="2"/>
       <c r="I149" s="2"/>
@@ -2777,7 +2982,7 @@
       <c r="C150" s="2"/>
       <c r="D150" s="2"/>
       <c r="E150" s="2"/>
-      <c r="F150" s="8"/>
+      <c r="F150" s="7"/>
       <c r="G150" s="2"/>
       <c r="H150" s="2"/>
       <c r="I150" s="2"/>
@@ -2790,7 +2995,7 @@
       <c r="C151" s="2"/>
       <c r="D151" s="2"/>
       <c r="E151" s="2"/>
-      <c r="F151" s="8"/>
+      <c r="F151" s="7"/>
       <c r="G151" s="2"/>
       <c r="H151" s="2"/>
       <c r="I151" s="2"/>
@@ -2803,7 +3008,7 @@
       <c r="C152" s="2"/>
       <c r="D152" s="2"/>
       <c r="E152" s="2"/>
-      <c r="F152" s="8"/>
+      <c r="F152" s="7"/>
       <c r="G152" s="2"/>
       <c r="H152" s="2"/>
       <c r="I152" s="2"/>
@@ -2816,7 +3021,7 @@
       <c r="C153" s="2"/>
       <c r="D153" s="2"/>
       <c r="E153" s="2"/>
-      <c r="F153" s="8"/>
+      <c r="F153" s="7"/>
       <c r="G153" s="2"/>
       <c r="H153" s="2"/>
       <c r="I153" s="2"/>
@@ -2829,7 +3034,7 @@
       <c r="C154" s="2"/>
       <c r="D154" s="2"/>
       <c r="E154" s="2"/>
-      <c r="F154" s="8"/>
+      <c r="F154" s="7"/>
       <c r="G154" s="2"/>
       <c r="H154" s="2"/>
       <c r="I154" s="2"/>
@@ -2842,7 +3047,7 @@
       <c r="C155" s="2"/>
       <c r="D155" s="2"/>
       <c r="E155" s="2"/>
-      <c r="F155" s="8"/>
+      <c r="F155" s="7"/>
       <c r="G155" s="2"/>
       <c r="H155" s="2"/>
       <c r="I155" s="2"/>
@@ -2855,7 +3060,7 @@
       <c r="C156" s="2"/>
       <c r="D156" s="2"/>
       <c r="E156" s="2"/>
-      <c r="F156" s="8"/>
+      <c r="F156" s="7"/>
       <c r="G156" s="2"/>
       <c r="H156" s="2"/>
       <c r="I156" s="2"/>
@@ -2868,7 +3073,7 @@
       <c r="C157" s="2"/>
       <c r="D157" s="2"/>
       <c r="E157" s="2"/>
-      <c r="F157" s="8"/>
+      <c r="F157" s="7"/>
       <c r="G157" s="2"/>
       <c r="H157" s="2"/>
       <c r="I157" s="2"/>
@@ -2881,7 +3086,7 @@
       <c r="C158" s="2"/>
       <c r="D158" s="2"/>
       <c r="E158" s="2"/>
-      <c r="F158" s="8"/>
+      <c r="F158" s="7"/>
       <c r="G158" s="2"/>
       <c r="H158" s="2"/>
       <c r="I158" s="2"/>
@@ -2894,7 +3099,7 @@
       <c r="C159" s="2"/>
       <c r="D159" s="2"/>
       <c r="E159" s="2"/>
-      <c r="F159" s="8"/>
+      <c r="F159" s="7"/>
       <c r="G159" s="2"/>
       <c r="H159" s="2"/>
       <c r="I159" s="2"/>
@@ -2907,7 +3112,7 @@
       <c r="C160" s="2"/>
       <c r="D160" s="2"/>
       <c r="E160" s="2"/>
-      <c r="F160" s="8"/>
+      <c r="F160" s="7"/>
       <c r="G160" s="2"/>
       <c r="H160" s="2"/>
       <c r="I160" s="2"/>
@@ -2920,7 +3125,7 @@
       <c r="C161" s="2"/>
       <c r="D161" s="2"/>
       <c r="E161" s="2"/>
-      <c r="F161" s="8"/>
+      <c r="F161" s="7"/>
       <c r="G161" s="2"/>
       <c r="H161" s="2"/>
       <c r="I161" s="2"/>
@@ -2933,7 +3138,7 @@
       <c r="C162" s="2"/>
       <c r="D162" s="2"/>
       <c r="E162" s="2"/>
-      <c r="F162" s="8"/>
+      <c r="F162" s="7"/>
       <c r="G162" s="2"/>
       <c r="H162" s="2"/>
       <c r="I162" s="2"/>
@@ -2946,7 +3151,7 @@
       <c r="C163" s="2"/>
       <c r="D163" s="2"/>
       <c r="E163" s="2"/>
-      <c r="F163" s="8"/>
+      <c r="F163" s="7"/>
       <c r="G163" s="2"/>
       <c r="H163" s="2"/>
       <c r="I163" s="2"/>
@@ -2959,7 +3164,7 @@
       <c r="C164" s="2"/>
       <c r="D164" s="2"/>
       <c r="E164" s="2"/>
-      <c r="F164" s="8"/>
+      <c r="F164" s="7"/>
       <c r="G164" s="2"/>
       <c r="H164" s="2"/>
       <c r="I164" s="2"/>
@@ -2972,7 +3177,7 @@
       <c r="C165" s="2"/>
       <c r="D165" s="2"/>
       <c r="E165" s="2"/>
-      <c r="F165" s="8"/>
+      <c r="F165" s="7"/>
       <c r="G165" s="2"/>
       <c r="H165" s="2"/>
       <c r="I165" s="2"/>
@@ -2985,7 +3190,7 @@
       <c r="C166" s="2"/>
       <c r="D166" s="2"/>
       <c r="E166" s="2"/>
-      <c r="F166" s="8"/>
+      <c r="F166" s="7"/>
       <c r="G166" s="2"/>
       <c r="H166" s="2"/>
       <c r="I166" s="2"/>
@@ -2998,7 +3203,7 @@
       <c r="C167" s="2"/>
       <c r="D167" s="2"/>
       <c r="E167" s="2"/>
-      <c r="F167" s="8"/>
+      <c r="F167" s="7"/>
       <c r="G167" s="2"/>
       <c r="H167" s="2"/>
       <c r="I167" s="2"/>
@@ -3011,7 +3216,7 @@
       <c r="C168" s="2"/>
       <c r="D168" s="2"/>
       <c r="E168" s="2"/>
-      <c r="F168" s="8"/>
+      <c r="F168" s="7"/>
       <c r="G168" s="2"/>
       <c r="H168" s="2"/>
       <c r="I168" s="2"/>
@@ -3024,7 +3229,7 @@
       <c r="C169" s="2"/>
       <c r="D169" s="2"/>
       <c r="E169" s="2"/>
-      <c r="F169" s="8"/>
+      <c r="F169" s="7"/>
       <c r="G169" s="2"/>
       <c r="H169" s="2"/>
       <c r="I169" s="2"/>
@@ -3037,7 +3242,7 @@
       <c r="C170" s="2"/>
       <c r="D170" s="2"/>
       <c r="E170" s="2"/>
-      <c r="F170" s="8"/>
+      <c r="F170" s="7"/>
       <c r="G170" s="2"/>
       <c r="H170" s="2"/>
       <c r="I170" s="2"/>
@@ -3050,7 +3255,7 @@
       <c r="C171" s="2"/>
       <c r="D171" s="2"/>
       <c r="E171" s="2"/>
-      <c r="F171" s="8"/>
+      <c r="F171" s="7"/>
       <c r="G171" s="2"/>
       <c r="H171" s="2"/>
       <c r="I171" s="2"/>
@@ -3063,7 +3268,7 @@
       <c r="C172" s="2"/>
       <c r="D172" s="2"/>
       <c r="E172" s="2"/>
-      <c r="F172" s="8"/>
+      <c r="F172" s="7"/>
       <c r="G172" s="2"/>
       <c r="H172" s="2"/>
       <c r="I172" s="2"/>
@@ -3076,7 +3281,7 @@
       <c r="C173" s="2"/>
       <c r="D173" s="2"/>
       <c r="E173" s="2"/>
-      <c r="F173" s="8"/>
+      <c r="F173" s="7"/>
       <c r="G173" s="2"/>
       <c r="H173" s="2"/>
       <c r="I173" s="2"/>
@@ -3089,7 +3294,7 @@
       <c r="C174" s="2"/>
       <c r="D174" s="2"/>
       <c r="E174" s="2"/>
-      <c r="F174" s="8"/>
+      <c r="F174" s="7"/>
       <c r="G174" s="2"/>
       <c r="H174" s="2"/>
       <c r="I174" s="2"/>
@@ -3102,7 +3307,7 @@
       <c r="C175" s="2"/>
       <c r="D175" s="2"/>
       <c r="E175" s="2"/>
-      <c r="F175" s="8"/>
+      <c r="F175" s="7"/>
       <c r="G175" s="2"/>
       <c r="H175" s="2"/>
       <c r="I175" s="2"/>
@@ -3115,7 +3320,7 @@
       <c r="C176" s="2"/>
       <c r="D176" s="2"/>
       <c r="E176" s="2"/>
-      <c r="F176" s="8"/>
+      <c r="F176" s="7"/>
       <c r="G176" s="2"/>
       <c r="H176" s="2"/>
       <c r="I176" s="2"/>
@@ -3128,7 +3333,7 @@
       <c r="C177" s="2"/>
       <c r="D177" s="2"/>
       <c r="E177" s="2"/>
-      <c r="F177" s="8"/>
+      <c r="F177" s="7"/>
       <c r="G177" s="2"/>
       <c r="H177" s="2"/>
       <c r="I177" s="2"/>
@@ -3141,7 +3346,7 @@
       <c r="C178" s="2"/>
       <c r="D178" s="2"/>
       <c r="E178" s="2"/>
-      <c r="F178" s="8"/>
+      <c r="F178" s="7"/>
       <c r="G178" s="2"/>
       <c r="H178" s="2"/>
       <c r="I178" s="2"/>
@@ -3154,7 +3359,7 @@
       <c r="C179" s="2"/>
       <c r="D179" s="2"/>
       <c r="E179" s="2"/>
-      <c r="F179" s="8"/>
+      <c r="F179" s="7"/>
       <c r="G179" s="2"/>
       <c r="H179" s="2"/>
       <c r="I179" s="2"/>
@@ -3167,7 +3372,7 @@
       <c r="C180" s="2"/>
       <c r="D180" s="2"/>
       <c r="E180" s="2"/>
-      <c r="F180" s="8"/>
+      <c r="F180" s="7"/>
       <c r="G180" s="2"/>
       <c r="H180" s="2"/>
       <c r="I180" s="2"/>
@@ -3180,7 +3385,7 @@
       <c r="C181" s="2"/>
       <c r="D181" s="2"/>
       <c r="E181" s="2"/>
-      <c r="F181" s="8"/>
+      <c r="F181" s="7"/>
       <c r="G181" s="2"/>
       <c r="H181" s="2"/>
       <c r="I181" s="2"/>
@@ -3193,7 +3398,7 @@
       <c r="C182" s="2"/>
       <c r="D182" s="2"/>
       <c r="E182" s="2"/>
-      <c r="F182" s="8"/>
+      <c r="F182" s="7"/>
       <c r="G182" s="2"/>
       <c r="H182" s="2"/>
       <c r="I182" s="2"/>
@@ -3206,7 +3411,7 @@
       <c r="C183" s="2"/>
       <c r="D183" s="2"/>
       <c r="E183" s="2"/>
-      <c r="F183" s="8"/>
+      <c r="F183" s="7"/>
       <c r="G183" s="2"/>
       <c r="H183" s="2"/>
       <c r="I183" s="2"/>
@@ -3219,7 +3424,7 @@
       <c r="C184" s="2"/>
       <c r="D184" s="2"/>
       <c r="E184" s="2"/>
-      <c r="F184" s="8"/>
+      <c r="F184" s="7"/>
       <c r="G184" s="2"/>
       <c r="H184" s="2"/>
       <c r="I184" s="2"/>
@@ -3232,7 +3437,7 @@
       <c r="C185" s="2"/>
       <c r="D185" s="2"/>
       <c r="E185" s="2"/>
-      <c r="F185" s="8"/>
+      <c r="F185" s="7"/>
       <c r="G185" s="2"/>
       <c r="H185" s="2"/>
       <c r="I185" s="2"/>
@@ -3245,7 +3450,7 @@
       <c r="C186" s="2"/>
       <c r="D186" s="2"/>
       <c r="E186" s="2"/>
-      <c r="F186" s="8"/>
+      <c r="F186" s="7"/>
       <c r="G186" s="2"/>
       <c r="H186" s="2"/>
       <c r="I186" s="2"/>
@@ -3258,7 +3463,7 @@
       <c r="C187" s="2"/>
       <c r="D187" s="2"/>
       <c r="E187" s="2"/>
-      <c r="F187" s="8"/>
+      <c r="F187" s="7"/>
       <c r="G187" s="2"/>
       <c r="H187" s="2"/>
       <c r="I187" s="2"/>
@@ -3271,7 +3476,7 @@
       <c r="C188" s="2"/>
       <c r="D188" s="2"/>
       <c r="E188" s="2"/>
-      <c r="F188" s="8"/>
+      <c r="F188" s="7"/>
       <c r="G188" s="2"/>
       <c r="H188" s="2"/>
       <c r="I188" s="2"/>
@@ -3284,7 +3489,7 @@
       <c r="C189" s="2"/>
       <c r="D189" s="2"/>
       <c r="E189" s="2"/>
-      <c r="F189" s="8"/>
+      <c r="F189" s="7"/>
       <c r="G189" s="2"/>
       <c r="H189" s="2"/>
       <c r="I189" s="2"/>
@@ -3297,7 +3502,7 @@
       <c r="C190" s="2"/>
       <c r="D190" s="2"/>
       <c r="E190" s="2"/>
-      <c r="F190" s="8"/>
+      <c r="F190" s="7"/>
       <c r="G190" s="2"/>
       <c r="H190" s="2"/>
       <c r="I190" s="2"/>
@@ -3310,7 +3515,7 @@
       <c r="C191" s="2"/>
       <c r="D191" s="2"/>
       <c r="E191" s="2"/>
-      <c r="F191" s="8"/>
+      <c r="F191" s="7"/>
       <c r="G191" s="2"/>
       <c r="H191" s="2"/>
       <c r="I191" s="2"/>
@@ -3323,7 +3528,7 @@
       <c r="C192" s="2"/>
       <c r="D192" s="2"/>
       <c r="E192" s="2"/>
-      <c r="F192" s="8"/>
+      <c r="F192" s="7"/>
       <c r="G192" s="2"/>
       <c r="H192" s="2"/>
       <c r="I192" s="2"/>
@@ -3336,7 +3541,7 @@
       <c r="C193" s="2"/>
       <c r="D193" s="2"/>
       <c r="E193" s="2"/>
-      <c r="F193" s="8"/>
+      <c r="F193" s="7"/>
       <c r="G193" s="2"/>
       <c r="H193" s="2"/>
       <c r="I193" s="2"/>
@@ -3349,7 +3554,7 @@
       <c r="C194" s="2"/>
       <c r="D194" s="2"/>
       <c r="E194" s="2"/>
-      <c r="F194" s="8"/>
+      <c r="F194" s="7"/>
       <c r="G194" s="2"/>
       <c r="H194" s="2"/>
       <c r="I194" s="2"/>

</xml_diff>

<commit_message>
update phan cua dang lam
</commit_message>
<xml_diff>
--- a/Project Plan/Mesurement.xlsx
+++ b/Project Plan/Mesurement.xlsx
@@ -12,14 +12,48 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$199</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$200</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>DangNguyen</author>
+  </authors>
+  <commentList>
+    <comment ref="B20" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>DangNguyen:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Snario viet lai nha</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="94">
   <si>
     <t>No.</t>
   </si>
@@ -226,13 +260,88 @@
   </si>
   <si>
     <t>13/1/2012</t>
+  </si>
+  <si>
+    <t>Define Detail Design process</t>
+  </si>
+  <si>
+    <t>Detail Design</t>
+  </si>
+  <si>
+    <t>Dang Nguyen</t>
+  </si>
+  <si>
+    <t>Doc Detail Design process</t>
+  </si>
+  <si>
+    <t>Concept of Operation: document Proposed System or Situation</t>
+  </si>
+  <si>
+    <t>Concept of Operation: document Current System or Situation</t>
+  </si>
+  <si>
+    <t>Read, Review and Draw Form of customer</t>
+  </si>
+  <si>
+    <t>Test Plan: ENTRANCE &amp; EXIT CRITERIA</t>
+  </si>
+  <si>
+    <t>Project .Plan: Project Quality Plan</t>
+  </si>
+  <si>
+    <t>Describe Quality Attribute</t>
+  </si>
+  <si>
+    <t>draw current system overview</t>
+  </si>
+  <si>
+    <t>List Use Case</t>
+  </si>
+  <si>
+    <t>draw Register the hour for teacher process</t>
+  </si>
+  <si>
+    <t>Draw Use Case</t>
+  </si>
+  <si>
+    <t>Describe Use Case</t>
+  </si>
+  <si>
+    <t>rework: System feature</t>
+  </si>
+  <si>
+    <t>review SRS</t>
+  </si>
+  <si>
+    <t>design Detail Design template</t>
+  </si>
+  <si>
+    <t>Implement Interface: manage major</t>
+  </si>
+  <si>
+    <t xml:space="preserve">review Use Case Description </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Decribe Detail design Introduction </t>
+  </si>
+  <si>
+    <t>Implement interface: Working Progress and Labor Union</t>
+  </si>
+  <si>
+    <t>Test Case : Working Progress and Labor Union</t>
+  </si>
+  <si>
+    <t>Design Interface: Detail Information</t>
+  </si>
+  <si>
+    <t>Plan Detail Design</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -269,6 +378,19 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -284,7 +406,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -320,6 +442,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -328,7 +489,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -347,87 +508,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="32">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="24">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -946,12 +1041,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I205"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I206"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B48" sqref="B48"/>
+      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2234,304 +2329,626 @@
       <c r="A47" s="3">
         <v>45</v>
       </c>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
+      <c r="B47" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E47" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F47" s="5"/>
-      <c r="G47" s="4"/>
-      <c r="H47" s="4"/>
-      <c r="I47" s="4"/>
+      <c r="G47" s="4">
+        <v>2</v>
+      </c>
+      <c r="H47" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I47" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
         <v>46</v>
       </c>
-      <c r="B48" s="4"/>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
+      <c r="B48" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D48" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E48" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F48" s="5"/>
-      <c r="G48" s="4"/>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4"/>
+      <c r="G48" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="H48" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="I48" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
         <v>47</v>
       </c>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
+      <c r="B49" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E49" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F49" s="5"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
+      <c r="G49" s="4">
+        <v>10</v>
+      </c>
+      <c r="H49" s="4">
+        <v>11.5</v>
+      </c>
+      <c r="I49" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
         <v>48</v>
       </c>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
+      <c r="B50" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F50" s="5"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
+      <c r="G50" s="4">
+        <v>4</v>
+      </c>
+      <c r="H50" s="4">
+        <v>5</v>
+      </c>
+      <c r="I50" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="3">
+      <c r="A51" s="10">
         <v>49</v>
       </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4"/>
-      <c r="D51" s="4"/>
-      <c r="E51" s="4"/>
+      <c r="B51" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C51" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="E51" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F51" s="5"/>
-      <c r="G51" s="4"/>
-      <c r="H51" s="4"/>
-      <c r="I51" s="4"/>
+      <c r="G51" s="4">
+        <v>3</v>
+      </c>
+      <c r="H51" s="4">
+        <v>3</v>
+      </c>
+      <c r="I51" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
         <v>50</v>
       </c>
-      <c r="B52" s="4"/>
-      <c r="C52" s="4"/>
-      <c r="D52" s="4"/>
-      <c r="E52" s="4"/>
+      <c r="B52" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D52" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E52" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F52" s="5"/>
-      <c r="G52" s="4"/>
-      <c r="H52" s="4"/>
-      <c r="I52" s="4"/>
+      <c r="G52" s="4">
+        <v>2</v>
+      </c>
+      <c r="H52" s="4">
+        <v>2</v>
+      </c>
+      <c r="I52" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3">
         <v>51</v>
       </c>
-      <c r="B53" s="4"/>
-      <c r="C53" s="4"/>
-      <c r="D53" s="4"/>
-      <c r="E53" s="4"/>
+      <c r="B53" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F53" s="5"/>
-      <c r="G53" s="4"/>
-      <c r="H53" s="4"/>
-      <c r="I53" s="4"/>
+      <c r="G53" s="4">
+        <v>1</v>
+      </c>
+      <c r="H53" s="4">
+        <v>1</v>
+      </c>
+      <c r="I53" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3">
         <v>52</v>
       </c>
-      <c r="B54" s="4"/>
-      <c r="C54" s="4"/>
-      <c r="D54" s="4"/>
-      <c r="E54" s="4"/>
+      <c r="B54" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D54" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E54" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F54" s="5"/>
-      <c r="G54" s="4"/>
-      <c r="H54" s="4"/>
-      <c r="I54" s="4"/>
+      <c r="G54" s="4">
+        <v>6</v>
+      </c>
+      <c r="H54" s="4">
+        <v>9</v>
+      </c>
+      <c r="I54" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="3">
         <v>53</v>
       </c>
-      <c r="B55" s="4"/>
-      <c r="C55" s="4"/>
-      <c r="D55" s="4"/>
-      <c r="E55" s="4"/>
+      <c r="B55" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D55" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E55" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F55" s="5"/>
-      <c r="G55" s="4"/>
-      <c r="H55" s="4"/>
-      <c r="I55" s="4"/>
+      <c r="G55" s="4">
+        <v>7</v>
+      </c>
+      <c r="H55" s="4">
+        <v>7</v>
+      </c>
+      <c r="I55" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3">
         <v>54</v>
       </c>
-      <c r="B56" s="4"/>
-      <c r="C56" s="4"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4"/>
+      <c r="B56" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D56" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E56" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F56" s="5"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4"/>
+      <c r="G56" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="H56" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I56" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3">
         <v>55</v>
       </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
+      <c r="B57" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E57" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F57" s="5"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
+      <c r="G57" s="4">
+        <v>1</v>
+      </c>
+      <c r="H57" s="4">
+        <v>1</v>
+      </c>
+      <c r="I57" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" s="3">
         <v>56</v>
       </c>
-      <c r="B58" s="4"/>
-      <c r="C58" s="4"/>
-      <c r="D58" s="4"/>
-      <c r="E58" s="4"/>
+      <c r="B58" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D58" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E58" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F58" s="5"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4"/>
+      <c r="G58" s="4">
+        <v>6</v>
+      </c>
+      <c r="H58" s="4">
+        <v>7</v>
+      </c>
+      <c r="I58" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3">
         <v>57</v>
       </c>
-      <c r="B59" s="4"/>
-      <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
+      <c r="B59" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D59" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E59" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F59" s="5"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4"/>
+      <c r="G59" s="4">
+        <v>5</v>
+      </c>
+      <c r="H59" s="4">
+        <v>7</v>
+      </c>
+      <c r="I59" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3">
         <v>58</v>
       </c>
-      <c r="B60" s="4"/>
-      <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="4"/>
+      <c r="B60" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E60" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F60" s="5"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4"/>
+      <c r="G60" s="4">
+        <v>2</v>
+      </c>
+      <c r="H60" s="4">
+        <v>2</v>
+      </c>
+      <c r="I60" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3">
         <v>59</v>
       </c>
-      <c r="B61" s="4"/>
-      <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4"/>
+      <c r="B61" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D61" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E61" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F61" s="5"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4"/>
+      <c r="G61" s="4">
+        <v>3</v>
+      </c>
+      <c r="H61" s="4">
+        <v>2.5</v>
+      </c>
+      <c r="I61" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3">
+        <v>60</v>
+      </c>
+      <c r="B62" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B62" s="4"/>
-      <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="4"/>
+      <c r="E62" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F62" s="5"/>
-      <c r="G62" s="4"/>
-      <c r="H62" s="4"/>
-      <c r="I62" s="4"/>
+      <c r="G62" s="4">
+        <v>3</v>
+      </c>
+      <c r="H62" s="4">
+        <v>4</v>
+      </c>
+      <c r="I62" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3">
+        <v>61</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="C63" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E63" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B63" s="4"/>
-      <c r="C63" s="4"/>
-      <c r="D63" s="4"/>
-      <c r="E63" s="4"/>
       <c r="F63" s="5"/>
-      <c r="G63" s="4"/>
-      <c r="H63" s="4"/>
-      <c r="I63" s="4"/>
+      <c r="G63" s="4">
+        <v>3</v>
+      </c>
+      <c r="H63" s="4">
+        <v>3</v>
+      </c>
+      <c r="I63" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3">
-        <v>72</v>
-      </c>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
+        <v>62</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F64" s="5"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
+      <c r="G64" s="4">
+        <v>1</v>
+      </c>
+      <c r="H64" s="4">
+        <v>1</v>
+      </c>
+      <c r="I64" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3">
-        <v>73</v>
-      </c>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D65" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E65" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F65" s="5"/>
-      <c r="G65" s="4"/>
-      <c r="H65" s="4"/>
-      <c r="I65" s="4"/>
+      <c r="G65" s="4">
+        <v>3</v>
+      </c>
+      <c r="H65" s="4">
+        <v>3</v>
+      </c>
+      <c r="I65" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3">
-        <v>74</v>
-      </c>
-      <c r="B66" s="4"/>
-      <c r="C66" s="4"/>
-      <c r="D66" s="4"/>
-      <c r="E66" s="4"/>
+        <v>64</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F66" s="5"/>
-      <c r="G66" s="4"/>
-      <c r="H66" s="4"/>
-      <c r="I66" s="4"/>
+      <c r="G66" s="4">
+        <v>1</v>
+      </c>
+      <c r="H66" s="4">
+        <v>1</v>
+      </c>
+      <c r="I66" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3">
-        <v>75</v>
-      </c>
-      <c r="B67" s="4"/>
-      <c r="C67" s="4"/>
-      <c r="D67" s="4"/>
-      <c r="E67" s="4"/>
+        <v>65</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E67" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F67" s="5"/>
-      <c r="G67" s="4"/>
-      <c r="H67" s="4"/>
-      <c r="I67" s="4"/>
+      <c r="G67" s="4">
+        <v>7</v>
+      </c>
+      <c r="H67" s="4">
+        <v>7</v>
+      </c>
+      <c r="I67" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="3">
-        <v>76</v>
-      </c>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="4"/>
+        <v>66</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="E68" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F68" s="5"/>
-      <c r="G68" s="4"/>
-      <c r="H68" s="4"/>
-      <c r="I68" s="4"/>
+      <c r="G68" s="4">
+        <v>2</v>
+      </c>
+      <c r="H68" s="4">
+        <v>3</v>
+      </c>
+      <c r="I68" s="4">
+        <v>100</v>
+      </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="3">
-        <v>77</v>
-      </c>
-      <c r="B69" s="4"/>
-      <c r="C69" s="4"/>
-      <c r="D69" s="4"/>
-      <c r="E69" s="4"/>
+        <v>67</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E69" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="F69" s="5"/>
-      <c r="G69" s="4"/>
-      <c r="H69" s="4"/>
-      <c r="I69" s="4"/>
+      <c r="G69" s="4">
+        <v>12</v>
+      </c>
+      <c r="H69" s="4">
+        <v>9</v>
+      </c>
+      <c r="I69" s="4">
+        <v>70</v>
+      </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3">
-        <v>78</v>
+        <v>68</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="4"/>
@@ -2544,7 +2961,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="4"/>
@@ -2557,7 +2974,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3">
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="4"/>
@@ -2570,7 +2987,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="3">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="4"/>
@@ -2583,7 +3000,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="3">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="4"/>
@@ -2596,7 +3013,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" s="3">
-        <v>83</v>
+        <v>73</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="4"/>
@@ -2609,7 +3026,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="3">
-        <v>84</v>
+        <v>74</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="4"/>
@@ -2622,7 +3039,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="3">
-        <v>85</v>
+        <v>75</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="4"/>
@@ -2635,7 +3052,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="3">
-        <v>86</v>
+        <v>76</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
@@ -2648,7 +3065,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="3">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="4"/>
@@ -2661,7 +3078,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" s="3">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="4"/>
@@ -2674,7 +3091,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="3">
-        <v>89</v>
+        <v>79</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
@@ -2687,7 +3104,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" s="3">
-        <v>90</v>
+        <v>80</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="4"/>
@@ -2700,7 +3117,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="3">
-        <v>91</v>
+        <v>81</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
@@ -2713,7 +3130,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="3">
-        <v>92</v>
+        <v>82</v>
       </c>
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
@@ -2726,7 +3143,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="3">
-        <v>93</v>
+        <v>83</v>
       </c>
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
@@ -2739,7 +3156,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="3">
-        <v>94</v>
+        <v>84</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="4"/>
@@ -2752,7 +3169,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="3">
-        <v>95</v>
+        <v>85</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="4"/>
@@ -2765,7 +3182,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88" s="3">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="4"/>
@@ -2778,7 +3195,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" s="3">
-        <v>97</v>
+        <v>87</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
@@ -2791,7 +3208,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" s="3">
-        <v>98</v>
+        <v>88</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
@@ -2804,7 +3221,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91" s="3">
-        <v>99</v>
+        <v>89</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
@@ -2817,7 +3234,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" s="3">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
@@ -2830,7 +3247,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" s="3">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
@@ -2843,7 +3260,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" s="3">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
@@ -2856,7 +3273,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" s="3">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
@@ -2869,7 +3286,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" s="3">
-        <v>104</v>
+        <v>94</v>
       </c>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
@@ -2882,7 +3299,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" s="3">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
@@ -2895,7 +3312,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" s="3">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
@@ -2908,7 +3325,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" s="3">
-        <v>107</v>
+        <v>97</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
@@ -2921,7 +3338,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="3">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
@@ -2934,7 +3351,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="3">
-        <v>109</v>
+        <v>99</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
@@ -2947,7 +3364,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="3">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
@@ -2960,7 +3377,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" s="3">
-        <v>111</v>
+        <v>101</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
@@ -2973,7 +3390,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" s="3">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
@@ -2986,7 +3403,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" s="3">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
@@ -2999,7 +3416,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106" s="3">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
@@ -3012,7 +3429,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" s="3">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
@@ -3025,7 +3442,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" s="3">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
@@ -3038,7 +3455,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" s="3">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
@@ -3051,7 +3468,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" s="3">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
@@ -3064,7 +3481,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" s="3">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
@@ -3077,7 +3494,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" s="3">
-        <v>120</v>
+        <v>110</v>
       </c>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
@@ -3090,7 +3507,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" s="3">
-        <v>121</v>
+        <v>111</v>
       </c>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
@@ -3103,7 +3520,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" s="3">
-        <v>122</v>
+        <v>112</v>
       </c>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
@@ -3116,7 +3533,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" s="3">
-        <v>123</v>
+        <v>113</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
@@ -3129,7 +3546,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" s="3">
-        <v>124</v>
+        <v>114</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
@@ -3142,7 +3559,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" s="3">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
@@ -3155,7 +3572,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" s="3">
-        <v>126</v>
+        <v>116</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
@@ -3168,7 +3585,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119" s="3">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
@@ -3181,7 +3598,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" s="3">
-        <v>128</v>
+        <v>118</v>
       </c>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
@@ -3194,7 +3611,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" s="3">
-        <v>129</v>
+        <v>119</v>
       </c>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
@@ -3207,7 +3624,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" s="3">
-        <v>130</v>
+        <v>120</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
@@ -3220,7 +3637,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" s="3">
-        <v>131</v>
+        <v>121</v>
       </c>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
@@ -3233,7 +3650,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" s="3">
-        <v>132</v>
+        <v>122</v>
       </c>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
@@ -3246,7 +3663,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" s="3">
-        <v>133</v>
+        <v>123</v>
       </c>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
@@ -3259,7 +3676,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" s="3">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
@@ -3272,7 +3689,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" s="3">
-        <v>135</v>
+        <v>125</v>
       </c>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
@@ -3285,7 +3702,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" s="3">
-        <v>136</v>
+        <v>126</v>
       </c>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
@@ -3298,7 +3715,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" s="3">
-        <v>137</v>
+        <v>127</v>
       </c>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
@@ -3311,7 +3728,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" s="3">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
@@ -3324,7 +3741,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131" s="3">
-        <v>139</v>
+        <v>129</v>
       </c>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
@@ -3337,7 +3754,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" s="3">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
@@ -3350,7 +3767,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" s="3">
-        <v>141</v>
+        <v>131</v>
       </c>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
@@ -3363,7 +3780,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" s="3">
-        <v>142</v>
+        <v>132</v>
       </c>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
@@ -3376,7 +3793,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" s="3">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
@@ -3389,7 +3806,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" s="3">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
@@ -3402,7 +3819,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" s="3">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
@@ -3415,7 +3832,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" s="3">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
@@ -3428,7 +3845,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" s="3">
-        <v>147</v>
+        <v>137</v>
       </c>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
@@ -3441,7 +3858,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" s="3">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
@@ -3454,7 +3871,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" s="3">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
@@ -3467,7 +3884,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" s="3">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
@@ -3480,7 +3897,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" s="3">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
@@ -3493,7 +3910,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" s="3">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
@@ -3506,7 +3923,7 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145" s="3">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
@@ -3519,7 +3936,7 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" s="3">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
@@ -3532,7 +3949,7 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" s="3">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
@@ -3545,7 +3962,7 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" s="3">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
@@ -3558,7 +3975,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" s="3">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
@@ -3571,7 +3988,7 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" s="3">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
@@ -3584,7 +4001,7 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" s="3">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
@@ -3597,7 +4014,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" s="3">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
@@ -3610,7 +4027,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" s="3">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
@@ -3623,7 +4040,7 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" s="3">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
@@ -3636,7 +4053,7 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155" s="3">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
@@ -3649,7 +4066,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156" s="3">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
@@ -3662,7 +4079,7 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" s="3">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
@@ -3675,7 +4092,7 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" s="3">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
@@ -3688,7 +4105,7 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159" s="3">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
@@ -3701,7 +4118,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160" s="3">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
@@ -3714,7 +4131,7 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" s="3">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
@@ -3727,7 +4144,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" s="3">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
@@ -3740,7 +4157,7 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" s="3">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
@@ -3753,7 +4170,7 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" s="3">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
@@ -3766,7 +4183,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165" s="3">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
@@ -3779,7 +4196,7 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" s="3">
-        <v>174</v>
+        <v>164</v>
       </c>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
@@ -3792,7 +4209,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" s="3">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
@@ -3805,7 +4222,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" s="3">
-        <v>176</v>
+        <v>166</v>
       </c>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
@@ -3818,7 +4235,7 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" s="3">
-        <v>177</v>
+        <v>167</v>
       </c>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
@@ -3831,7 +4248,7 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" s="3">
-        <v>178</v>
+        <v>168</v>
       </c>
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
@@ -3844,7 +4261,7 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171" s="3">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
@@ -3857,7 +4274,7 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" s="3">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
@@ -3870,7 +4287,7 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" s="3">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
@@ -3883,7 +4300,7 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" s="3">
-        <v>182</v>
+        <v>172</v>
       </c>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
@@ -3896,7 +4313,7 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" s="3">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
@@ -3909,7 +4326,7 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" s="3">
-        <v>184</v>
+        <v>174</v>
       </c>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
@@ -3922,7 +4339,7 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" s="3">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
@@ -3935,7 +4352,7 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" s="3">
-        <v>186</v>
+        <v>176</v>
       </c>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
@@ -3948,7 +4365,7 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" s="3">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
@@ -3961,7 +4378,7 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" s="3">
-        <v>188</v>
+        <v>178</v>
       </c>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
@@ -3974,7 +4391,7 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" s="3">
-        <v>189</v>
+        <v>179</v>
       </c>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
@@ -3987,7 +4404,7 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" s="3">
-        <v>190</v>
+        <v>180</v>
       </c>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
@@ -4000,7 +4417,7 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" s="3">
-        <v>191</v>
+        <v>181</v>
       </c>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
@@ -4013,7 +4430,7 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" s="3">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
@@ -4026,7 +4443,7 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" s="3">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
@@ -4039,7 +4456,7 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" s="3">
-        <v>194</v>
+        <v>184</v>
       </c>
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
@@ -4052,7 +4469,7 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" s="3">
-        <v>195</v>
+        <v>185</v>
       </c>
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
@@ -4065,7 +4482,7 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" s="3">
-        <v>196</v>
+        <v>186</v>
       </c>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
@@ -4078,7 +4495,7 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" s="3">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
@@ -4091,7 +4508,7 @@
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" s="3">
-        <v>198</v>
+        <v>188</v>
       </c>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
@@ -4104,7 +4521,7 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191" s="3">
-        <v>199</v>
+        <v>189</v>
       </c>
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
@@ -4117,7 +4534,7 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" s="3">
-        <v>200</v>
+        <v>190</v>
       </c>
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
@@ -4130,7 +4547,7 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" s="3">
-        <v>201</v>
+        <v>191</v>
       </c>
       <c r="B193" s="4"/>
       <c r="C193" s="4"/>
@@ -4143,7 +4560,7 @@
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" s="3">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="B194" s="4"/>
       <c r="C194" s="4"/>
@@ -4156,20 +4573,20 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195" s="3">
-        <v>203</v>
+        <v>193</v>
       </c>
       <c r="B195" s="4"/>
       <c r="C195" s="4"/>
       <c r="D195" s="4"/>
       <c r="E195" s="4"/>
-      <c r="F195" s="4"/>
+      <c r="F195" s="5"/>
       <c r="G195" s="4"/>
       <c r="H195" s="4"/>
       <c r="I195" s="4"/>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196" s="3">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="B196" s="4"/>
       <c r="C196" s="4"/>
@@ -4182,7 +4599,7 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197" s="3">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="B197" s="4"/>
       <c r="C197" s="4"/>
@@ -4195,7 +4612,7 @@
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198" s="3">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="B198" s="4"/>
       <c r="C198" s="4"/>
@@ -4208,7 +4625,7 @@
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199" s="3">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B199" s="4"/>
       <c r="C199" s="4"/>
@@ -4220,7 +4637,9 @@
       <c r="I199" s="4"/>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A200" s="4"/>
+      <c r="A200" s="3">
+        <v>198</v>
+      </c>
       <c r="B200" s="4"/>
       <c r="C200" s="4"/>
       <c r="D200" s="4"/>
@@ -4231,7 +4650,9 @@
       <c r="I200" s="4"/>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A201" s="4"/>
+      <c r="A201" s="3">
+        <v>199</v>
+      </c>
       <c r="B201" s="4"/>
       <c r="C201" s="4"/>
       <c r="D201" s="4"/>
@@ -4242,7 +4663,9 @@
       <c r="I201" s="4"/>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A202" s="4"/>
+      <c r="A202" s="3">
+        <v>200</v>
+      </c>
       <c r="B202" s="4"/>
       <c r="C202" s="4"/>
       <c r="D202" s="4"/>
@@ -4253,7 +4676,9 @@
       <c r="I202" s="4"/>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A203" s="4"/>
+      <c r="A203" s="3">
+        <v>201</v>
+      </c>
       <c r="B203" s="4"/>
       <c r="C203" s="4"/>
       <c r="D203" s="4"/>
@@ -4264,7 +4689,9 @@
       <c r="I203" s="4"/>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A204" s="4"/>
+      <c r="A204" s="3">
+        <v>202</v>
+      </c>
       <c r="B204" s="4"/>
       <c r="C204" s="4"/>
       <c r="D204" s="4"/>
@@ -4275,7 +4702,9 @@
       <c r="I204" s="4"/>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A205" s="4"/>
+      <c r="A205" s="3">
+        <v>203</v>
+      </c>
       <c r="B205" s="4"/>
       <c r="C205" s="4"/>
       <c r="D205" s="4"/>
@@ -4285,27 +4714,38 @@
       <c r="H205" s="4"/>
       <c r="I205" s="4"/>
     </row>
+    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A206" s="4"/>
+      <c r="B206" s="4"/>
+      <c r="C206" s="4"/>
+      <c r="D206" s="4"/>
+      <c r="E206" s="4"/>
+      <c r="F206" s="4"/>
+      <c r="G206" s="4"/>
+      <c r="H206" s="4"/>
+      <c r="I206" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A2:I199"/>
+  <autoFilter ref="A2:I200"/>
   <dataConsolidate/>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
   </mergeCells>
   <conditionalFormatting sqref="C1:C28 C47:C1048576">
-    <cfRule type="cellIs" dxfId="31" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="20" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="21" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="22" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="23" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I28 I47:I199">
+  <conditionalFormatting sqref="I3:I28 I47:I200">
     <cfRule type="colorScale" priority="91">
       <colorScale>
         <cfvo type="min"/>
@@ -4318,44 +4758,44 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
-    <cfRule type="cellIs" dxfId="23" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="10" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="12" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="13" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C29:C35">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4384,18 +4824,19 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E199">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E200">
       <formula1>"Tan Tran, Nhung Huyng, Tuong Nguyen, Nguyen Dinh, Quyet Nguyen, Dang Nguyen, Tung Nguyen, Loc Phan"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C199">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C200">
       <formula1>"Very High,High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D198">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D199">
       <formula1>"RE, Architecture, Detail Design, Implementation, Testing, Management"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Loc update measure about effort
</commit_message>
<xml_diff>
--- a/Project Plan/Mesurement.xlsx
+++ b/Project Plan/Mesurement.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="18195" windowHeight="8445"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="18192" windowHeight="8448"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,9 +12,9 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$200</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$2:$I$193</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="354" uniqueCount="111">
   <si>
     <t>No.</t>
   </si>
@@ -250,18 +250,9 @@
     <t>Doc risk management plan and create template</t>
   </si>
   <si>
-    <t>13/10/2011</t>
-  </si>
-  <si>
     <t>Add new Risk category</t>
   </si>
   <si>
-    <t>19/12/2011</t>
-  </si>
-  <si>
-    <t>13/1/2012</t>
-  </si>
-  <si>
     <t>Define Detail Design process</t>
   </si>
   <si>
@@ -335,12 +326,76 @@
   </si>
   <si>
     <t>Plan Detail Design</t>
+  </si>
+  <si>
+    <t>Write document content for meeting with customer</t>
+  </si>
+  <si>
+    <t>List questions for meeting with customer</t>
+  </si>
+  <si>
+    <t>Research about Design Process</t>
+  </si>
+  <si>
+    <t>List questions and answer for meeting 
+with customer</t>
+  </si>
+  <si>
+    <t>Document list questions and answer</t>
+  </si>
+  <si>
+    <t>Write introduction for ConceptOperation</t>
+  </si>
+  <si>
+    <t>Update part 6 for ConceptOperation</t>
+  </si>
+  <si>
+    <t>Update part 3 for ConceptOperation</t>
+  </si>
+  <si>
+    <t>Group catalog (from customer requirement)</t>
+  </si>
+  <si>
+    <t>List informations to manage and group its.</t>
+  </si>
+  <si>
+    <t>Document SRS part 2.5; 2.6; 2.7</t>
+  </si>
+  <si>
+    <t>Draw context Diagram and descript context</t>
+  </si>
+  <si>
+    <t>Update Funtional Requirement and Business Rule</t>
+  </si>
+  <si>
+    <t>Descript Use-case</t>
+  </si>
+  <si>
+    <t>Update 2.3, 2.4, 2.6 , 2.7, 5 SRS and Functionlist.</t>
+  </si>
+  <si>
+    <t>Update All use-case</t>
+  </si>
+  <si>
+    <t>Update Risk Register</t>
+  </si>
+  <si>
+    <t>Draw activities diagram</t>
+  </si>
+  <si>
+    <t>Update activities diagram</t>
+  </si>
+  <si>
+    <t>Loc Phan</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -489,7 +544,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -499,15 +554,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -515,88 +566,22 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="24">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="16">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1042,41 +1027,41 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I206"/>
+  <dimension ref="A1:I199"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F66" sqref="F66"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F48" sqref="F48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.88671875" style="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5546875" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="9.140625" style="2"/>
+    <col min="9" max="9" width="17.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -1092,7 +1077,7 @@
       <c r="E2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="14" t="s">
         <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
@@ -1105,11 +1090,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
         <v>1</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -1121,24 +1106,24 @@
       <c r="E3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="15">
         <v>40734</v>
       </c>
       <c r="G3" s="3">
         <v>8</v>
       </c>
-      <c r="H3" s="6">
+      <c r="H3" s="5">
         <v>2</v>
       </c>
       <c r="I3" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
         <v>2</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -1150,22 +1135,22 @@
       <c r="E4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="15"/>
       <c r="G4" s="3">
         <v>3</v>
       </c>
-      <c r="H4" s="6">
+      <c r="H4" s="5">
         <v>2.5</v>
       </c>
       <c r="I4" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
         <v>3</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="6" t="s">
         <v>12</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -1177,22 +1162,22 @@
       <c r="E5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="5"/>
+      <c r="F5" s="15"/>
       <c r="G5" s="3">
         <v>3</v>
       </c>
-      <c r="H5" s="6">
+      <c r="H5" s="5">
         <v>1.5</v>
       </c>
       <c r="I5" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
         <v>4</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="6" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1204,22 +1189,22 @@
       <c r="E6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="5"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="3">
         <v>16</v>
       </c>
-      <c r="H6" s="6">
+      <c r="H6" s="5">
         <v>24</v>
       </c>
       <c r="I6" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
         <v>5</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="6" t="s">
         <v>23</v>
       </c>
       <c r="C7" s="4" t="s">
@@ -1231,22 +1216,22 @@
       <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="5"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="3">
         <v>3</v>
       </c>
-      <c r="H7" s="6">
+      <c r="H7" s="5">
         <v>4.5</v>
       </c>
       <c r="I7" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C8" s="4" t="s">
@@ -1258,22 +1243,22 @@
       <c r="E8" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="5"/>
+      <c r="F8" s="15"/>
       <c r="G8" s="3">
         <v>70</v>
       </c>
-      <c r="H8" s="6">
+      <c r="H8" s="5">
         <v>45.5</v>
       </c>
       <c r="I8" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A9" s="3">
         <v>7</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="6" t="s">
         <v>13</v>
       </c>
       <c r="C9" s="4" t="s">
@@ -1285,22 +1270,22 @@
       <c r="E9" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="5"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="3">
         <v>6</v>
       </c>
-      <c r="H9" s="6">
+      <c r="H9" s="5">
         <v>2</v>
       </c>
       <c r="I9" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="3">
         <v>8</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="4" t="s">
@@ -1312,22 +1297,22 @@
       <c r="E10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F10" s="5"/>
+      <c r="F10" s="15"/>
       <c r="G10" s="3">
         <v>15</v>
       </c>
-      <c r="H10" s="6">
+      <c r="H10" s="5">
         <v>6.5</v>
       </c>
       <c r="I10" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -1339,22 +1324,22 @@
       <c r="E11" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F11" s="5"/>
+      <c r="F11" s="15"/>
       <c r="G11" s="3">
         <v>20</v>
       </c>
-      <c r="H11" s="6">
+      <c r="H11" s="5">
         <v>14</v>
       </c>
       <c r="I11" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="3">
         <v>10</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B12" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -1366,22 +1351,22 @@
       <c r="E12" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F12" s="5"/>
+      <c r="F12" s="15"/>
       <c r="G12" s="3">
         <v>5</v>
       </c>
-      <c r="H12" s="6">
+      <c r="H12" s="5">
         <v>3</v>
       </c>
       <c r="I12" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="3">
         <v>11</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1393,22 +1378,22 @@
       <c r="E13" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F13" s="5"/>
+      <c r="F13" s="15"/>
       <c r="G13" s="3">
         <v>35</v>
       </c>
-      <c r="H13" s="6">
+      <c r="H13" s="5">
         <v>8</v>
       </c>
       <c r="I13" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="3">
         <v>12</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="7" t="s">
         <v>26</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -1420,22 +1405,22 @@
       <c r="E14" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F14" s="5"/>
+      <c r="F14" s="15"/>
       <c r="G14" s="3">
         <v>35</v>
       </c>
-      <c r="H14" s="6">
+      <c r="H14" s="5">
         <v>11</v>
       </c>
       <c r="I14" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3">
         <v>13</v>
       </c>
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C15" s="4" t="s">
@@ -1447,22 +1432,22 @@
       <c r="E15" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F15" s="5"/>
+      <c r="F15" s="15"/>
       <c r="G15" s="3">
         <v>35</v>
       </c>
-      <c r="H15" s="6">
+      <c r="H15" s="5">
         <v>1.5</v>
       </c>
       <c r="I15" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="3">
         <v>14</v>
       </c>
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="6" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="4" t="s">
@@ -1474,22 +1459,22 @@
       <c r="E16" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F16" s="5"/>
+      <c r="F16" s="15"/>
       <c r="G16" s="3">
         <v>6</v>
       </c>
-      <c r="H16" s="6">
+      <c r="H16" s="5">
         <v>6.5</v>
       </c>
       <c r="I16" s="4">
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="3">
         <v>15</v>
       </c>
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -1501,18 +1486,18 @@
       <c r="E17" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F17" s="5"/>
+      <c r="F17" s="15"/>
       <c r="G17" s="3">
         <v>42</v>
       </c>
-      <c r="H17" s="6">
+      <c r="H17" s="5">
         <v>5</v>
       </c>
       <c r="I17" s="4">
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="3">
         <v>16</v>
       </c>
@@ -1528,7 +1513,7 @@
       <c r="E18" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F18" s="5"/>
+      <c r="F18" s="15"/>
       <c r="G18" s="3">
         <v>5</v>
       </c>
@@ -1539,7 +1524,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="3">
         <v>17</v>
       </c>
@@ -1555,7 +1540,7 @@
       <c r="E19" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F19" s="5"/>
+      <c r="F19" s="15"/>
       <c r="G19" s="3">
         <v>8</v>
       </c>
@@ -1566,7 +1551,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>18</v>
       </c>
@@ -1582,7 +1567,7 @@
       <c r="E20" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F20" s="5"/>
+      <c r="F20" s="15"/>
       <c r="G20" s="3">
         <v>1</v>
       </c>
@@ -1593,7 +1578,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="3">
         <v>19</v>
       </c>
@@ -1609,7 +1594,7 @@
       <c r="E21" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F21" s="5"/>
+      <c r="F21" s="15"/>
       <c r="G21" s="3">
         <v>7</v>
       </c>
@@ -1620,7 +1605,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="3">
         <v>20</v>
       </c>
@@ -1636,7 +1621,7 @@
       <c r="E22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="15">
         <v>40613</v>
       </c>
       <c r="G22" s="3">
@@ -1649,7 +1634,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="3">
         <v>21</v>
       </c>
@@ -1665,7 +1650,7 @@
       <c r="E23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F23" s="5"/>
+      <c r="F23" s="15"/>
       <c r="G23" s="3">
         <v>4</v>
       </c>
@@ -1676,7 +1661,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="3">
         <v>22</v>
       </c>
@@ -1692,7 +1677,7 @@
       <c r="E24" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F24" s="5"/>
+      <c r="F24" s="15"/>
       <c r="G24" s="3">
         <v>6</v>
       </c>
@@ -1703,7 +1688,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="3">
         <v>23</v>
       </c>
@@ -1719,7 +1704,7 @@
       <c r="E25" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F25" s="5"/>
+      <c r="F25" s="15"/>
       <c r="G25" s="3">
         <v>6</v>
       </c>
@@ -1730,7 +1715,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>24</v>
       </c>
@@ -1746,7 +1731,7 @@
       <c r="E26" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="15">
         <v>40798</v>
       </c>
       <c r="G26" s="3">
@@ -1759,7 +1744,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="3">
         <v>25</v>
       </c>
@@ -1775,7 +1760,7 @@
       <c r="E27" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F27" s="5"/>
+      <c r="F27" s="15"/>
       <c r="G27" s="3">
         <v>5</v>
       </c>
@@ -1786,7 +1771,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="3">
         <v>26</v>
       </c>
@@ -1802,7 +1787,7 @@
       <c r="E28" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="F28" s="5"/>
+      <c r="F28" s="15"/>
       <c r="G28" s="3">
         <v>4</v>
       </c>
@@ -1813,7 +1798,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="3">
         <v>27</v>
       </c>
@@ -1829,7 +1814,7 @@
       <c r="E29" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F29" s="5"/>
+      <c r="F29" s="15"/>
       <c r="G29" s="3">
         <v>35</v>
       </c>
@@ -1840,7 +1825,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
         <v>28</v>
       </c>
@@ -1856,7 +1841,7 @@
       <c r="E30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F30" s="5"/>
+      <c r="F30" s="15"/>
       <c r="G30" s="3">
         <v>6</v>
       </c>
@@ -1867,7 +1852,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="3">
         <v>29</v>
       </c>
@@ -1883,7 +1868,7 @@
       <c r="E31" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F31" s="5"/>
+      <c r="F31" s="15"/>
       <c r="G31" s="3">
         <v>42</v>
       </c>
@@ -1894,7 +1879,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="3">
         <v>30</v>
       </c>
@@ -1910,7 +1895,7 @@
       <c r="E32" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F32" s="5"/>
+      <c r="F32" s="15"/>
       <c r="G32" s="3">
         <v>5</v>
       </c>
@@ -1921,7 +1906,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
         <v>31</v>
       </c>
@@ -1937,7 +1922,7 @@
       <c r="E33" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F33" s="5"/>
+      <c r="F33" s="15"/>
       <c r="G33" s="3">
         <v>8</v>
       </c>
@@ -1948,7 +1933,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="3">
         <v>32</v>
       </c>
@@ -1964,8 +1949,8 @@
       <c r="E34" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F34" s="5">
-        <v>40857</v>
+      <c r="F34" s="15">
+        <v>40827</v>
       </c>
       <c r="G34" s="3">
         <v>7</v>
@@ -1977,7 +1962,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="3">
         <v>33</v>
       </c>
@@ -1993,8 +1978,8 @@
       <c r="E35" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F35" s="5" t="s">
-        <v>65</v>
+      <c r="F35" s="15">
+        <v>40829</v>
       </c>
       <c r="G35" s="3">
         <v>5</v>
@@ -2006,7 +1991,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>34</v>
       </c>
@@ -2022,7 +2007,7 @@
       <c r="E36" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="15">
         <v>40889</v>
       </c>
       <c r="G36" s="3">
@@ -2035,7 +2020,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>35</v>
       </c>
@@ -2051,8 +2036,8 @@
       <c r="E37" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F37" s="5">
-        <v>40735</v>
+      <c r="F37" s="15">
+        <v>40854</v>
       </c>
       <c r="G37" s="3">
         <v>15</v>
@@ -2064,7 +2049,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>36</v>
       </c>
@@ -2080,8 +2065,8 @@
       <c r="E38" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F38" s="5">
-        <v>40940</v>
+      <c r="F38" s="15">
+        <v>40910</v>
       </c>
       <c r="G38" s="3">
         <v>13</v>
@@ -2093,7 +2078,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>37</v>
       </c>
@@ -2109,8 +2094,8 @@
       <c r="E39" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F39" s="5">
-        <v>40859</v>
+      <c r="F39" s="15">
+        <v>40888</v>
       </c>
       <c r="G39" s="3">
         <v>11</v>
@@ -2122,7 +2107,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>38</v>
       </c>
@@ -2138,7 +2123,7 @@
       <c r="E40" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F40" s="5">
+      <c r="F40" s="15">
         <v>40889</v>
       </c>
       <c r="G40" s="3">
@@ -2151,7 +2136,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>39</v>
       </c>
@@ -2167,7 +2152,7 @@
       <c r="E41" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F41" s="5">
+      <c r="F41" s="15">
         <v>40889</v>
       </c>
       <c r="G41" s="3">
@@ -2180,12 +2165,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>40</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>20</v>
@@ -2196,8 +2181,8 @@
       <c r="E42" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>67</v>
+      <c r="F42" s="15">
+        <v>40896</v>
       </c>
       <c r="G42" s="3">
         <v>1</v>
@@ -2209,7 +2194,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>41</v>
       </c>
@@ -2225,8 +2210,8 @@
       <c r="E43" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F43" s="5">
-        <v>40859</v>
+      <c r="F43" s="15">
+        <v>40888</v>
       </c>
       <c r="G43" s="3">
         <v>5</v>
@@ -2238,7 +2223,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>42</v>
       </c>
@@ -2254,8 +2239,8 @@
       <c r="E44" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F44" s="5" t="s">
-        <v>68</v>
+      <c r="F44" s="15">
+        <v>40921</v>
       </c>
       <c r="G44" s="3">
         <v>4</v>
@@ -2267,7 +2252,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>43</v>
       </c>
@@ -2283,8 +2268,8 @@
       <c r="E45" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F45" s="5" t="s">
-        <v>68</v>
+      <c r="F45" s="15">
+        <v>40921</v>
       </c>
       <c r="G45" s="3">
         <v>4</v>
@@ -2296,7 +2281,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>44</v>
       </c>
@@ -2312,8 +2297,8 @@
       <c r="E46" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="F46" s="5" t="s">
-        <v>68</v>
+      <c r="F46" s="15">
+        <v>40921</v>
       </c>
       <c r="G46" s="3">
         <v>4</v>
@@ -2325,23 +2310,23 @@
         <v>100</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>45</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F47" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F47" s="15"/>
       <c r="G47" s="4">
         <v>2</v>
       </c>
@@ -2352,23 +2337,23 @@
         <v>100</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>46</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F48" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F48" s="15"/>
       <c r="G48" s="4">
         <v>0.5</v>
       </c>
@@ -2379,12 +2364,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>47</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
@@ -2393,9 +2378,9 @@
         <v>28</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F49" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F49" s="15"/>
       <c r="G49" s="4">
         <v>10</v>
       </c>
@@ -2406,23 +2391,23 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>48</v>
       </c>
-      <c r="B50" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="C50" s="12" t="s">
+      <c r="B50" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C50" s="10" t="s">
         <v>21</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>28</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F50" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F50" s="15"/>
       <c r="G50" s="4">
         <v>4</v>
       </c>
@@ -2433,23 +2418,23 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A51" s="10">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A51" s="8">
         <v>49</v>
       </c>
-      <c r="B51" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="C51" s="12" t="s">
+      <c r="B51" s="12" t="s">
+        <v>72</v>
+      </c>
+      <c r="C51" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D51" s="9" t="s">
         <v>28</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F51" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F51" s="15"/>
       <c r="G51" s="4">
         <v>3</v>
       </c>
@@ -2460,23 +2445,23 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>50</v>
       </c>
-      <c r="B52" s="13" t="s">
-        <v>76</v>
-      </c>
-      <c r="C52" s="13" t="s">
+      <c r="B52" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>21</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>32</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F52" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F52" s="15"/>
       <c r="G52" s="4">
         <v>2</v>
       </c>
@@ -2487,12 +2472,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>51</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>21</v>
@@ -2501,9 +2486,9 @@
         <v>29</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F53" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F53" s="15"/>
       <c r="G53" s="4">
         <v>1</v>
       </c>
@@ -2514,12 +2499,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>52</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>21</v>
@@ -2528,9 +2513,9 @@
         <v>28</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F54" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F54" s="15"/>
       <c r="G54" s="4">
         <v>6</v>
       </c>
@@ -2541,12 +2526,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>53</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>21</v>
@@ -2555,9 +2540,9 @@
         <v>28</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F55" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F55" s="15"/>
       <c r="G55" s="4">
         <v>7</v>
       </c>
@@ -2568,12 +2553,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>54</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>20</v>
@@ -2582,9 +2567,9 @@
         <v>28</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F56" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F56" s="15"/>
       <c r="G56" s="4">
         <v>1.5</v>
       </c>
@@ -2595,12 +2580,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>55</v>
       </c>
-      <c r="B57" s="14" t="s">
-        <v>81</v>
+      <c r="B57" s="13" t="s">
+        <v>78</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>20</v>
@@ -2609,9 +2594,9 @@
         <v>28</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F57" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F57" s="15"/>
       <c r="G57" s="4">
         <v>1</v>
       </c>
@@ -2622,12 +2607,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>56</v>
       </c>
-      <c r="B58" s="14" t="s">
-        <v>82</v>
+      <c r="B58" s="13" t="s">
+        <v>79</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>21</v>
@@ -2636,9 +2621,9 @@
         <v>28</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F58" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F58" s="15"/>
       <c r="G58" s="4">
         <v>6</v>
       </c>
@@ -2649,12 +2634,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>57</v>
       </c>
-      <c r="B59" s="15" t="s">
-        <v>83</v>
+      <c r="B59" s="6" t="s">
+        <v>80</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>21</v>
@@ -2663,9 +2648,9 @@
         <v>28</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F59" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F59" s="15"/>
       <c r="G59" s="4">
         <v>5</v>
       </c>
@@ -2676,12 +2661,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>58</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>21</v>
@@ -2690,9 +2675,9 @@
         <v>28</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F60" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F60" s="15"/>
       <c r="G60" s="4">
         <v>2</v>
       </c>
@@ -2703,12 +2688,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>59</v>
       </c>
-      <c r="B61" s="14" t="s">
-        <v>85</v>
+      <c r="B61" s="13" t="s">
+        <v>82</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>20</v>
@@ -2717,9 +2702,9 @@
         <v>28</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F61" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F61" s="15"/>
       <c r="G61" s="4">
         <v>3</v>
       </c>
@@ -2730,23 +2715,23 @@
         <v>100</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>60</v>
       </c>
-      <c r="B62" s="14" t="s">
-        <v>86</v>
+      <c r="B62" s="13" t="s">
+        <v>83</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>20</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F62" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F62" s="15"/>
       <c r="G62" s="4">
         <v>3</v>
       </c>
@@ -2757,12 +2742,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>61</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C63" s="4" t="s">
         <v>20</v>
@@ -2771,9 +2756,9 @@
         <v>30</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F63" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F63" s="15"/>
       <c r="G63" s="4">
         <v>3</v>
       </c>
@@ -2784,12 +2769,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>62</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>20</v>
@@ -2798,9 +2783,9 @@
         <v>28</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F64" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F64" s="15"/>
       <c r="G64" s="4">
         <v>1</v>
       </c>
@@ -2811,23 +2796,23 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>63</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F65" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F65" s="15"/>
       <c r="G65" s="4">
         <v>3</v>
       </c>
@@ -2838,23 +2823,23 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>64</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>38</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F66" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F66" s="15"/>
       <c r="G66" s="4">
         <v>1</v>
       </c>
@@ -2865,12 +2850,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>65</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>20</v>
@@ -2879,9 +2864,9 @@
         <v>30</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F67" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F67" s="15"/>
       <c r="G67" s="4">
         <v>7</v>
       </c>
@@ -2892,12 +2877,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>20</v>
@@ -2906,9 +2891,9 @@
         <v>32</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F68" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F68" s="15"/>
       <c r="G68" s="4">
         <v>2</v>
       </c>
@@ -2919,12 +2904,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>67</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>9</v>
@@ -2933,9 +2918,9 @@
         <v>30</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="F69" s="5"/>
+        <v>68</v>
+      </c>
+      <c r="F69" s="15"/>
       <c r="G69" s="4">
         <v>12</v>
       </c>
@@ -2946,1787 +2931,1962 @@
         <v>70</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
-        <v>68</v>
-      </c>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="4"/>
-      <c r="F70" s="5"/>
+        <v>69</v>
+      </c>
+      <c r="B70" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E70" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F70" s="15">
+        <v>40816</v>
+      </c>
       <c r="G70" s="4"/>
-      <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H70" s="4">
+        <v>3</v>
+      </c>
+      <c r="I70" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
-        <v>69</v>
-      </c>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="5"/>
+        <v>70</v>
+      </c>
+      <c r="B71" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="C71" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E71" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F71" s="15">
+        <v>40816</v>
+      </c>
       <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H71" s="4">
+        <v>4</v>
+      </c>
+      <c r="I71" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="3">
-        <v>70</v>
-      </c>
-      <c r="B72" s="4"/>
-      <c r="C72" s="4"/>
-      <c r="D72" s="4"/>
-      <c r="E72" s="4"/>
-      <c r="F72" s="5"/>
+        <v>74</v>
+      </c>
+      <c r="B72" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="C72" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E72" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F72" s="15">
+        <v>40821</v>
+      </c>
       <c r="G72" s="4"/>
-      <c r="H72" s="4"/>
-      <c r="I72" s="4"/>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H72" s="4">
+        <v>5</v>
+      </c>
+      <c r="I72" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="3">
-        <v>71</v>
-      </c>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="4"/>
-      <c r="F73" s="5"/>
+        <v>75</v>
+      </c>
+      <c r="B73" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="C73" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D73" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E73" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F73" s="15">
+        <v>40821</v>
+      </c>
       <c r="G73" s="4"/>
-      <c r="H73" s="4"/>
-      <c r="I73" s="4"/>
-    </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H73" s="4">
+        <v>2</v>
+      </c>
+      <c r="I73" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="3">
-        <v>72</v>
-      </c>
-      <c r="B74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-      <c r="E74" s="4"/>
-      <c r="F74" s="5"/>
+        <v>77</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D74" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E74" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F74" s="15">
+        <v>40822</v>
+      </c>
       <c r="G74" s="4"/>
-      <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
-    </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H74" s="4">
+        <v>4</v>
+      </c>
+      <c r="I74" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="3">
-        <v>73</v>
-      </c>
-      <c r="B75" s="4"/>
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="5"/>
+        <v>78</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E75" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F75" s="15">
+        <v>40823</v>
+      </c>
       <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
-    </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H75" s="4">
+        <v>2</v>
+      </c>
+      <c r="I75" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="3">
-        <v>74</v>
-      </c>
-      <c r="B76" s="4"/>
-      <c r="C76" s="4"/>
-      <c r="D76" s="4"/>
-      <c r="E76" s="4"/>
-      <c r="F76" s="5"/>
+        <v>79</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D76" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E76" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F76" s="15">
+        <v>40846</v>
+      </c>
       <c r="G76" s="4"/>
-      <c r="H76" s="4"/>
-      <c r="I76" s="4"/>
-    </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H76" s="4">
+        <v>3</v>
+      </c>
+      <c r="I76" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="3">
-        <v>75</v>
-      </c>
-      <c r="B77" s="4"/>
-      <c r="C77" s="4"/>
-      <c r="D77" s="4"/>
-      <c r="E77" s="4"/>
-      <c r="F77" s="5"/>
+        <v>80</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D77" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E77" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F77" s="15">
+        <v>40847</v>
+      </c>
       <c r="G77" s="4"/>
-      <c r="H77" s="4"/>
-      <c r="I77" s="4"/>
-    </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H77" s="4">
+        <v>2</v>
+      </c>
+      <c r="I77" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="3">
-        <v>76</v>
-      </c>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="5"/>
+        <v>81</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D78" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E78" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F78" s="15">
+        <v>40848</v>
+      </c>
       <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="4"/>
-    </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H78" s="4">
+        <v>2</v>
+      </c>
+      <c r="I78" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="3">
-        <v>77</v>
-      </c>
-      <c r="B79" s="4"/>
-      <c r="C79" s="4"/>
-      <c r="D79" s="4"/>
-      <c r="E79" s="4"/>
-      <c r="F79" s="5"/>
+        <v>82</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="C79" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D79" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E79" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F79" s="15">
+        <v>40851</v>
+      </c>
       <c r="G79" s="4"/>
-      <c r="H79" s="4"/>
-      <c r="I79" s="4"/>
-    </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H79" s="4">
+        <v>1.5</v>
+      </c>
+      <c r="I79" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="3">
-        <v>78</v>
-      </c>
-      <c r="B80" s="4"/>
-      <c r="C80" s="4"/>
-      <c r="D80" s="4"/>
-      <c r="E80" s="4"/>
-      <c r="F80" s="5"/>
+        <v>83</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D80" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E80" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F80" s="15">
+        <v>40854</v>
+      </c>
       <c r="G80" s="4"/>
-      <c r="H80" s="4"/>
-      <c r="I80" s="4"/>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H80" s="4">
+        <v>5</v>
+      </c>
+      <c r="I80" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="3">
-        <v>79</v>
-      </c>
-      <c r="B81" s="4"/>
-      <c r="C81" s="4"/>
-      <c r="D81" s="4"/>
-      <c r="E81" s="4"/>
-      <c r="F81" s="5"/>
+        <v>84</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>102</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D81" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E81" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F81" s="15">
+        <v>40855</v>
+      </c>
       <c r="G81" s="4"/>
-      <c r="H81" s="4"/>
-      <c r="I81" s="4"/>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H81" s="4">
+        <v>3</v>
+      </c>
+      <c r="I81" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="3">
-        <v>80</v>
-      </c>
-      <c r="B82" s="4"/>
-      <c r="C82" s="4"/>
-      <c r="D82" s="4"/>
-      <c r="E82" s="4"/>
-      <c r="F82" s="5"/>
+        <v>85</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F82" s="15">
+        <v>40862</v>
+      </c>
       <c r="G82" s="4"/>
-      <c r="H82" s="4"/>
-      <c r="I82" s="4"/>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H82" s="4">
+        <v>7</v>
+      </c>
+      <c r="I82" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="3">
-        <v>81</v>
-      </c>
-      <c r="B83" s="4"/>
-      <c r="C83" s="4"/>
-      <c r="D83" s="4"/>
-      <c r="E83" s="4"/>
-      <c r="F83" s="5"/>
+        <v>86</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E83" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F83" s="15">
+        <v>40871</v>
+      </c>
       <c r="G83" s="4"/>
-      <c r="H83" s="4"/>
-      <c r="I83" s="4"/>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H83" s="4">
+        <v>8</v>
+      </c>
+      <c r="I83" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="3">
-        <v>82</v>
-      </c>
-      <c r="B84" s="4"/>
-      <c r="C84" s="4"/>
-      <c r="D84" s="4"/>
-      <c r="E84" s="4"/>
-      <c r="F84" s="5"/>
+        <v>87</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F84" s="15">
+        <v>40882</v>
+      </c>
       <c r="G84" s="4"/>
-      <c r="H84" s="4"/>
-      <c r="I84" s="4"/>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H84" s="4">
+        <v>4</v>
+      </c>
+      <c r="I84" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="3">
-        <v>83</v>
-      </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="5"/>
+        <v>89</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C85" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D85" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E85" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F85" s="15">
+        <v>40888</v>
+      </c>
       <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H85" s="4">
+        <v>5</v>
+      </c>
+      <c r="I85" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="3">
-        <v>84</v>
-      </c>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
-      <c r="E86" s="4"/>
-      <c r="F86" s="5"/>
+        <v>91</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C86" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D86" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E86" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F86" s="15">
+        <v>40895</v>
+      </c>
       <c r="G86" s="4"/>
-      <c r="H86" s="4"/>
-      <c r="I86" s="4"/>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H86" s="4">
+        <v>3</v>
+      </c>
+      <c r="I86" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="3">
-        <v>85</v>
-      </c>
-      <c r="B87" s="4"/>
-      <c r="C87" s="4"/>
-      <c r="D87" s="4"/>
-      <c r="E87" s="4"/>
-      <c r="F87" s="5"/>
+        <v>92</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C87" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D87" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E87" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F87" s="15">
+        <v>40941</v>
+      </c>
       <c r="G87" s="4"/>
-      <c r="H87" s="4"/>
-      <c r="I87" s="4"/>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H87" s="4">
+        <v>6</v>
+      </c>
+      <c r="I87" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="3">
-        <v>86</v>
-      </c>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="4"/>
-      <c r="F88" s="5"/>
+        <v>93</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C88" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D88" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E88" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F88" s="15">
+        <v>41245</v>
+      </c>
       <c r="G88" s="4"/>
-      <c r="H88" s="4"/>
-      <c r="I88" s="4"/>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="H88" s="4">
+        <v>3</v>
+      </c>
+      <c r="I88" s="4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="3">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="4"/>
       <c r="D89" s="4"/>
       <c r="E89" s="4"/>
-      <c r="F89" s="5"/>
+      <c r="F89" s="15"/>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="3">
-        <v>88</v>
+        <v>95</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
       <c r="E90" s="4"/>
-      <c r="F90" s="5"/>
+      <c r="F90" s="15"/>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="3">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B91" s="4"/>
       <c r="C91" s="4"/>
       <c r="D91" s="4"/>
       <c r="E91" s="4"/>
-      <c r="F91" s="5"/>
+      <c r="F91" s="15"/>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="3">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="4"/>
       <c r="D92" s="4"/>
       <c r="E92" s="4"/>
-      <c r="F92" s="5"/>
+      <c r="F92" s="15"/>
       <c r="G92" s="4"/>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="3">
-        <v>91</v>
+        <v>98</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="4"/>
       <c r="D93" s="4"/>
       <c r="E93" s="4"/>
-      <c r="F93" s="5"/>
+      <c r="F93" s="15"/>
       <c r="G93" s="4"/>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="3">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
       <c r="E94" s="4"/>
-      <c r="F94" s="5"/>
+      <c r="F94" s="15"/>
       <c r="G94" s="4"/>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="3">
-        <v>93</v>
+        <v>100</v>
       </c>
       <c r="B95" s="4"/>
       <c r="C95" s="4"/>
       <c r="D95" s="4"/>
       <c r="E95" s="4"/>
-      <c r="F95" s="5"/>
+      <c r="F95" s="15"/>
       <c r="G95" s="4"/>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="3">
-        <v>94</v>
+        <v>101</v>
       </c>
       <c r="B96" s="4"/>
       <c r="C96" s="4"/>
       <c r="D96" s="4"/>
       <c r="E96" s="4"/>
-      <c r="F96" s="5"/>
+      <c r="F96" s="15"/>
       <c r="G96" s="4"/>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="3">
-        <v>95</v>
+        <v>102</v>
       </c>
       <c r="B97" s="4"/>
       <c r="C97" s="4"/>
       <c r="D97" s="4"/>
       <c r="E97" s="4"/>
-      <c r="F97" s="5"/>
+      <c r="F97" s="15"/>
       <c r="G97" s="4"/>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="3">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B98" s="4"/>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
       <c r="E98" s="4"/>
-      <c r="F98" s="5"/>
+      <c r="F98" s="15"/>
       <c r="G98" s="4"/>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="3">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B99" s="4"/>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
       <c r="E99" s="4"/>
-      <c r="F99" s="5"/>
+      <c r="F99" s="15"/>
       <c r="G99" s="4"/>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="3">
-        <v>98</v>
+        <v>105</v>
       </c>
       <c r="B100" s="4"/>
       <c r="C100" s="4"/>
       <c r="D100" s="4"/>
       <c r="E100" s="4"/>
-      <c r="F100" s="5"/>
+      <c r="F100" s="15"/>
       <c r="G100" s="4"/>
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="3">
-        <v>99</v>
+        <v>106</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="4"/>
       <c r="D101" s="4"/>
       <c r="E101" s="4"/>
-      <c r="F101" s="5"/>
+      <c r="F101" s="15"/>
       <c r="G101" s="4"/>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="3">
-        <v>100</v>
+        <v>107</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="4"/>
       <c r="D102" s="4"/>
       <c r="E102" s="4"/>
-      <c r="F102" s="5"/>
+      <c r="F102" s="15"/>
       <c r="G102" s="4"/>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="3">
-        <v>101</v>
+        <v>108</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="4"/>
       <c r="D103" s="4"/>
       <c r="E103" s="4"/>
-      <c r="F103" s="5"/>
+      <c r="F103" s="15"/>
       <c r="G103" s="4"/>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="3">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B104" s="4"/>
       <c r="C104" s="4"/>
       <c r="D104" s="4"/>
       <c r="E104" s="4"/>
-      <c r="F104" s="5"/>
+      <c r="F104" s="15"/>
       <c r="G104" s="4"/>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="3">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="B105" s="4"/>
       <c r="C105" s="4"/>
       <c r="D105" s="4"/>
       <c r="E105" s="4"/>
-      <c r="F105" s="5"/>
+      <c r="F105" s="15"/>
       <c r="G105" s="4"/>
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="3">
-        <v>104</v>
+        <v>111</v>
       </c>
       <c r="B106" s="4"/>
       <c r="C106" s="4"/>
       <c r="D106" s="4"/>
       <c r="E106" s="4"/>
-      <c r="F106" s="5"/>
+      <c r="F106" s="15"/>
       <c r="G106" s="4"/>
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="3">
-        <v>105</v>
+        <v>112</v>
       </c>
       <c r="B107" s="4"/>
       <c r="C107" s="4"/>
       <c r="D107" s="4"/>
       <c r="E107" s="4"/>
-      <c r="F107" s="5"/>
+      <c r="F107" s="15"/>
       <c r="G107" s="4"/>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="3">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="B108" s="4"/>
       <c r="C108" s="4"/>
       <c r="D108" s="4"/>
       <c r="E108" s="4"/>
-      <c r="F108" s="5"/>
+      <c r="F108" s="15"/>
       <c r="G108" s="4"/>
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="3">
-        <v>107</v>
+        <v>114</v>
       </c>
       <c r="B109" s="4"/>
       <c r="C109" s="4"/>
       <c r="D109" s="4"/>
       <c r="E109" s="4"/>
-      <c r="F109" s="5"/>
+      <c r="F109" s="15"/>
       <c r="G109" s="4"/>
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="3">
-        <v>108</v>
+        <v>115</v>
       </c>
       <c r="B110" s="4"/>
       <c r="C110" s="4"/>
       <c r="D110" s="4"/>
       <c r="E110" s="4"/>
-      <c r="F110" s="5"/>
+      <c r="F110" s="15"/>
       <c r="G110" s="4"/>
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="3">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="B111" s="4"/>
       <c r="C111" s="4"/>
       <c r="D111" s="4"/>
       <c r="E111" s="4"/>
-      <c r="F111" s="5"/>
+      <c r="F111" s="15"/>
       <c r="G111" s="4"/>
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="3">
-        <v>110</v>
+        <v>117</v>
       </c>
       <c r="B112" s="4"/>
       <c r="C112" s="4"/>
       <c r="D112" s="4"/>
       <c r="E112" s="4"/>
-      <c r="F112" s="5"/>
+      <c r="F112" s="15"/>
       <c r="G112" s="4"/>
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="3">
-        <v>111</v>
+        <v>118</v>
       </c>
       <c r="B113" s="4"/>
       <c r="C113" s="4"/>
       <c r="D113" s="4"/>
       <c r="E113" s="4"/>
-      <c r="F113" s="5"/>
+      <c r="F113" s="15"/>
       <c r="G113" s="4"/>
       <c r="H113" s="4"/>
       <c r="I113" s="4"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="3">
-        <v>112</v>
+        <v>119</v>
       </c>
       <c r="B114" s="4"/>
       <c r="C114" s="4"/>
       <c r="D114" s="4"/>
       <c r="E114" s="4"/>
-      <c r="F114" s="5"/>
+      <c r="F114" s="15"/>
       <c r="G114" s="4"/>
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" s="3">
-        <v>113</v>
+        <v>120</v>
       </c>
       <c r="B115" s="4"/>
       <c r="C115" s="4"/>
       <c r="D115" s="4"/>
       <c r="E115" s="4"/>
-      <c r="F115" s="5"/>
+      <c r="F115" s="15"/>
       <c r="G115" s="4"/>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" s="3">
-        <v>114</v>
+        <v>121</v>
       </c>
       <c r="B116" s="4"/>
       <c r="C116" s="4"/>
       <c r="D116" s="4"/>
       <c r="E116" s="4"/>
-      <c r="F116" s="5"/>
+      <c r="F116" s="15"/>
       <c r="G116" s="4"/>
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" s="3">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="B117" s="4"/>
       <c r="C117" s="4"/>
       <c r="D117" s="4"/>
       <c r="E117" s="4"/>
-      <c r="F117" s="5"/>
+      <c r="F117" s="15"/>
       <c r="G117" s="4"/>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" s="3">
-        <v>116</v>
+        <v>123</v>
       </c>
       <c r="B118" s="4"/>
       <c r="C118" s="4"/>
       <c r="D118" s="4"/>
       <c r="E118" s="4"/>
-      <c r="F118" s="5"/>
+      <c r="F118" s="15"/>
       <c r="G118" s="4"/>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" s="3">
-        <v>117</v>
+        <v>124</v>
       </c>
       <c r="B119" s="4"/>
       <c r="C119" s="4"/>
       <c r="D119" s="4"/>
       <c r="E119" s="4"/>
-      <c r="F119" s="5"/>
+      <c r="F119" s="15"/>
       <c r="G119" s="4"/>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" s="3">
-        <v>118</v>
+        <v>125</v>
       </c>
       <c r="B120" s="4"/>
       <c r="C120" s="4"/>
       <c r="D120" s="4"/>
       <c r="E120" s="4"/>
-      <c r="F120" s="5"/>
+      <c r="F120" s="15"/>
       <c r="G120" s="4"/>
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" s="3">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="B121" s="4"/>
       <c r="C121" s="4"/>
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
-      <c r="F121" s="5"/>
+      <c r="F121" s="15"/>
       <c r="G121" s="4"/>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" s="3">
-        <v>120</v>
+        <v>127</v>
       </c>
       <c r="B122" s="4"/>
       <c r="C122" s="4"/>
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
-      <c r="F122" s="5"/>
+      <c r="F122" s="15"/>
       <c r="G122" s="4"/>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" s="3">
-        <v>121</v>
+        <v>128</v>
       </c>
       <c r="B123" s="4"/>
       <c r="C123" s="4"/>
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
-      <c r="F123" s="5"/>
+      <c r="F123" s="15"/>
       <c r="G123" s="4"/>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" s="3">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B124" s="4"/>
       <c r="C124" s="4"/>
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
-      <c r="F124" s="5"/>
+      <c r="F124" s="15"/>
       <c r="G124" s="4"/>
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" s="3">
-        <v>123</v>
+        <v>130</v>
       </c>
       <c r="B125" s="4"/>
       <c r="C125" s="4"/>
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
-      <c r="F125" s="5"/>
+      <c r="F125" s="15"/>
       <c r="G125" s="4"/>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" s="3">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
-      <c r="F126" s="5"/>
+      <c r="F126" s="15"/>
       <c r="G126" s="4"/>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" s="3">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
-      <c r="F127" s="5"/>
+      <c r="F127" s="15"/>
       <c r="G127" s="4"/>
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" s="3">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B128" s="4"/>
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
-      <c r="F128" s="5"/>
+      <c r="F128" s="15"/>
       <c r="G128" s="4"/>
       <c r="H128" s="4"/>
       <c r="I128" s="4"/>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" s="3">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="B129" s="4"/>
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
-      <c r="F129" s="5"/>
+      <c r="F129" s="15"/>
       <c r="G129" s="4"/>
       <c r="H129" s="4"/>
       <c r="I129" s="4"/>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" s="3">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="B130" s="4"/>
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
-      <c r="F130" s="5"/>
+      <c r="F130" s="15"/>
       <c r="G130" s="4"/>
       <c r="H130" s="4"/>
       <c r="I130" s="4"/>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" s="3">
-        <v>129</v>
+        <v>136</v>
       </c>
       <c r="B131" s="4"/>
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
-      <c r="F131" s="5"/>
+      <c r="F131" s="15"/>
       <c r="G131" s="4"/>
       <c r="H131" s="4"/>
       <c r="I131" s="4"/>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" s="3">
-        <v>130</v>
+        <v>137</v>
       </c>
       <c r="B132" s="4"/>
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
-      <c r="F132" s="5"/>
+      <c r="F132" s="15"/>
       <c r="G132" s="4"/>
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" s="3">
-        <v>131</v>
+        <v>138</v>
       </c>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
-      <c r="F133" s="5"/>
+      <c r="F133" s="15"/>
       <c r="G133" s="4"/>
       <c r="H133" s="4"/>
       <c r="I133" s="4"/>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" s="3">
-        <v>132</v>
+        <v>139</v>
       </c>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
-      <c r="F134" s="5"/>
+      <c r="F134" s="15"/>
       <c r="G134" s="4"/>
       <c r="H134" s="4"/>
       <c r="I134" s="4"/>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" s="3">
-        <v>133</v>
+        <v>140</v>
       </c>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
-      <c r="F135" s="5"/>
+      <c r="F135" s="15"/>
       <c r="G135" s="4"/>
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" s="3">
-        <v>134</v>
+        <v>141</v>
       </c>
       <c r="B136" s="4"/>
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
-      <c r="F136" s="5"/>
+      <c r="F136" s="15"/>
       <c r="G136" s="4"/>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" s="3">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
-      <c r="F137" s="5"/>
+      <c r="F137" s="15"/>
       <c r="G137" s="4"/>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" s="3">
-        <v>136</v>
+        <v>143</v>
       </c>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
-      <c r="F138" s="5"/>
+      <c r="F138" s="15"/>
       <c r="G138" s="4"/>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" s="3">
-        <v>137</v>
+        <v>144</v>
       </c>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
-      <c r="F139" s="5"/>
+      <c r="F139" s="15"/>
       <c r="G139" s="4"/>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" s="3">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="B140" s="4"/>
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
-      <c r="F140" s="5"/>
+      <c r="F140" s="15"/>
       <c r="G140" s="4"/>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" s="3">
-        <v>139</v>
+        <v>146</v>
       </c>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
-      <c r="F141" s="5"/>
+      <c r="F141" s="15"/>
       <c r="G141" s="4"/>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A142" s="3">
-        <v>140</v>
+        <v>147</v>
       </c>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
-      <c r="F142" s="5"/>
+      <c r="F142" s="15"/>
       <c r="G142" s="4"/>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A143" s="3">
-        <v>141</v>
+        <v>148</v>
       </c>
       <c r="B143" s="4"/>
       <c r="C143" s="4"/>
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
-      <c r="F143" s="5"/>
+      <c r="F143" s="15"/>
       <c r="G143" s="4"/>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A144" s="3">
-        <v>142</v>
+        <v>149</v>
       </c>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
-      <c r="F144" s="5"/>
+      <c r="F144" s="15"/>
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A145" s="3">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="B145" s="4"/>
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
-      <c r="F145" s="5"/>
+      <c r="F145" s="15"/>
       <c r="G145" s="4"/>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A146" s="3">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="B146" s="4"/>
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
-      <c r="F146" s="5"/>
+      <c r="F146" s="15"/>
       <c r="G146" s="4"/>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A147" s="3">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="B147" s="4"/>
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
-      <c r="F147" s="5"/>
+      <c r="F147" s="15"/>
       <c r="G147" s="4"/>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A148" s="3">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
-      <c r="F148" s="5"/>
+      <c r="F148" s="15"/>
       <c r="G148" s="4"/>
       <c r="H148" s="4"/>
       <c r="I148" s="4"/>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A149" s="3">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="B149" s="4"/>
       <c r="C149" s="4"/>
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
-      <c r="F149" s="5"/>
+      <c r="F149" s="15"/>
       <c r="G149" s="4"/>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A150" s="3">
-        <v>148</v>
+        <v>155</v>
       </c>
       <c r="B150" s="4"/>
       <c r="C150" s="4"/>
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
-      <c r="F150" s="5"/>
+      <c r="F150" s="15"/>
       <c r="G150" s="4"/>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A151" s="3">
-        <v>149</v>
+        <v>156</v>
       </c>
       <c r="B151" s="4"/>
       <c r="C151" s="4"/>
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
-      <c r="F151" s="5"/>
+      <c r="F151" s="15"/>
       <c r="G151" s="4"/>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A152" s="3">
-        <v>150</v>
+        <v>157</v>
       </c>
       <c r="B152" s="4"/>
       <c r="C152" s="4"/>
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
-      <c r="F152" s="5"/>
+      <c r="F152" s="15"/>
       <c r="G152" s="4"/>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A153" s="3">
-        <v>151</v>
+        <v>158</v>
       </c>
       <c r="B153" s="4"/>
       <c r="C153" s="4"/>
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
-      <c r="F153" s="5"/>
+      <c r="F153" s="15"/>
       <c r="G153" s="4"/>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A154" s="3">
-        <v>152</v>
+        <v>159</v>
       </c>
       <c r="B154" s="4"/>
       <c r="C154" s="4"/>
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
-      <c r="F154" s="5"/>
+      <c r="F154" s="15"/>
       <c r="G154" s="4"/>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A155" s="3">
-        <v>153</v>
+        <v>160</v>
       </c>
       <c r="B155" s="4"/>
       <c r="C155" s="4"/>
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
-      <c r="F155" s="5"/>
+      <c r="F155" s="15"/>
       <c r="G155" s="4"/>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A156" s="3">
-        <v>154</v>
+        <v>161</v>
       </c>
       <c r="B156" s="4"/>
       <c r="C156" s="4"/>
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
-      <c r="F156" s="5"/>
+      <c r="F156" s="15"/>
       <c r="G156" s="4"/>
       <c r="H156" s="4"/>
       <c r="I156" s="4"/>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A157" s="3">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="B157" s="4"/>
       <c r="C157" s="4"/>
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
-      <c r="F157" s="5"/>
+      <c r="F157" s="15"/>
       <c r="G157" s="4"/>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A158" s="3">
-        <v>156</v>
+        <v>163</v>
       </c>
       <c r="B158" s="4"/>
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
-      <c r="F158" s="5"/>
+      <c r="F158" s="15"/>
       <c r="G158" s="4"/>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A159" s="3">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="B159" s="4"/>
       <c r="C159" s="4"/>
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
-      <c r="F159" s="5"/>
+      <c r="F159" s="15"/>
       <c r="G159" s="4"/>
       <c r="H159" s="4"/>
       <c r="I159" s="4"/>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A160" s="3">
-        <v>158</v>
+        <v>165</v>
       </c>
       <c r="B160" s="4"/>
       <c r="C160" s="4"/>
       <c r="D160" s="4"/>
       <c r="E160" s="4"/>
-      <c r="F160" s="5"/>
+      <c r="F160" s="15"/>
       <c r="G160" s="4"/>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A161" s="3">
-        <v>159</v>
+        <v>166</v>
       </c>
       <c r="B161" s="4"/>
       <c r="C161" s="4"/>
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
-      <c r="F161" s="5"/>
+      <c r="F161" s="15"/>
       <c r="G161" s="4"/>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A162" s="3">
-        <v>160</v>
+        <v>167</v>
       </c>
       <c r="B162" s="4"/>
       <c r="C162" s="4"/>
       <c r="D162" s="4"/>
       <c r="E162" s="4"/>
-      <c r="F162" s="5"/>
+      <c r="F162" s="15"/>
       <c r="G162" s="4"/>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A163" s="3">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="B163" s="4"/>
       <c r="C163" s="4"/>
       <c r="D163" s="4"/>
       <c r="E163" s="4"/>
-      <c r="F163" s="5"/>
+      <c r="F163" s="15"/>
       <c r="G163" s="4"/>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A164" s="3">
-        <v>162</v>
+        <v>169</v>
       </c>
       <c r="B164" s="4"/>
       <c r="C164" s="4"/>
       <c r="D164" s="4"/>
       <c r="E164" s="4"/>
-      <c r="F164" s="5"/>
+      <c r="F164" s="15"/>
       <c r="G164" s="4"/>
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A165" s="3">
-        <v>163</v>
+        <v>170</v>
       </c>
       <c r="B165" s="4"/>
       <c r="C165" s="4"/>
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
-      <c r="F165" s="5"/>
+      <c r="F165" s="15"/>
       <c r="G165" s="4"/>
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A166" s="3">
-        <v>164</v>
+        <v>171</v>
       </c>
       <c r="B166" s="4"/>
       <c r="C166" s="4"/>
       <c r="D166" s="4"/>
       <c r="E166" s="4"/>
-      <c r="F166" s="5"/>
+      <c r="F166" s="15"/>
       <c r="G166" s="4"/>
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A167" s="3">
-        <v>165</v>
+        <v>172</v>
       </c>
       <c r="B167" s="4"/>
       <c r="C167" s="4"/>
       <c r="D167" s="4"/>
       <c r="E167" s="4"/>
-      <c r="F167" s="5"/>
+      <c r="F167" s="15"/>
       <c r="G167" s="4"/>
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A168" s="3">
-        <v>166</v>
+        <v>173</v>
       </c>
       <c r="B168" s="4"/>
       <c r="C168" s="4"/>
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
-      <c r="F168" s="5"/>
+      <c r="F168" s="15"/>
       <c r="G168" s="4"/>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A169" s="3">
-        <v>167</v>
+        <v>174</v>
       </c>
       <c r="B169" s="4"/>
       <c r="C169" s="4"/>
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
-      <c r="F169" s="5"/>
+      <c r="F169" s="15"/>
       <c r="G169" s="4"/>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A170" s="3">
-        <v>168</v>
+        <v>175</v>
       </c>
       <c r="B170" s="4"/>
       <c r="C170" s="4"/>
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
-      <c r="F170" s="5"/>
+      <c r="F170" s="15"/>
       <c r="G170" s="4"/>
       <c r="H170" s="4"/>
       <c r="I170" s="4"/>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A171" s="3">
-        <v>169</v>
+        <v>176</v>
       </c>
       <c r="B171" s="4"/>
       <c r="C171" s="4"/>
       <c r="D171" s="4"/>
       <c r="E171" s="4"/>
-      <c r="F171" s="5"/>
+      <c r="F171" s="15"/>
       <c r="G171" s="4"/>
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A172" s="3">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="B172" s="4"/>
       <c r="C172" s="4"/>
       <c r="D172" s="4"/>
       <c r="E172" s="4"/>
-      <c r="F172" s="5"/>
+      <c r="F172" s="15"/>
       <c r="G172" s="4"/>
       <c r="H172" s="4"/>
       <c r="I172" s="4"/>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A173" s="3">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="B173" s="4"/>
       <c r="C173" s="4"/>
       <c r="D173" s="4"/>
       <c r="E173" s="4"/>
-      <c r="F173" s="5"/>
+      <c r="F173" s="15"/>
       <c r="G173" s="4"/>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A174" s="3">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="B174" s="4"/>
       <c r="C174" s="4"/>
       <c r="D174" s="4"/>
       <c r="E174" s="4"/>
-      <c r="F174" s="5"/>
+      <c r="F174" s="15"/>
       <c r="G174" s="4"/>
       <c r="H174" s="4"/>
       <c r="I174" s="4"/>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A175" s="3">
-        <v>173</v>
+        <v>180</v>
       </c>
       <c r="B175" s="4"/>
       <c r="C175" s="4"/>
       <c r="D175" s="4"/>
       <c r="E175" s="4"/>
-      <c r="F175" s="5"/>
+      <c r="F175" s="15"/>
       <c r="G175" s="4"/>
       <c r="H175" s="4"/>
       <c r="I175" s="4"/>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A176" s="3">
-        <v>174</v>
+        <v>181</v>
       </c>
       <c r="B176" s="4"/>
       <c r="C176" s="4"/>
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
-      <c r="F176" s="5"/>
+      <c r="F176" s="15"/>
       <c r="G176" s="4"/>
       <c r="H176" s="4"/>
       <c r="I176" s="4"/>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A177" s="3">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="B177" s="4"/>
       <c r="C177" s="4"/>
       <c r="D177" s="4"/>
       <c r="E177" s="4"/>
-      <c r="F177" s="5"/>
+      <c r="F177" s="15"/>
       <c r="G177" s="4"/>
       <c r="H177" s="4"/>
       <c r="I177" s="4"/>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A178" s="3">
-        <v>176</v>
+        <v>183</v>
       </c>
       <c r="B178" s="4"/>
       <c r="C178" s="4"/>
       <c r="D178" s="4"/>
       <c r="E178" s="4"/>
-      <c r="F178" s="5"/>
+      <c r="F178" s="15"/>
       <c r="G178" s="4"/>
       <c r="H178" s="4"/>
       <c r="I178" s="4"/>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A179" s="3">
-        <v>177</v>
+        <v>184</v>
       </c>
       <c r="B179" s="4"/>
       <c r="C179" s="4"/>
       <c r="D179" s="4"/>
       <c r="E179" s="4"/>
-      <c r="F179" s="5"/>
+      <c r="F179" s="15"/>
       <c r="G179" s="4"/>
       <c r="H179" s="4"/>
       <c r="I179" s="4"/>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A180" s="3">
-        <v>178</v>
+        <v>185</v>
       </c>
       <c r="B180" s="4"/>
       <c r="C180" s="4"/>
       <c r="D180" s="4"/>
       <c r="E180" s="4"/>
-      <c r="F180" s="5"/>
+      <c r="F180" s="15"/>
       <c r="G180" s="4"/>
       <c r="H180" s="4"/>
       <c r="I180" s="4"/>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A181" s="3">
-        <v>179</v>
+        <v>186</v>
       </c>
       <c r="B181" s="4"/>
       <c r="C181" s="4"/>
       <c r="D181" s="4"/>
       <c r="E181" s="4"/>
-      <c r="F181" s="5"/>
+      <c r="F181" s="15"/>
       <c r="G181" s="4"/>
       <c r="H181" s="4"/>
       <c r="I181" s="4"/>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A182" s="3">
-        <v>180</v>
+        <v>187</v>
       </c>
       <c r="B182" s="4"/>
       <c r="C182" s="4"/>
       <c r="D182" s="4"/>
       <c r="E182" s="4"/>
-      <c r="F182" s="5"/>
+      <c r="F182" s="15"/>
       <c r="G182" s="4"/>
       <c r="H182" s="4"/>
       <c r="I182" s="4"/>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A183" s="3">
-        <v>181</v>
+        <v>188</v>
       </c>
       <c r="B183" s="4"/>
       <c r="C183" s="4"/>
       <c r="D183" s="4"/>
       <c r="E183" s="4"/>
-      <c r="F183" s="5"/>
+      <c r="F183" s="15"/>
       <c r="G183" s="4"/>
       <c r="H183" s="4"/>
       <c r="I183" s="4"/>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A184" s="3">
-        <v>182</v>
+        <v>189</v>
       </c>
       <c r="B184" s="4"/>
       <c r="C184" s="4"/>
       <c r="D184" s="4"/>
       <c r="E184" s="4"/>
-      <c r="F184" s="5"/>
+      <c r="F184" s="15"/>
       <c r="G184" s="4"/>
       <c r="H184" s="4"/>
       <c r="I184" s="4"/>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A185" s="3">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="B185" s="4"/>
       <c r="C185" s="4"/>
       <c r="D185" s="4"/>
       <c r="E185" s="4"/>
-      <c r="F185" s="5"/>
+      <c r="F185" s="15"/>
       <c r="G185" s="4"/>
       <c r="H185" s="4"/>
       <c r="I185" s="4"/>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A186" s="3">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="B186" s="4"/>
       <c r="C186" s="4"/>
       <c r="D186" s="4"/>
       <c r="E186" s="4"/>
-      <c r="F186" s="5"/>
+      <c r="F186" s="15"/>
       <c r="G186" s="4"/>
       <c r="H186" s="4"/>
       <c r="I186" s="4"/>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A187" s="3">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="B187" s="4"/>
       <c r="C187" s="4"/>
       <c r="D187" s="4"/>
       <c r="E187" s="4"/>
-      <c r="F187" s="5"/>
+      <c r="F187" s="15"/>
       <c r="G187" s="4"/>
       <c r="H187" s="4"/>
       <c r="I187" s="4"/>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A188" s="3">
-        <v>186</v>
+        <v>193</v>
       </c>
       <c r="B188" s="4"/>
       <c r="C188" s="4"/>
       <c r="D188" s="4"/>
       <c r="E188" s="4"/>
-      <c r="F188" s="5"/>
+      <c r="F188" s="15"/>
       <c r="G188" s="4"/>
       <c r="H188" s="4"/>
       <c r="I188" s="4"/>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A189" s="3">
-        <v>187</v>
+        <v>194</v>
       </c>
       <c r="B189" s="4"/>
       <c r="C189" s="4"/>
       <c r="D189" s="4"/>
       <c r="E189" s="4"/>
-      <c r="F189" s="5"/>
+      <c r="F189" s="15"/>
       <c r="G189" s="4"/>
       <c r="H189" s="4"/>
       <c r="I189" s="4"/>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A190" s="3">
-        <v>188</v>
+        <v>195</v>
       </c>
       <c r="B190" s="4"/>
       <c r="C190" s="4"/>
       <c r="D190" s="4"/>
       <c r="E190" s="4"/>
-      <c r="F190" s="5"/>
+      <c r="F190" s="15"/>
       <c r="G190" s="4"/>
       <c r="H190" s="4"/>
       <c r="I190" s="4"/>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A191" s="3">
-        <v>189</v>
+        <v>196</v>
       </c>
       <c r="B191" s="4"/>
       <c r="C191" s="4"/>
       <c r="D191" s="4"/>
       <c r="E191" s="4"/>
-      <c r="F191" s="5"/>
+      <c r="F191" s="15"/>
       <c r="G191" s="4"/>
       <c r="H191" s="4"/>
       <c r="I191" s="4"/>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A192" s="3">
-        <v>190</v>
+        <v>197</v>
       </c>
       <c r="B192" s="4"/>
       <c r="C192" s="4"/>
       <c r="D192" s="4"/>
       <c r="E192" s="4"/>
-      <c r="F192" s="5"/>
+      <c r="F192" s="15"/>
       <c r="G192" s="4"/>
       <c r="H192" s="4"/>
       <c r="I192" s="4"/>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A193" s="3">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="B193" s="4"/>
       <c r="C193" s="4"/>
       <c r="D193" s="4"/>
       <c r="E193" s="4"/>
-      <c r="F193" s="5"/>
+      <c r="F193" s="15"/>
       <c r="G193" s="4"/>
       <c r="H193" s="4"/>
       <c r="I193" s="4"/>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A194" s="3">
-        <v>192</v>
+        <v>199</v>
       </c>
       <c r="B194" s="4"/>
       <c r="C194" s="4"/>
       <c r="D194" s="4"/>
       <c r="E194" s="4"/>
-      <c r="F194" s="5"/>
+      <c r="F194" s="15"/>
       <c r="G194" s="4"/>
       <c r="H194" s="4"/>
       <c r="I194" s="4"/>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A195" s="3">
-        <v>193</v>
+        <v>200</v>
       </c>
       <c r="B195" s="4"/>
       <c r="C195" s="4"/>
       <c r="D195" s="4"/>
       <c r="E195" s="4"/>
-      <c r="F195" s="5"/>
+      <c r="F195" s="15"/>
       <c r="G195" s="4"/>
       <c r="H195" s="4"/>
       <c r="I195" s="4"/>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A196" s="3">
-        <v>194</v>
+        <v>201</v>
       </c>
       <c r="B196" s="4"/>
       <c r="C196" s="4"/>
       <c r="D196" s="4"/>
       <c r="E196" s="4"/>
-      <c r="F196" s="4"/>
+      <c r="F196" s="15"/>
       <c r="G196" s="4"/>
       <c r="H196" s="4"/>
       <c r="I196" s="4"/>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A197" s="3">
-        <v>195</v>
+        <v>202</v>
       </c>
       <c r="B197" s="4"/>
       <c r="C197" s="4"/>
       <c r="D197" s="4"/>
       <c r="E197" s="4"/>
-      <c r="F197" s="4"/>
+      <c r="F197" s="15"/>
       <c r="G197" s="4"/>
       <c r="H197" s="4"/>
       <c r="I197" s="4"/>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A198" s="3">
-        <v>196</v>
+        <v>203</v>
       </c>
       <c r="B198" s="4"/>
       <c r="C198" s="4"/>
       <c r="D198" s="4"/>
       <c r="E198" s="4"/>
-      <c r="F198" s="4"/>
+      <c r="F198" s="15"/>
       <c r="G198" s="4"/>
       <c r="H198" s="4"/>
       <c r="I198" s="4"/>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A199" s="3">
-        <v>197</v>
-      </c>
+    <row r="199" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A199" s="4"/>
       <c r="B199" s="4"/>
       <c r="C199" s="4"/>
       <c r="D199" s="4"/>
       <c r="E199" s="4"/>
-      <c r="F199" s="4"/>
+      <c r="F199" s="15"/>
       <c r="G199" s="4"/>
       <c r="H199" s="4"/>
       <c r="I199" s="4"/>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A200" s="3">
-        <v>198</v>
-      </c>
-      <c r="B200" s="4"/>
-      <c r="C200" s="4"/>
-      <c r="D200" s="4"/>
-      <c r="E200" s="4"/>
-      <c r="F200" s="4"/>
-      <c r="G200" s="4"/>
-      <c r="H200" s="4"/>
-      <c r="I200" s="4"/>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A201" s="3">
-        <v>199</v>
-      </c>
-      <c r="B201" s="4"/>
-      <c r="C201" s="4"/>
-      <c r="D201" s="4"/>
-      <c r="E201" s="4"/>
-      <c r="F201" s="4"/>
-      <c r="G201" s="4"/>
-      <c r="H201" s="4"/>
-      <c r="I201" s="4"/>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A202" s="3">
-        <v>200</v>
-      </c>
-      <c r="B202" s="4"/>
-      <c r="C202" s="4"/>
-      <c r="D202" s="4"/>
-      <c r="E202" s="4"/>
-      <c r="F202" s="4"/>
-      <c r="G202" s="4"/>
-      <c r="H202" s="4"/>
-      <c r="I202" s="4"/>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A203" s="3">
-        <v>201</v>
-      </c>
-      <c r="B203" s="4"/>
-      <c r="C203" s="4"/>
-      <c r="D203" s="4"/>
-      <c r="E203" s="4"/>
-      <c r="F203" s="4"/>
-      <c r="G203" s="4"/>
-      <c r="H203" s="4"/>
-      <c r="I203" s="4"/>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A204" s="3">
-        <v>202</v>
-      </c>
-      <c r="B204" s="4"/>
-      <c r="C204" s="4"/>
-      <c r="D204" s="4"/>
-      <c r="E204" s="4"/>
-      <c r="F204" s="4"/>
-      <c r="G204" s="4"/>
-      <c r="H204" s="4"/>
-      <c r="I204" s="4"/>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A205" s="3">
-        <v>203</v>
-      </c>
-      <c r="B205" s="4"/>
-      <c r="C205" s="4"/>
-      <c r="D205" s="4"/>
-      <c r="E205" s="4"/>
-      <c r="F205" s="4"/>
-      <c r="G205" s="4"/>
-      <c r="H205" s="4"/>
-      <c r="I205" s="4"/>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A206" s="4"/>
-      <c r="B206" s="4"/>
-      <c r="C206" s="4"/>
-      <c r="D206" s="4"/>
-      <c r="E206" s="4"/>
-      <c r="F206" s="4"/>
-      <c r="G206" s="4"/>
-      <c r="H206" s="4"/>
-      <c r="I206" s="4"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A2:I200"/>
+  <autoFilter ref="A2:I193"/>
   <dataConsolidate/>
   <mergeCells count="1">
     <mergeCell ref="A1:I1"/>
@@ -4743,18 +4903,6 @@
     </cfRule>
     <cfRule type="cellIs" dxfId="12" priority="23" operator="equal">
       <formula>"Very High"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I3:I28 I47:I200">
-    <cfRule type="colorScale" priority="91">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C46">
@@ -4823,14 +4971,26 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="I3:I28 I47:I193">
+    <cfRule type="colorScale" priority="169">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E200">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E193">
       <formula1>"Tan Tran, Nhung Huyng, Tuong Nguyen, Nguyen Dinh, Quyet Nguyen, Dang Nguyen, Tung Nguyen, Loc Phan"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C200">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C3:C193">
       <formula1>"Very High,High, Medium, Low"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D199">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D3:D192">
       <formula1>"RE, Architecture, Detail Design, Implementation, Testing, Management"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4846,7 +5006,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4858,7 +5018,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Dang update Measurement and Project Plan
</commit_message>
<xml_diff>
--- a/Project Plan/Mesurement.xlsx
+++ b/Project Plan/Mesurement.xlsx
@@ -267,9 +267,6 @@
     <t>Test Case : Working Progress and Labor Union</t>
   </si>
   <si>
-    <t>Design Interface: Detail Information</t>
-  </si>
-  <si>
     <t>Plan Detail Design</t>
   </si>
   <si>
@@ -437,6 +434,9 @@
   </si>
   <si>
     <t>Nhung Huynh</t>
+  </si>
+  <si>
+    <t>Design Interface: Detail and Expand Information</t>
   </si>
 </sst>
 </file>
@@ -581,7 +581,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -599,7 +599,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -620,7 +619,155 @@
     <cellStyle name="Normal 2" xfId="1"/>
     <cellStyle name="Normal 3" xfId="2"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="8" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1068,9 +1215,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K183"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1081,7 +1228,7 @@
     <col min="4" max="4" width="15.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.85546875" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" style="14" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" style="2" bestFit="1" customWidth="1"/>
@@ -1090,18 +1237,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1120,9 +1267,9 @@
         <v>2</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="G2" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="G2" s="12" t="s">
         <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -1151,11 +1298,11 @@
       <c r="E3" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="18">
+      <c r="F3" s="17">
         <f>INT((G3-$K$3)/7)+1</f>
         <v>2</v>
       </c>
-      <c r="G3" s="14">
+      <c r="G3" s="13">
         <v>40823</v>
       </c>
       <c r="H3" s="3">
@@ -1167,7 +1314,7 @@
       <c r="J3" s="4">
         <v>100</v>
       </c>
-      <c r="K3" s="17">
+      <c r="K3" s="16">
         <v>40812</v>
       </c>
     </row>
@@ -1187,11 +1334,11 @@
       <c r="E4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F4" s="18">
+      <c r="F4" s="17">
         <f t="shared" ref="F4:F66" si="0">INT((G4-$K$3)/7)+1</f>
         <v>3</v>
       </c>
-      <c r="G4" s="14">
+      <c r="G4" s="13">
         <v>40827</v>
       </c>
       <c r="H4" s="3">
@@ -1220,11 +1367,11 @@
       <c r="E5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F5" s="18">
+      <c r="F5" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G5" s="14">
+      <c r="G5" s="13">
         <v>40828</v>
       </c>
       <c r="H5" s="3">
@@ -1253,11 +1400,11 @@
       <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="18">
+      <c r="F6" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G6" s="14">
+      <c r="G6" s="13">
         <v>40845</v>
       </c>
       <c r="H6" s="3">
@@ -1286,11 +1433,11 @@
       <c r="E7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F7" s="18">
+      <c r="F7" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G7" s="14">
+      <c r="G7" s="13">
         <v>40874</v>
       </c>
       <c r="H7" s="3">
@@ -1319,11 +1466,11 @@
       <c r="E8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="18">
+      <c r="F8" s="17">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="G8" s="14">
+      <c r="G8" s="13">
         <v>40934</v>
       </c>
       <c r="H8" s="3">
@@ -1341,7 +1488,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>19</v>
@@ -1352,11 +1499,11 @@
       <c r="E9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="18">
+      <c r="F9" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G9" s="14">
+      <c r="G9" s="13">
         <v>40929</v>
       </c>
       <c r="H9" s="3">
@@ -1385,11 +1532,11 @@
       <c r="E10" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F10" s="18">
+      <c r="F10" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G10" s="14">
+      <c r="G10" s="13">
         <v>40916</v>
       </c>
       <c r="H10" s="3">
@@ -1418,11 +1565,11 @@
       <c r="E11" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F11" s="18">
+      <c r="F11" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G11" s="14">
+      <c r="G11" s="13">
         <v>40850</v>
       </c>
       <c r="H11" s="3">
@@ -1451,11 +1598,11 @@
       <c r="E12" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F12" s="18">
+      <c r="F12" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G12" s="14">
+      <c r="G12" s="13">
         <v>40921</v>
       </c>
       <c r="H12" s="3">
@@ -1484,11 +1631,11 @@
       <c r="E13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F13" s="18">
+      <c r="F13" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G13" s="14">
+      <c r="G13" s="13">
         <v>40924</v>
       </c>
       <c r="H13" s="3">
@@ -1517,11 +1664,11 @@
       <c r="E14" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F14" s="18">
+      <c r="F14" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G14" s="14">
+      <c r="G14" s="13">
         <v>40926</v>
       </c>
       <c r="H14" s="3">
@@ -1550,11 +1697,11 @@
       <c r="E15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F15" s="18">
+      <c r="F15" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="G15" s="14">
+      <c r="G15" s="13">
         <v>40925</v>
       </c>
       <c r="H15" s="3">
@@ -1583,11 +1730,11 @@
       <c r="E16" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F16" s="18">
+      <c r="F16" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G16" s="14">
+      <c r="G16" s="13">
         <v>40890</v>
       </c>
       <c r="H16" s="3">
@@ -1616,11 +1763,11 @@
       <c r="E17" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F17" s="18">
+      <c r="F17" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G17" s="14">
+      <c r="G17" s="13">
         <v>40896</v>
       </c>
       <c r="H17" s="3">
@@ -1649,11 +1796,11 @@
       <c r="E18" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="18">
+      <c r="F18" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G18" s="14">
+      <c r="G18" s="13">
         <v>40826</v>
       </c>
       <c r="H18" s="3">
@@ -1671,7 +1818,7 @@
         <v>17</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>33</v>
@@ -1682,11 +1829,11 @@
       <c r="E19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="18">
+      <c r="F19" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="G19" s="14">
+      <c r="G19" s="13">
         <v>40841</v>
       </c>
       <c r="H19" s="3">
@@ -1715,11 +1862,11 @@
       <c r="E20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F20" s="18">
+      <c r="F20" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G20" s="14">
+      <c r="G20" s="13">
         <v>40851</v>
       </c>
       <c r="H20" s="3">
@@ -1748,11 +1895,11 @@
       <c r="E21" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F21" s="18">
+      <c r="F21" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="G21" s="14">
+      <c r="G21" s="13">
         <v>40850</v>
       </c>
       <c r="H21" s="3">
@@ -1781,11 +1928,11 @@
       <c r="E22" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G22" s="14">
+      <c r="G22" s="13">
         <v>40902</v>
       </c>
       <c r="H22" s="3">
@@ -1814,11 +1961,11 @@
       <c r="E23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F23" s="18">
+      <c r="F23" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G23" s="14">
+      <c r="G23" s="13">
         <v>40916</v>
       </c>
       <c r="H23" s="3">
@@ -1847,11 +1994,11 @@
       <c r="E24" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F24" s="18">
+      <c r="F24" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="G24" s="14">
+      <c r="G24" s="13">
         <v>40871</v>
       </c>
       <c r="H24" s="3">
@@ -1880,11 +2027,11 @@
       <c r="E25" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G25" s="14">
+      <c r="G25" s="13">
         <v>40886</v>
       </c>
       <c r="H25" s="3">
@@ -1913,11 +2060,11 @@
       <c r="E26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G26" s="14">
+      <c r="G26" s="13">
         <v>40886</v>
       </c>
       <c r="H26" s="3">
@@ -1946,11 +2093,11 @@
       <c r="E27" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="17">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="G27" s="14">
+      <c r="G27" s="13">
         <v>40908</v>
       </c>
       <c r="H27" s="3">
@@ -1977,13 +2124,13 @@
         <v>27</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F28" s="18">
+        <v>137</v>
+      </c>
+      <c r="F28" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G28" s="14">
+      <c r="G28" s="13">
         <v>40900</v>
       </c>
       <c r="H28" s="3">
@@ -2010,13 +2157,13 @@
         <v>27</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F29" s="18">
+        <v>137</v>
+      </c>
+      <c r="F29" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G29" s="14">
+      <c r="G29" s="13">
         <v>40900</v>
       </c>
       <c r="H29" s="3">
@@ -2043,13 +2190,13 @@
         <v>27</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F30" s="18">
+        <v>137</v>
+      </c>
+      <c r="F30" s="17">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G30" s="14">
+      <c r="G30" s="13">
         <v>40954</v>
       </c>
       <c r="H30" s="3">
@@ -2076,13 +2223,13 @@
         <v>27</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F31" s="18">
+        <v>137</v>
+      </c>
+      <c r="F31" s="17">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G31" s="14">
+      <c r="G31" s="13">
         <v>40954</v>
       </c>
       <c r="H31" s="3">
@@ -2109,13 +2256,13 @@
         <v>27</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F32" s="18">
+        <v>137</v>
+      </c>
+      <c r="F32" s="17">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="G32" s="14">
+      <c r="G32" s="13">
         <v>40954</v>
       </c>
       <c r="H32" s="3">
@@ -2142,13 +2289,13 @@
         <v>27</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F33" s="18">
+        <v>137</v>
+      </c>
+      <c r="F33" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G33" s="14">
+      <c r="G33" s="13">
         <v>40827</v>
       </c>
       <c r="H33" s="3">
@@ -2175,13 +2322,13 @@
         <v>27</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F34" s="18">
+        <v>137</v>
+      </c>
+      <c r="F34" s="17">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="G34" s="14">
+      <c r="G34" s="13">
         <v>40829</v>
       </c>
       <c r="H34" s="3">
@@ -2208,13 +2355,13 @@
         <v>27</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F35" s="18">
+        <v>137</v>
+      </c>
+      <c r="F35" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G35" s="14">
+      <c r="G35" s="13">
         <v>40889</v>
       </c>
       <c r="H35" s="3">
@@ -2241,13 +2388,13 @@
         <v>26</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F36" s="18">
+        <v>137</v>
+      </c>
+      <c r="F36" s="17">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="G36" s="14">
+      <c r="G36" s="13">
         <v>40854</v>
       </c>
       <c r="H36" s="3">
@@ -2274,13 +2421,13 @@
         <v>27</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F37" s="18">
+        <v>137</v>
+      </c>
+      <c r="F37" s="17">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G37" s="14">
+      <c r="G37" s="13">
         <v>40910</v>
       </c>
       <c r="H37" s="3">
@@ -2307,13 +2454,13 @@
         <v>26</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F38" s="18">
+        <v>137</v>
+      </c>
+      <c r="F38" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G38" s="14">
+      <c r="G38" s="13">
         <v>40888</v>
       </c>
       <c r="H38" s="3">
@@ -2340,13 +2487,13 @@
         <v>26</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F39" s="18">
+        <v>137</v>
+      </c>
+      <c r="F39" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G39" s="14">
+      <c r="G39" s="13">
         <v>40889</v>
       </c>
       <c r="H39" s="3">
@@ -2373,13 +2520,13 @@
         <v>26</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F40" s="18">
+        <v>137</v>
+      </c>
+      <c r="F40" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="G40" s="14">
+      <c r="G40" s="13">
         <v>40889</v>
       </c>
       <c r="H40" s="3">
@@ -2406,13 +2553,13 @@
         <v>27</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F41" s="18">
+        <v>137</v>
+      </c>
+      <c r="F41" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="G41" s="14">
+      <c r="G41" s="13">
         <v>40896</v>
       </c>
       <c r="H41" s="3">
@@ -2439,13 +2586,13 @@
         <v>27</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F42" s="18">
+        <v>137</v>
+      </c>
+      <c r="F42" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="G42" s="14">
+      <c r="G42" s="13">
         <v>40888</v>
       </c>
       <c r="H42" s="3">
@@ -2472,13 +2619,13 @@
         <v>27</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F43" s="18">
+        <v>137</v>
+      </c>
+      <c r="F43" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G43" s="14">
+      <c r="G43" s="13">
         <v>40921</v>
       </c>
       <c r="H43" s="3">
@@ -2505,13 +2652,13 @@
         <v>27</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F44" s="18">
+        <v>137</v>
+      </c>
+      <c r="F44" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G44" s="14">
+      <c r="G44" s="13">
         <v>40921</v>
       </c>
       <c r="H44" s="3">
@@ -2538,13 +2685,13 @@
         <v>27</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="F45" s="18">
+        <v>137</v>
+      </c>
+      <c r="F45" s="17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="G45" s="14">
+      <c r="G45" s="13">
         <v>40921</v>
       </c>
       <c r="H45" s="3">
@@ -2559,30 +2706,32 @@
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A46" s="3">
-        <v>44</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>60</v>
+        <v>48</v>
+      </c>
+      <c r="B46" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>26</v>
       </c>
       <c r="E46" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F46" s="18">
-        <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G46" s="14"/>
+      <c r="F46" s="17">
+        <f>INT((G46-$K$3)/7)+1</f>
+        <v>2</v>
+      </c>
+      <c r="G46" s="13">
+        <v>40819</v>
+      </c>
       <c r="H46" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I46" s="3">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="J46" s="4">
         <v>100</v>
@@ -2590,13 +2739,13 @@
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A47" s="3">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="D47" s="4" t="s">
         <v>60</v>
@@ -2604,16 +2753,18 @@
       <c r="E47" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F47" s="18">
+      <c r="F47" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G47" s="14"/>
+        <v>2</v>
+      </c>
+      <c r="G47" s="13">
+        <v>40824</v>
+      </c>
       <c r="H47" s="3">
-        <v>0.5</v>
+        <v>2</v>
       </c>
       <c r="I47" s="3">
-        <v>0.5</v>
+        <v>1.5</v>
       </c>
       <c r="J47" s="4">
         <v>100</v>
@@ -2621,30 +2772,32 @@
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A48" s="3">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>9</v>
+        <v>33</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="E48" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F48" s="18">
+      <c r="F48" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G48" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="G48" s="13">
+        <v>40826</v>
+      </c>
       <c r="H48" s="3">
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="I48" s="3">
-        <v>11.5</v>
+        <v>0.5</v>
       </c>
       <c r="J48" s="4">
         <v>100</v>
@@ -2652,30 +2805,32 @@
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" s="3">
-        <v>47</v>
-      </c>
-      <c r="B49" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="C49" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="C49" s="10" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="E49" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F49" s="18">
-        <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G49" s="14"/>
+      <c r="F49" s="17">
+        <f>INT((G49-$K$3)/7)+1</f>
+        <v>4</v>
+      </c>
+      <c r="G49" s="13">
+        <v>40834</v>
+      </c>
       <c r="H49" s="3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I49" s="3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="J49" s="4">
         <v>100</v>
@@ -2683,30 +2838,32 @@
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" s="3">
-        <v>48</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>26</v>
+        <v>50</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>27</v>
       </c>
       <c r="E50" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F50" s="18">
+      <c r="F50" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G50" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="G50" s="13">
+        <v>40839</v>
+      </c>
       <c r="H50" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I50" s="3">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J50" s="4">
         <v>100</v>
@@ -2714,30 +2871,32 @@
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" s="3">
-        <v>49</v>
-      </c>
-      <c r="B51" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C51" s="10" t="s">
-        <v>20</v>
+        <v>46</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>9</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="E51" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F51" s="18">
-        <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G51" s="14"/>
+      <c r="F51" s="17">
+        <f>INT((G51-$K$3)/7)+1</f>
+        <v>6</v>
+      </c>
+      <c r="G51" s="13">
+        <v>40851</v>
+      </c>
       <c r="H51" s="3">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="I51" s="3">
-        <v>2</v>
+        <v>11.5</v>
       </c>
       <c r="J51" s="4">
         <v>100</v>
@@ -2745,30 +2904,32 @@
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A52" s="3">
-        <v>50</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="C52" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B52" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>20</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E52" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F52" s="18">
-        <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G52" s="14"/>
+      <c r="F52" s="17">
+        <f>INT((G52-$K$3)/7)+1</f>
+        <v>6</v>
+      </c>
+      <c r="G52" s="13">
+        <v>40852</v>
+      </c>
       <c r="H52" s="3">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I52" s="3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J52" s="4">
         <v>100</v>
@@ -2790,11 +2951,13 @@
       <c r="E53" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F53" s="18">
+      <c r="F53" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G53" s="14"/>
+        <v>6</v>
+      </c>
+      <c r="G53" s="13">
+        <v>40848</v>
+      </c>
       <c r="H53" s="3">
         <v>6</v>
       </c>
@@ -2821,11 +2984,13 @@
       <c r="E54" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F54" s="18">
+      <c r="F54" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G54" s="14"/>
+        <v>4</v>
+      </c>
+      <c r="G54" s="13">
+        <v>40839</v>
+      </c>
       <c r="H54" s="3">
         <v>7</v>
       </c>
@@ -2852,11 +3017,13 @@
       <c r="E55" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F55" s="18">
+      <c r="F55" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G55" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="G55" s="13">
+        <v>40859</v>
+      </c>
       <c r="H55" s="3">
         <v>1.5</v>
       </c>
@@ -2871,7 +3038,7 @@
       <c r="A56" s="3">
         <v>54</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B56" s="11" t="s">
         <v>71</v>
       </c>
       <c r="C56" s="4" t="s">
@@ -2883,11 +3050,13 @@
       <c r="E56" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F56" s="18">
+      <c r="F56" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G56" s="14"/>
+        <v>7</v>
+      </c>
+      <c r="G56" s="13">
+        <v>40854</v>
+      </c>
       <c r="H56" s="3">
         <v>1</v>
       </c>
@@ -2902,7 +3071,7 @@
       <c r="A57" s="3">
         <v>55</v>
       </c>
-      <c r="B57" s="12" t="s">
+      <c r="B57" s="11" t="s">
         <v>72</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -2914,11 +3083,13 @@
       <c r="E57" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F57" s="18">
-        <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G57" s="14"/>
+      <c r="F57" s="17">
+        <f>INT((G57-$K$3)/7)+1</f>
+        <v>11</v>
+      </c>
+      <c r="G57" s="13">
+        <v>40886</v>
+      </c>
       <c r="H57" s="3">
         <v>6</v>
       </c>
@@ -2945,11 +3116,13 @@
       <c r="E58" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F58" s="18">
+      <c r="F58" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G58" s="14"/>
+        <v>12</v>
+      </c>
+      <c r="G58" s="13">
+        <v>40890</v>
+      </c>
       <c r="H58" s="3">
         <v>5</v>
       </c>
@@ -2976,11 +3149,13 @@
       <c r="E59" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F59" s="18">
+      <c r="F59" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G59" s="14"/>
+        <v>10</v>
+      </c>
+      <c r="G59" s="13">
+        <v>40879</v>
+      </c>
       <c r="H59" s="3">
         <v>2</v>
       </c>
@@ -2995,7 +3170,7 @@
       <c r="A60" s="3">
         <v>58</v>
       </c>
-      <c r="B60" s="12" t="s">
+      <c r="B60" s="11" t="s">
         <v>75</v>
       </c>
       <c r="C60" s="4" t="s">
@@ -3007,11 +3182,13 @@
       <c r="E60" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F60" s="18">
+      <c r="F60" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G60" s="14"/>
+        <v>12</v>
+      </c>
+      <c r="G60" s="13">
+        <v>40890</v>
+      </c>
       <c r="H60" s="3">
         <v>3</v>
       </c>
@@ -3026,7 +3203,7 @@
       <c r="A61" s="3">
         <v>59</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="11" t="s">
         <v>76</v>
       </c>
       <c r="C61" s="4" t="s">
@@ -3038,11 +3215,13 @@
       <c r="E61" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F61" s="18">
+      <c r="F61" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G61" s="14"/>
+        <v>10</v>
+      </c>
+      <c r="G61" s="13">
+        <v>40878</v>
+      </c>
       <c r="H61" s="3">
         <v>3</v>
       </c>
@@ -3069,11 +3248,13 @@
       <c r="E62" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F62" s="18">
+      <c r="F62" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G62" s="14"/>
+        <v>12</v>
+      </c>
+      <c r="G62" s="13">
+        <v>40889</v>
+      </c>
       <c r="H62" s="3">
         <v>3</v>
       </c>
@@ -3100,11 +3281,13 @@
       <c r="E63" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F63" s="18">
+      <c r="F63" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G63" s="14"/>
+        <v>12</v>
+      </c>
+      <c r="G63" s="13">
+        <v>40890</v>
+      </c>
       <c r="H63" s="3">
         <v>1</v>
       </c>
@@ -3120,7 +3303,7 @@
         <v>62</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>20</v>
@@ -3131,11 +3314,13 @@
       <c r="E64" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F64" s="18">
+      <c r="F64" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G64" s="14"/>
+        <v>12</v>
+      </c>
+      <c r="G64" s="13">
+        <v>40890</v>
+      </c>
       <c r="H64" s="3">
         <v>3</v>
       </c>
@@ -3162,11 +3347,13 @@
       <c r="E65" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F65" s="18">
+      <c r="F65" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G65" s="14"/>
+        <v>15</v>
+      </c>
+      <c r="G65" s="13">
+        <v>40916</v>
+      </c>
       <c r="H65" s="3">
         <v>1</v>
       </c>
@@ -3193,11 +3380,13 @@
       <c r="E66" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F66" s="18">
+      <c r="F66" s="17">
         <f t="shared" si="0"/>
-        <v>-5830</v>
-      </c>
-      <c r="G66" s="14"/>
+        <v>13</v>
+      </c>
+      <c r="G66" s="13">
+        <v>40896</v>
+      </c>
       <c r="H66" s="3">
         <v>7</v>
       </c>
@@ -3224,11 +3413,13 @@
       <c r="E67" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F67" s="18">
+      <c r="F67" s="17">
         <f t="shared" ref="F67:F120" si="1">INT((G67-$K$3)/7)+1</f>
-        <v>-5830</v>
-      </c>
-      <c r="G67" s="14"/>
+        <v>13</v>
+      </c>
+      <c r="G67" s="13">
+        <v>40896</v>
+      </c>
       <c r="H67" s="3">
         <v>2</v>
       </c>
@@ -3244,7 +3435,7 @@
         <v>66</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>82</v>
+        <v>138</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>9</v>
@@ -3255,17 +3446,17 @@
       <c r="E68" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F68" s="18">
+      <c r="F68" s="17">
         <f t="shared" si="1"/>
-        <v>-5830</v>
-      </c>
-      <c r="G68" s="14"/>
+        <v>17</v>
+      </c>
+      <c r="G68" s="13">
+        <v>40924</v>
+      </c>
       <c r="H68" s="3">
-        <v>12</v>
-      </c>
-      <c r="I68" s="3">
-        <v>9</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="I68" s="3"/>
       <c r="J68" s="4">
         <v>70</v>
       </c>
@@ -3275,7 +3466,7 @@
         <v>67</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>19</v>
@@ -3284,13 +3475,13 @@
         <v>26</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F69" s="18">
+        <v>102</v>
+      </c>
+      <c r="F69" s="17">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G69" s="14">
+      <c r="G69" s="13">
         <v>40816</v>
       </c>
       <c r="H69" s="3"/>
@@ -3306,7 +3497,7 @@
         <v>68</v>
       </c>
       <c r="B70" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C70" s="4" t="s">
         <v>20</v>
@@ -3315,13 +3506,13 @@
         <v>26</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F70" s="18">
+        <v>102</v>
+      </c>
+      <c r="F70" s="17">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="G70" s="14">
+      <c r="G70" s="13">
         <v>40816</v>
       </c>
       <c r="H70" s="3"/>
@@ -3337,7 +3528,7 @@
         <v>69</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C71" s="4" t="s">
         <v>19</v>
@@ -3346,13 +3537,13 @@
         <v>26</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F71" s="18">
+        <v>102</v>
+      </c>
+      <c r="F71" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G71" s="14">
+      <c r="G71" s="13">
         <v>40821</v>
       </c>
       <c r="H71" s="3"/>
@@ -3368,7 +3559,7 @@
         <v>70</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C72" s="4" t="s">
         <v>19</v>
@@ -3377,13 +3568,13 @@
         <v>26</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F72" s="18">
+        <v>102</v>
+      </c>
+      <c r="F72" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G72" s="14">
+      <c r="G72" s="13">
         <v>40821</v>
       </c>
       <c r="H72" s="3"/>
@@ -3399,7 +3590,7 @@
         <v>71</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C73" s="4" t="s">
         <v>20</v>
@@ -3408,13 +3599,13 @@
         <v>26</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F73" s="18">
+        <v>102</v>
+      </c>
+      <c r="F73" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G73" s="14">
+      <c r="G73" s="13">
         <v>40822</v>
       </c>
       <c r="H73" s="3"/>
@@ -3430,7 +3621,7 @@
         <v>72</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C74" s="4" t="s">
         <v>33</v>
@@ -3439,13 +3630,13 @@
         <v>26</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F74" s="18">
+        <v>102</v>
+      </c>
+      <c r="F74" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G74" s="14">
+      <c r="G74" s="13">
         <v>40823</v>
       </c>
       <c r="H74" s="3"/>
@@ -3461,7 +3652,7 @@
         <v>73</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C75" s="4" t="s">
         <v>20</v>
@@ -3470,13 +3661,13 @@
         <v>26</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F75" s="18">
+        <v>102</v>
+      </c>
+      <c r="F75" s="17">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G75" s="14">
+      <c r="G75" s="13">
         <v>40846</v>
       </c>
       <c r="H75" s="3"/>
@@ -3492,7 +3683,7 @@
         <v>74</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C76" s="4" t="s">
         <v>20</v>
@@ -3501,13 +3692,13 @@
         <v>26</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F76" s="18">
+        <v>102</v>
+      </c>
+      <c r="F76" s="17">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G76" s="14">
+      <c r="G76" s="13">
         <v>40847</v>
       </c>
       <c r="H76" s="3"/>
@@ -3523,7 +3714,7 @@
         <v>75</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C77" s="4" t="s">
         <v>19</v>
@@ -3532,13 +3723,13 @@
         <v>26</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F77" s="18">
+        <v>102</v>
+      </c>
+      <c r="F77" s="17">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G77" s="14">
+      <c r="G77" s="13">
         <v>40848</v>
       </c>
       <c r="H77" s="3"/>
@@ -3554,7 +3745,7 @@
         <v>76</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C78" s="4" t="s">
         <v>19</v>
@@ -3563,13 +3754,13 @@
         <v>26</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F78" s="18">
+        <v>102</v>
+      </c>
+      <c r="F78" s="17">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G78" s="14">
+      <c r="G78" s="13">
         <v>40851</v>
       </c>
       <c r="H78" s="3"/>
@@ -3585,7 +3776,7 @@
         <v>77</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C79" s="4" t="s">
         <v>20</v>
@@ -3594,13 +3785,13 @@
         <v>26</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F79" s="18">
+        <v>102</v>
+      </c>
+      <c r="F79" s="17">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G79" s="14">
+      <c r="G79" s="13">
         <v>40854</v>
       </c>
       <c r="H79" s="3"/>
@@ -3616,7 +3807,7 @@
         <v>78</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C80" s="4" t="s">
         <v>19</v>
@@ -3625,13 +3816,13 @@
         <v>26</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F80" s="18">
+        <v>102</v>
+      </c>
+      <c r="F80" s="17">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G80" s="14">
+      <c r="G80" s="13">
         <v>40855</v>
       </c>
       <c r="H80" s="3"/>
@@ -3647,7 +3838,7 @@
         <v>79</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C81" s="4" t="s">
         <v>20</v>
@@ -3656,13 +3847,13 @@
         <v>26</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F81" s="18">
+        <v>102</v>
+      </c>
+      <c r="F81" s="17">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G81" s="14">
+      <c r="G81" s="13">
         <v>40862</v>
       </c>
       <c r="H81" s="3"/>
@@ -3678,7 +3869,7 @@
         <v>80</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C82" s="4" t="s">
         <v>20</v>
@@ -3687,13 +3878,13 @@
         <v>26</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F82" s="18">
+        <v>102</v>
+      </c>
+      <c r="F82" s="17">
         <f t="shared" si="1"/>
         <v>9</v>
       </c>
-      <c r="G82" s="14">
+      <c r="G82" s="13">
         <v>40871</v>
       </c>
       <c r="H82" s="3"/>
@@ -3709,7 +3900,7 @@
         <v>81</v>
       </c>
       <c r="B83" s="4" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C83" s="4" t="s">
         <v>20</v>
@@ -3718,13 +3909,13 @@
         <v>26</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F83" s="18">
+        <v>102</v>
+      </c>
+      <c r="F83" s="17">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="G83" s="14">
+      <c r="G83" s="13">
         <v>40882</v>
       </c>
       <c r="H83" s="3"/>
@@ -3740,7 +3931,7 @@
         <v>82</v>
       </c>
       <c r="B84" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C84" s="4" t="s">
         <v>20</v>
@@ -3749,13 +3940,13 @@
         <v>26</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F84" s="18">
+        <v>102</v>
+      </c>
+      <c r="F84" s="17">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="G84" s="14">
+      <c r="G84" s="13">
         <v>40888</v>
       </c>
       <c r="H84" s="3"/>
@@ -3771,7 +3962,7 @@
         <v>83</v>
       </c>
       <c r="B85" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C85" s="4" t="s">
         <v>19</v>
@@ -3780,13 +3971,13 @@
         <v>26</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F85" s="18">
+        <v>102</v>
+      </c>
+      <c r="F85" s="17">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="G85" s="14">
+      <c r="G85" s="13">
         <v>40895</v>
       </c>
       <c r="H85" s="3"/>
@@ -3802,7 +3993,7 @@
         <v>84</v>
       </c>
       <c r="B86" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C86" s="4" t="s">
         <v>19</v>
@@ -3811,13 +4002,13 @@
         <v>26</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F86" s="18">
+        <v>102</v>
+      </c>
+      <c r="F86" s="17">
         <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="G86" s="14">
+      <c r="G86" s="13">
         <v>40941</v>
       </c>
       <c r="H86" s="3"/>
@@ -3833,7 +4024,7 @@
         <v>85</v>
       </c>
       <c r="B87" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C87" s="4" t="s">
         <v>19</v>
@@ -3842,13 +4033,13 @@
         <v>26</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="F87" s="18">
+        <v>102</v>
+      </c>
+      <c r="F87" s="17">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G87" s="14">
+      <c r="G87" s="13">
         <v>40879</v>
       </c>
       <c r="H87" s="3"/>
@@ -3864,7 +4055,7 @@
         <v>86</v>
       </c>
       <c r="B88" s="4" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C88" s="4" t="s">
         <v>19</v>
@@ -3873,13 +4064,13 @@
         <v>26</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F88" s="18">
+        <v>115</v>
+      </c>
+      <c r="F88" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G88" s="14">
+      <c r="G88" s="13">
         <v>40819</v>
       </c>
       <c r="H88" s="3"/>
@@ -3895,7 +4086,7 @@
         <v>87</v>
       </c>
       <c r="B89" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C89" s="4" t="s">
         <v>20</v>
@@ -3904,13 +4095,13 @@
         <v>26</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F89" s="18">
+        <v>115</v>
+      </c>
+      <c r="F89" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G89" s="14">
+      <c r="G89" s="13">
         <v>40820</v>
       </c>
       <c r="H89" s="3"/>
@@ -3926,7 +4117,7 @@
         <v>88</v>
       </c>
       <c r="B90" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C90" s="4" t="s">
         <v>33</v>
@@ -3935,13 +4126,13 @@
         <v>26</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F90" s="18">
+        <v>115</v>
+      </c>
+      <c r="F90" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G90" s="14">
+      <c r="G90" s="13">
         <v>40822</v>
       </c>
       <c r="H90" s="3"/>
@@ -3957,7 +4148,7 @@
         <v>89</v>
       </c>
       <c r="B91" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>20</v>
@@ -3966,13 +4157,13 @@
         <v>30</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F91" s="18">
+        <v>115</v>
+      </c>
+      <c r="F91" s="17">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G91" s="14">
+      <c r="G91" s="13">
         <v>40830</v>
       </c>
       <c r="H91" s="3"/>
@@ -3988,7 +4179,7 @@
         <v>90</v>
       </c>
       <c r="B92" s="4" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C92" s="4" t="s">
         <v>19</v>
@@ -3997,13 +4188,13 @@
         <v>26</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F92" s="18">
+        <v>115</v>
+      </c>
+      <c r="F92" s="17">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="G92" s="14">
+      <c r="G92" s="13">
         <v>40823</v>
       </c>
       <c r="H92" s="3"/>
@@ -4019,7 +4210,7 @@
         <v>91</v>
       </c>
       <c r="B93" s="4" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C93" s="4" t="s">
         <v>9</v>
@@ -4028,13 +4219,13 @@
         <v>30</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F93" s="18">
+        <v>115</v>
+      </c>
+      <c r="F93" s="17">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G93" s="14">
+      <c r="G93" s="13">
         <v>40855</v>
       </c>
       <c r="H93" s="3"/>
@@ -4050,7 +4241,7 @@
         <v>92</v>
       </c>
       <c r="B94" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C94" s="4" t="s">
         <v>20</v>
@@ -4059,13 +4250,13 @@
         <v>30</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F94" s="18">
+        <v>115</v>
+      </c>
+      <c r="F94" s="17">
         <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="G94" s="14">
+      <c r="G94" s="13">
         <v>40827</v>
       </c>
       <c r="H94" s="3"/>
@@ -4081,7 +4272,7 @@
         <v>93</v>
       </c>
       <c r="B95" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C95" s="4" t="s">
         <v>9</v>
@@ -4090,13 +4281,13 @@
         <v>30</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F95" s="18">
+        <v>115</v>
+      </c>
+      <c r="F95" s="17">
         <f t="shared" si="1"/>
         <v>4</v>
       </c>
-      <c r="G95" s="14">
+      <c r="G95" s="13">
         <v>40836</v>
       </c>
       <c r="H95" s="3"/>
@@ -4112,7 +4303,7 @@
         <v>94</v>
       </c>
       <c r="B96" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C96" s="4" t="s">
         <v>20</v>
@@ -4121,13 +4312,13 @@
         <v>30</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F96" s="18">
+        <v>115</v>
+      </c>
+      <c r="F96" s="17">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G96" s="14">
+      <c r="G96" s="13">
         <v>40842</v>
       </c>
       <c r="H96" s="3"/>
@@ -4152,13 +4343,13 @@
         <v>26</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F97" s="18">
+        <v>115</v>
+      </c>
+      <c r="F97" s="17">
         <f t="shared" si="1"/>
         <v>5</v>
       </c>
-      <c r="G97" s="14">
+      <c r="G97" s="13">
         <v>40845</v>
       </c>
       <c r="H97" s="3"/>
@@ -4183,13 +4374,13 @@
         <v>26</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F98" s="18">
+        <v>115</v>
+      </c>
+      <c r="F98" s="17">
         <f t="shared" si="1"/>
         <v>6</v>
       </c>
-      <c r="G98" s="14">
+      <c r="G98" s="13">
         <v>40847</v>
       </c>
       <c r="H98" s="3"/>
@@ -4214,13 +4405,13 @@
         <v>26</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F99" s="18">
+        <v>115</v>
+      </c>
+      <c r="F99" s="17">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G99" s="14">
+      <c r="G99" s="13">
         <v>40876</v>
       </c>
       <c r="H99" s="3"/>
@@ -4236,7 +4427,7 @@
         <v>98</v>
       </c>
       <c r="B100" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C100" s="4" t="s">
         <v>19</v>
@@ -4245,13 +4436,13 @@
         <v>30</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F100" s="18">
+        <v>115</v>
+      </c>
+      <c r="F100" s="17">
         <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="G100" s="14">
+      <c r="G100" s="13">
         <v>40864</v>
       </c>
       <c r="H100" s="3"/>
@@ -4267,7 +4458,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C101" s="4" t="s">
         <v>19</v>
@@ -4276,13 +4467,13 @@
         <v>30</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F101" s="18">
+        <v>115</v>
+      </c>
+      <c r="F101" s="17">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="G101" s="14">
+      <c r="G101" s="13">
         <v>40879</v>
       </c>
       <c r="H101" s="3"/>
@@ -4298,7 +4489,7 @@
         <v>100</v>
       </c>
       <c r="B102" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C102" s="4" t="s">
         <v>20</v>
@@ -4307,13 +4498,13 @@
         <v>30</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F102" s="18">
+        <v>115</v>
+      </c>
+      <c r="F102" s="17">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="G102" s="14">
+      <c r="G102" s="13">
         <v>40899</v>
       </c>
       <c r="H102" s="3"/>
@@ -4329,7 +4520,7 @@
         <v>101</v>
       </c>
       <c r="B103" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C103" s="4" t="s">
         <v>19</v>
@@ -4338,13 +4529,13 @@
         <v>30</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="F103" s="18">
+        <v>115</v>
+      </c>
+      <c r="F103" s="17">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="G103" s="14">
+      <c r="G103" s="13">
         <v>40894</v>
       </c>
       <c r="H103" s="3"/>
@@ -4360,7 +4551,7 @@
         <v>102</v>
       </c>
       <c r="B104" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C104" s="4" t="s">
         <v>20</v>
@@ -4369,13 +4560,13 @@
         <v>26</v>
       </c>
       <c r="E104" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F104" s="18">
+        <v>117</v>
+      </c>
+      <c r="F104" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G104" s="16"/>
+      <c r="G104" s="15"/>
       <c r="H104" s="3">
         <v>15</v>
       </c>
@@ -4391,7 +4582,7 @@
         <v>103</v>
       </c>
       <c r="B105" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C105" s="4" t="s">
         <v>9</v>
@@ -4400,13 +4591,13 @@
         <v>26</v>
       </c>
       <c r="E105" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F105" s="18">
+        <v>117</v>
+      </c>
+      <c r="F105" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G105" s="16"/>
+      <c r="G105" s="15"/>
       <c r="H105" s="3">
         <v>5</v>
       </c>
@@ -4422,7 +4613,7 @@
         <v>104</v>
       </c>
       <c r="B106" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C106" s="4" t="s">
         <v>20</v>
@@ -4431,13 +4622,13 @@
         <v>26</v>
       </c>
       <c r="E106" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F106" s="18">
+        <v>117</v>
+      </c>
+      <c r="F106" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G106" s="16"/>
+      <c r="G106" s="15"/>
       <c r="H106" s="3">
         <v>6</v>
       </c>
@@ -4453,7 +4644,7 @@
         <v>105</v>
       </c>
       <c r="B107" s="4" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C107" s="4" t="s">
         <v>19</v>
@@ -4462,13 +4653,13 @@
         <v>26</v>
       </c>
       <c r="E107" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F107" s="18">
+        <v>117</v>
+      </c>
+      <c r="F107" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G107" s="16"/>
+      <c r="G107" s="15"/>
       <c r="H107" s="3">
         <v>10</v>
       </c>
@@ -4484,7 +4675,7 @@
         <v>106</v>
       </c>
       <c r="B108" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C108" s="4" t="s">
         <v>19</v>
@@ -4493,13 +4684,13 @@
         <v>26</v>
       </c>
       <c r="E108" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F108" s="18">
+        <v>117</v>
+      </c>
+      <c r="F108" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G108" s="16"/>
+      <c r="G108" s="15"/>
       <c r="H108" s="3">
         <v>2</v>
       </c>
@@ -4515,7 +4706,7 @@
         <v>107</v>
       </c>
       <c r="B109" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C109" s="4" t="s">
         <v>20</v>
@@ -4524,13 +4715,13 @@
         <v>26</v>
       </c>
       <c r="E109" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F109" s="18">
+        <v>117</v>
+      </c>
+      <c r="F109" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G109" s="16"/>
+      <c r="G109" s="15"/>
       <c r="H109" s="3">
         <v>2</v>
       </c>
@@ -4546,7 +4737,7 @@
         <v>108</v>
       </c>
       <c r="B110" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C110" s="4" t="s">
         <v>20</v>
@@ -4555,13 +4746,13 @@
         <v>26</v>
       </c>
       <c r="E110" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F110" s="18">
+        <v>117</v>
+      </c>
+      <c r="F110" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G110" s="16"/>
+      <c r="G110" s="15"/>
       <c r="H110" s="3">
         <v>8</v>
       </c>
@@ -4577,7 +4768,7 @@
         <v>109</v>
       </c>
       <c r="B111" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C111" s="4" t="s">
         <v>20</v>
@@ -4586,13 +4777,13 @@
         <v>26</v>
       </c>
       <c r="E111" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F111" s="18">
+        <v>117</v>
+      </c>
+      <c r="F111" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G111" s="16"/>
+      <c r="G111" s="15"/>
       <c r="H111" s="3">
         <v>5</v>
       </c>
@@ -4608,7 +4799,7 @@
         <v>110</v>
       </c>
       <c r="B112" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C112" s="4" t="s">
         <v>20</v>
@@ -4617,13 +4808,13 @@
         <v>26</v>
       </c>
       <c r="E112" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F112" s="18">
+        <v>117</v>
+      </c>
+      <c r="F112" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G112" s="16"/>
+      <c r="G112" s="15"/>
       <c r="H112" s="3"/>
       <c r="I112" s="3">
         <v>3</v>
@@ -4637,7 +4828,7 @@
         <v>111</v>
       </c>
       <c r="B113" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C113" s="4" t="s">
         <v>9</v>
@@ -4646,13 +4837,13 @@
         <v>26</v>
       </c>
       <c r="E113" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F113" s="18">
+        <v>117</v>
+      </c>
+      <c r="F113" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G113" s="16"/>
+      <c r="G113" s="15"/>
       <c r="H113" s="3"/>
       <c r="I113" s="3">
         <v>18</v>
@@ -4666,7 +4857,7 @@
         <v>112</v>
       </c>
       <c r="B114" s="4" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C114" s="4" t="s">
         <v>19</v>
@@ -4675,13 +4866,13 @@
         <v>26</v>
       </c>
       <c r="E114" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F114" s="18">
+        <v>117</v>
+      </c>
+      <c r="F114" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G114" s="16"/>
+      <c r="G114" s="15"/>
       <c r="H114" s="3"/>
       <c r="I114" s="3">
         <v>3</v>
@@ -4695,7 +4886,7 @@
         <v>113</v>
       </c>
       <c r="B115" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C115" s="4" t="s">
         <v>20</v>
@@ -4704,13 +4895,13 @@
         <v>26</v>
       </c>
       <c r="E115" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F115" s="18">
+        <v>117</v>
+      </c>
+      <c r="F115" s="17">
         <f t="shared" si="1"/>
         <v>7</v>
       </c>
-      <c r="G115" s="16">
+      <c r="G115" s="15">
         <v>40855</v>
       </c>
       <c r="H115" s="3"/>
@@ -4726,7 +4917,7 @@
         <v>114</v>
       </c>
       <c r="B116" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C116" s="4" t="s">
         <v>20</v>
@@ -4735,13 +4926,13 @@
         <v>26</v>
       </c>
       <c r="E116" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F116" s="18">
+        <v>117</v>
+      </c>
+      <c r="F116" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G116" s="16"/>
+      <c r="G116" s="15"/>
       <c r="H116" s="3"/>
       <c r="I116" s="3">
         <v>3</v>
@@ -4755,7 +4946,7 @@
         <v>115</v>
       </c>
       <c r="B117" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C117" s="4" t="s">
         <v>20</v>
@@ -4764,13 +4955,13 @@
         <v>26</v>
       </c>
       <c r="E117" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F117" s="18">
+        <v>117</v>
+      </c>
+      <c r="F117" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G117" s="16"/>
+      <c r="G117" s="15"/>
       <c r="H117" s="3"/>
       <c r="I117" s="3">
         <v>2</v>
@@ -4784,7 +4975,7 @@
         <v>116</v>
       </c>
       <c r="B118" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C118" s="4" t="s">
         <v>20</v>
@@ -4793,13 +4984,13 @@
         <v>26</v>
       </c>
       <c r="E118" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F118" s="18">
+        <v>117</v>
+      </c>
+      <c r="F118" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G118" s="16"/>
+      <c r="G118" s="15"/>
       <c r="H118" s="3"/>
       <c r="I118" s="3">
         <v>2.5</v>
@@ -4813,7 +5004,7 @@
         <v>117</v>
       </c>
       <c r="B119" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C119" s="4" t="s">
         <v>20</v>
@@ -4822,13 +5013,13 @@
         <v>26</v>
       </c>
       <c r="E119" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F119" s="18">
+        <v>117</v>
+      </c>
+      <c r="F119" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G119" s="16"/>
+      <c r="G119" s="15"/>
       <c r="H119" s="3"/>
       <c r="I119" s="3">
         <v>4</v>
@@ -4842,7 +5033,7 @@
         <v>118</v>
       </c>
       <c r="B120" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C120" s="4" t="s">
         <v>9</v>
@@ -4851,13 +5042,13 @@
         <v>26</v>
       </c>
       <c r="E120" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="F120" s="18">
+        <v>117</v>
+      </c>
+      <c r="F120" s="17">
         <f t="shared" si="1"/>
         <v>-5830</v>
       </c>
-      <c r="G120" s="14"/>
+      <c r="G120" s="13"/>
       <c r="H120" s="3">
         <v>20</v>
       </c>
@@ -4877,7 +5068,7 @@
       <c r="D121" s="4"/>
       <c r="E121" s="4"/>
       <c r="F121" s="4"/>
-      <c r="G121" s="14"/>
+      <c r="G121" s="13"/>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
       <c r="J121" s="4"/>
@@ -4891,7 +5082,7 @@
       <c r="D122" s="4"/>
       <c r="E122" s="4"/>
       <c r="F122" s="4"/>
-      <c r="G122" s="14"/>
+      <c r="G122" s="13"/>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
       <c r="J122" s="4"/>
@@ -4905,7 +5096,7 @@
       <c r="D123" s="4"/>
       <c r="E123" s="4"/>
       <c r="F123" s="4"/>
-      <c r="G123" s="14"/>
+      <c r="G123" s="13"/>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
       <c r="J123" s="4"/>
@@ -4919,7 +5110,7 @@
       <c r="D124" s="4"/>
       <c r="E124" s="4"/>
       <c r="F124" s="4"/>
-      <c r="G124" s="14"/>
+      <c r="G124" s="13"/>
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
       <c r="J124" s="4"/>
@@ -4933,7 +5124,7 @@
       <c r="D125" s="4"/>
       <c r="E125" s="4"/>
       <c r="F125" s="4"/>
-      <c r="G125" s="14"/>
+      <c r="G125" s="13"/>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
       <c r="J125" s="4"/>
@@ -4947,7 +5138,7 @@
       <c r="D126" s="4"/>
       <c r="E126" s="4"/>
       <c r="F126" s="4"/>
-      <c r="G126" s="14"/>
+      <c r="G126" s="13"/>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
       <c r="J126" s="4"/>
@@ -4961,7 +5152,7 @@
       <c r="D127" s="4"/>
       <c r="E127" s="4"/>
       <c r="F127" s="4"/>
-      <c r="G127" s="14"/>
+      <c r="G127" s="13"/>
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
       <c r="J127" s="4"/>
@@ -4975,7 +5166,7 @@
       <c r="D128" s="4"/>
       <c r="E128" s="4"/>
       <c r="F128" s="4"/>
-      <c r="G128" s="14"/>
+      <c r="G128" s="13"/>
       <c r="H128" s="4"/>
       <c r="I128" s="4"/>
       <c r="J128" s="4"/>
@@ -4989,7 +5180,7 @@
       <c r="D129" s="4"/>
       <c r="E129" s="4"/>
       <c r="F129" s="4"/>
-      <c r="G129" s="14"/>
+      <c r="G129" s="13"/>
       <c r="H129" s="4"/>
       <c r="I129" s="4"/>
       <c r="J129" s="4"/>
@@ -5003,7 +5194,7 @@
       <c r="D130" s="4"/>
       <c r="E130" s="4"/>
       <c r="F130" s="4"/>
-      <c r="G130" s="14"/>
+      <c r="G130" s="13"/>
       <c r="H130" s="4"/>
       <c r="I130" s="4"/>
       <c r="J130" s="4"/>
@@ -5017,7 +5208,7 @@
       <c r="D131" s="4"/>
       <c r="E131" s="4"/>
       <c r="F131" s="4"/>
-      <c r="G131" s="14"/>
+      <c r="G131" s="13"/>
       <c r="H131" s="4"/>
       <c r="I131" s="4"/>
       <c r="J131" s="4"/>
@@ -5031,7 +5222,7 @@
       <c r="D132" s="4"/>
       <c r="E132" s="4"/>
       <c r="F132" s="4"/>
-      <c r="G132" s="14"/>
+      <c r="G132" s="13"/>
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
       <c r="J132" s="4"/>
@@ -5045,7 +5236,7 @@
       <c r="D133" s="4"/>
       <c r="E133" s="4"/>
       <c r="F133" s="4"/>
-      <c r="G133" s="14"/>
+      <c r="G133" s="13"/>
       <c r="H133" s="4"/>
       <c r="I133" s="4"/>
       <c r="J133" s="4"/>
@@ -5059,7 +5250,7 @@
       <c r="D134" s="4"/>
       <c r="E134" s="4"/>
       <c r="F134" s="4"/>
-      <c r="G134" s="14"/>
+      <c r="G134" s="13"/>
       <c r="H134" s="4"/>
       <c r="I134" s="4"/>
       <c r="J134" s="4"/>
@@ -5073,7 +5264,7 @@
       <c r="D135" s="4"/>
       <c r="E135" s="4"/>
       <c r="F135" s="4"/>
-      <c r="G135" s="14"/>
+      <c r="G135" s="13"/>
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
       <c r="J135" s="4"/>
@@ -5087,7 +5278,7 @@
       <c r="D136" s="4"/>
       <c r="E136" s="4"/>
       <c r="F136" s="4"/>
-      <c r="G136" s="14"/>
+      <c r="G136" s="13"/>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
       <c r="J136" s="4"/>
@@ -5101,7 +5292,7 @@
       <c r="D137" s="4"/>
       <c r="E137" s="4"/>
       <c r="F137" s="4"/>
-      <c r="G137" s="14"/>
+      <c r="G137" s="13"/>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
       <c r="J137" s="4"/>
@@ -5115,7 +5306,7 @@
       <c r="D138" s="4"/>
       <c r="E138" s="4"/>
       <c r="F138" s="4"/>
-      <c r="G138" s="14"/>
+      <c r="G138" s="13"/>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
       <c r="J138" s="4"/>
@@ -5129,7 +5320,7 @@
       <c r="D139" s="4"/>
       <c r="E139" s="4"/>
       <c r="F139" s="4"/>
-      <c r="G139" s="14"/>
+      <c r="G139" s="13"/>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
       <c r="J139" s="4"/>
@@ -5143,7 +5334,7 @@
       <c r="D140" s="4"/>
       <c r="E140" s="4"/>
       <c r="F140" s="4"/>
-      <c r="G140" s="14"/>
+      <c r="G140" s="13"/>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
       <c r="J140" s="4"/>
@@ -5157,7 +5348,7 @@
       <c r="D141" s="4"/>
       <c r="E141" s="4"/>
       <c r="F141" s="4"/>
-      <c r="G141" s="14"/>
+      <c r="G141" s="13"/>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
       <c r="J141" s="4"/>
@@ -5171,7 +5362,7 @@
       <c r="D142" s="4"/>
       <c r="E142" s="4"/>
       <c r="F142" s="4"/>
-      <c r="G142" s="14"/>
+      <c r="G142" s="13"/>
       <c r="H142" s="4"/>
       <c r="I142" s="4"/>
       <c r="J142" s="4"/>
@@ -5185,7 +5376,7 @@
       <c r="D143" s="4"/>
       <c r="E143" s="4"/>
       <c r="F143" s="4"/>
-      <c r="G143" s="14"/>
+      <c r="G143" s="13"/>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
       <c r="J143" s="4"/>
@@ -5199,7 +5390,7 @@
       <c r="D144" s="4"/>
       <c r="E144" s="4"/>
       <c r="F144" s="4"/>
-      <c r="G144" s="14"/>
+      <c r="G144" s="13"/>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
       <c r="J144" s="4"/>
@@ -5213,7 +5404,7 @@
       <c r="D145" s="4"/>
       <c r="E145" s="4"/>
       <c r="F145" s="4"/>
-      <c r="G145" s="14"/>
+      <c r="G145" s="13"/>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
       <c r="J145" s="4"/>
@@ -5227,7 +5418,7 @@
       <c r="D146" s="4"/>
       <c r="E146" s="4"/>
       <c r="F146" s="4"/>
-      <c r="G146" s="14"/>
+      <c r="G146" s="13"/>
       <c r="H146" s="4"/>
       <c r="I146" s="4"/>
       <c r="J146" s="4"/>
@@ -5241,7 +5432,7 @@
       <c r="D147" s="4"/>
       <c r="E147" s="4"/>
       <c r="F147" s="4"/>
-      <c r="G147" s="14"/>
+      <c r="G147" s="13"/>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
       <c r="J147" s="4"/>
@@ -5255,7 +5446,7 @@
       <c r="D148" s="4"/>
       <c r="E148" s="4"/>
       <c r="F148" s="4"/>
-      <c r="G148" s="14"/>
+      <c r="G148" s="13"/>
       <c r="H148" s="4"/>
       <c r="I148" s="4"/>
       <c r="J148" s="4"/>
@@ -5269,7 +5460,7 @@
       <c r="D149" s="4"/>
       <c r="E149" s="4"/>
       <c r="F149" s="4"/>
-      <c r="G149" s="14"/>
+      <c r="G149" s="13"/>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
       <c r="J149" s="4"/>
@@ -5283,7 +5474,7 @@
       <c r="D150" s="4"/>
       <c r="E150" s="4"/>
       <c r="F150" s="4"/>
-      <c r="G150" s="14"/>
+      <c r="G150" s="13"/>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
       <c r="J150" s="4"/>
@@ -5297,7 +5488,7 @@
       <c r="D151" s="4"/>
       <c r="E151" s="4"/>
       <c r="F151" s="4"/>
-      <c r="G151" s="14"/>
+      <c r="G151" s="13"/>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
       <c r="J151" s="4"/>
@@ -5311,7 +5502,7 @@
       <c r="D152" s="4"/>
       <c r="E152" s="4"/>
       <c r="F152" s="4"/>
-      <c r="G152" s="14"/>
+      <c r="G152" s="13"/>
       <c r="H152" s="4"/>
       <c r="I152" s="4"/>
       <c r="J152" s="4"/>
@@ -5325,7 +5516,7 @@
       <c r="D153" s="4"/>
       <c r="E153" s="4"/>
       <c r="F153" s="4"/>
-      <c r="G153" s="14"/>
+      <c r="G153" s="13"/>
       <c r="H153" s="4"/>
       <c r="I153" s="4"/>
       <c r="J153" s="4"/>
@@ -5339,7 +5530,7 @@
       <c r="D154" s="4"/>
       <c r="E154" s="4"/>
       <c r="F154" s="4"/>
-      <c r="G154" s="14"/>
+      <c r="G154" s="13"/>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
       <c r="J154" s="4"/>
@@ -5353,7 +5544,7 @@
       <c r="D155" s="4"/>
       <c r="E155" s="4"/>
       <c r="F155" s="4"/>
-      <c r="G155" s="14"/>
+      <c r="G155" s="13"/>
       <c r="H155" s="4"/>
       <c r="I155" s="4"/>
       <c r="J155" s="4"/>
@@ -5367,7 +5558,7 @@
       <c r="D156" s="4"/>
       <c r="E156" s="4"/>
       <c r="F156" s="4"/>
-      <c r="G156" s="14"/>
+      <c r="G156" s="13"/>
       <c r="H156" s="4"/>
       <c r="I156" s="4"/>
       <c r="J156" s="4"/>
@@ -5381,7 +5572,7 @@
       <c r="D157" s="4"/>
       <c r="E157" s="4"/>
       <c r="F157" s="4"/>
-      <c r="G157" s="14"/>
+      <c r="G157" s="13"/>
       <c r="H157" s="4"/>
       <c r="I157" s="4"/>
       <c r="J157" s="4"/>
@@ -5395,7 +5586,7 @@
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
       <c r="F158" s="4"/>
-      <c r="G158" s="14"/>
+      <c r="G158" s="13"/>
       <c r="H158" s="4"/>
       <c r="I158" s="4"/>
       <c r="J158" s="4"/>
@@ -5409,7 +5600,7 @@
       <c r="D159" s="4"/>
       <c r="E159" s="4"/>
       <c r="F159" s="4"/>
-      <c r="G159" s="14"/>
+      <c r="G159" s="13"/>
       <c r="H159" s="4"/>
       <c r="I159" s="4"/>
       <c r="J159" s="4"/>
@@ -5423,7 +5614,7 @@
       <c r="D160" s="4"/>
       <c r="E160" s="4"/>
       <c r="F160" s="4"/>
-      <c r="G160" s="14"/>
+      <c r="G160" s="13"/>
       <c r="H160" s="4"/>
       <c r="I160" s="4"/>
       <c r="J160" s="4"/>
@@ -5437,7 +5628,7 @@
       <c r="D161" s="4"/>
       <c r="E161" s="4"/>
       <c r="F161" s="4"/>
-      <c r="G161" s="14"/>
+      <c r="G161" s="13"/>
       <c r="H161" s="4"/>
       <c r="I161" s="4"/>
       <c r="J161" s="4"/>
@@ -5451,7 +5642,7 @@
       <c r="D162" s="4"/>
       <c r="E162" s="4"/>
       <c r="F162" s="4"/>
-      <c r="G162" s="14"/>
+      <c r="G162" s="13"/>
       <c r="H162" s="4"/>
       <c r="I162" s="4"/>
       <c r="J162" s="4"/>
@@ -5465,7 +5656,7 @@
       <c r="D163" s="4"/>
       <c r="E163" s="4"/>
       <c r="F163" s="4"/>
-      <c r="G163" s="14"/>
+      <c r="G163" s="13"/>
       <c r="H163" s="4"/>
       <c r="I163" s="4"/>
       <c r="J163" s="4"/>
@@ -5479,7 +5670,7 @@
       <c r="D164" s="4"/>
       <c r="E164" s="4"/>
       <c r="F164" s="4"/>
-      <c r="G164" s="14"/>
+      <c r="G164" s="13"/>
       <c r="H164" s="4"/>
       <c r="I164" s="4"/>
       <c r="J164" s="4"/>
@@ -5493,7 +5684,7 @@
       <c r="D165" s="4"/>
       <c r="E165" s="4"/>
       <c r="F165" s="4"/>
-      <c r="G165" s="14"/>
+      <c r="G165" s="13"/>
       <c r="H165" s="4"/>
       <c r="I165" s="4"/>
       <c r="J165" s="4"/>
@@ -5507,7 +5698,7 @@
       <c r="D166" s="4"/>
       <c r="E166" s="4"/>
       <c r="F166" s="4"/>
-      <c r="G166" s="14"/>
+      <c r="G166" s="13"/>
       <c r="H166" s="4"/>
       <c r="I166" s="4"/>
       <c r="J166" s="4"/>
@@ -5521,7 +5712,7 @@
       <c r="D167" s="4"/>
       <c r="E167" s="4"/>
       <c r="F167" s="4"/>
-      <c r="G167" s="14"/>
+      <c r="G167" s="13"/>
       <c r="H167" s="4"/>
       <c r="I167" s="4"/>
       <c r="J167" s="4"/>
@@ -5535,7 +5726,7 @@
       <c r="D168" s="4"/>
       <c r="E168" s="4"/>
       <c r="F168" s="4"/>
-      <c r="G168" s="14"/>
+      <c r="G168" s="13"/>
       <c r="H168" s="4"/>
       <c r="I168" s="4"/>
       <c r="J168" s="4"/>
@@ -5549,7 +5740,7 @@
       <c r="D169" s="4"/>
       <c r="E169" s="4"/>
       <c r="F169" s="4"/>
-      <c r="G169" s="14"/>
+      <c r="G169" s="13"/>
       <c r="H169" s="4"/>
       <c r="I169" s="4"/>
       <c r="J169" s="4"/>
@@ -5563,7 +5754,7 @@
       <c r="D170" s="4"/>
       <c r="E170" s="4"/>
       <c r="F170" s="4"/>
-      <c r="G170" s="14"/>
+      <c r="G170" s="13"/>
       <c r="H170" s="4"/>
       <c r="I170" s="4"/>
       <c r="J170" s="4"/>
@@ -5577,7 +5768,7 @@
       <c r="D171" s="4"/>
       <c r="E171" s="4"/>
       <c r="F171" s="4"/>
-      <c r="G171" s="14"/>
+      <c r="G171" s="13"/>
       <c r="H171" s="4"/>
       <c r="I171" s="4"/>
       <c r="J171" s="4"/>
@@ -5591,7 +5782,7 @@
       <c r="D172" s="4"/>
       <c r="E172" s="4"/>
       <c r="F172" s="4"/>
-      <c r="G172" s="14"/>
+      <c r="G172" s="13"/>
       <c r="H172" s="4"/>
       <c r="I172" s="4"/>
       <c r="J172" s="4"/>
@@ -5605,7 +5796,7 @@
       <c r="D173" s="4"/>
       <c r="E173" s="4"/>
       <c r="F173" s="4"/>
-      <c r="G173" s="14"/>
+      <c r="G173" s="13"/>
       <c r="H173" s="4"/>
       <c r="I173" s="4"/>
       <c r="J173" s="4"/>
@@ -5619,7 +5810,7 @@
       <c r="D174" s="4"/>
       <c r="E174" s="4"/>
       <c r="F174" s="4"/>
-      <c r="G174" s="14"/>
+      <c r="G174" s="13"/>
       <c r="H174" s="4"/>
       <c r="I174" s="4"/>
       <c r="J174" s="4"/>
@@ -5633,7 +5824,7 @@
       <c r="D175" s="4"/>
       <c r="E175" s="4"/>
       <c r="F175" s="4"/>
-      <c r="G175" s="14"/>
+      <c r="G175" s="13"/>
       <c r="H175" s="4"/>
       <c r="I175" s="4"/>
       <c r="J175" s="4"/>
@@ -5647,7 +5838,7 @@
       <c r="D176" s="4"/>
       <c r="E176" s="4"/>
       <c r="F176" s="4"/>
-      <c r="G176" s="14"/>
+      <c r="G176" s="13"/>
       <c r="H176" s="4"/>
       <c r="I176" s="4"/>
       <c r="J176" s="4"/>
@@ -5661,7 +5852,7 @@
       <c r="D177" s="4"/>
       <c r="E177" s="4"/>
       <c r="F177" s="4"/>
-      <c r="G177" s="14"/>
+      <c r="G177" s="13"/>
       <c r="H177" s="4"/>
       <c r="I177" s="4"/>
       <c r="J177" s="4"/>
@@ -5675,7 +5866,7 @@
       <c r="D178" s="4"/>
       <c r="E178" s="4"/>
       <c r="F178" s="4"/>
-      <c r="G178" s="14"/>
+      <c r="G178" s="13"/>
       <c r="H178" s="4"/>
       <c r="I178" s="4"/>
       <c r="J178" s="4"/>
@@ -5689,7 +5880,7 @@
       <c r="D179" s="4"/>
       <c r="E179" s="4"/>
       <c r="F179" s="4"/>
-      <c r="G179" s="14"/>
+      <c r="G179" s="13"/>
       <c r="H179" s="4"/>
       <c r="I179" s="4"/>
       <c r="J179" s="4"/>
@@ -5703,7 +5894,7 @@
       <c r="D180" s="4"/>
       <c r="E180" s="4"/>
       <c r="F180" s="4"/>
-      <c r="G180" s="14"/>
+      <c r="G180" s="13"/>
       <c r="H180" s="4"/>
       <c r="I180" s="4"/>
       <c r="J180" s="4"/>
@@ -5717,7 +5908,7 @@
       <c r="D181" s="4"/>
       <c r="E181" s="4"/>
       <c r="F181" s="4"/>
-      <c r="G181" s="14"/>
+      <c r="G181" s="13"/>
       <c r="H181" s="4"/>
       <c r="I181" s="4"/>
       <c r="J181" s="4"/>
@@ -5731,7 +5922,7 @@
       <c r="D182" s="4"/>
       <c r="E182" s="4"/>
       <c r="F182" s="4"/>
-      <c r="G182" s="14"/>
+      <c r="G182" s="13"/>
       <c r="H182" s="4"/>
       <c r="I182" s="4"/>
       <c r="J182" s="4"/>
@@ -5743,7 +5934,7 @@
       <c r="D183" s="4"/>
       <c r="E183" s="4"/>
       <c r="F183" s="4"/>
-      <c r="G183" s="14"/>
+      <c r="G183" s="13"/>
       <c r="H183" s="4"/>
       <c r="I183" s="4"/>
       <c r="J183" s="4"/>
@@ -5754,63 +5945,125 @@
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="C1:C27 C46:C1048576">
-    <cfRule type="cellIs" dxfId="15" priority="25" operator="equal">
+  <conditionalFormatting sqref="C1:C27 C53:C1048576 C47:C50">
+    <cfRule type="cellIs" dxfId="23" priority="35" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="36" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="37" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="38" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C36:C45">
-    <cfRule type="cellIs" dxfId="11" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="25" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="26" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="27" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="28" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C28:C34">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="21" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="22" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="23" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="24" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C35">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
       <formula>"Low"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="17" operator="equal">
       <formula>"Medium"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="equal">
       <formula>"High"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="19" operator="equal">
       <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J35">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J28:J34 J36:J45">
+    <cfRule type="colorScale" priority="29">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J120:J177 J3:J27 J47:J50 J53:J103">
+    <cfRule type="colorScale" priority="223">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J104:J119">
+    <cfRule type="colorScale" priority="279">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C46">
+    <cfRule type="cellIs" dxfId="7" priority="6" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="equal">
+      <formula>"Very High"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J46">
     <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
@@ -5822,32 +6075,22 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J28:J34 J36:J45">
-    <cfRule type="colorScale" priority="19">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
+  <conditionalFormatting sqref="C51:C52">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Low"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Medium"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"High"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"Very High"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J120:J177 J3:J27 J46:J103">
-    <cfRule type="colorScale" priority="213">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J104:J119">
-    <cfRule type="colorScale" priority="269">
+  <conditionalFormatting sqref="J51:J52">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>